<commit_message>
log time for JA, JB, DD
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -358,15 +358,15 @@
   </sheetPr>
   <dimension ref="A1:AO50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE9" activeCellId="0" sqref="AE9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="1" width="4.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="17" style="1" width="5.78"/>
@@ -590,7 +590,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" s="8" t="n">
         <f aca="false">SUM(D17:D23)</f>
@@ -630,13 +630,15 @@
       </c>
       <c r="M4" s="9" t="n">
         <f aca="false">SUM(C4:L4)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="8"/>
+      <c r="Q4" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
@@ -651,7 +653,9 @@
         <v>7</v>
       </c>
       <c r="AD4" s="7"/>
-      <c r="AE4" s="11"/>
+      <c r="AE4" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="AF4" s="11"/>
       <c r="AG4" s="11"/>
       <c r="AH4" s="11"/>
@@ -670,7 +674,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="n">
         <f aca="false">SUM(C30:C36)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="8" t="n">
         <f aca="false">SUM(D30:D36)</f>
@@ -710,7 +714,7 @@
       </c>
       <c r="M5" s="9" t="n">
         <f aca="false">SUM(C5:L5)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>10</v>
@@ -731,7 +735,9 @@
         <v>9</v>
       </c>
       <c r="AD5" s="7"/>
-      <c r="AE5" s="11"/>
+      <c r="AE5" s="11" t="n">
+        <v>3</v>
+      </c>
       <c r="AF5" s="11"/>
       <c r="AG5" s="11"/>
       <c r="AH5" s="11"/>
@@ -750,7 +756,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="n">
         <f aca="false">SUM(C43:C49)</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="8" t="n">
         <f aca="false">SUM(D43:D49)</f>
@@ -790,7 +796,7 @@
       </c>
       <c r="M6" s="9" t="n">
         <f aca="false">SUM(C6:L6)</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>12</v>
@@ -832,7 +838,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="n">
         <f aca="false">SUM(Q4:Q10)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="8" t="n">
         <f aca="false">SUM(R4:R10)</f>
@@ -872,7 +878,7 @@
       </c>
       <c r="M7" s="9" t="n">
         <f aca="false">SUM(C7:L7)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>14</v>
@@ -893,7 +899,9 @@
         <v>13</v>
       </c>
       <c r="AD7" s="7"/>
-      <c r="AE7" s="11"/>
+      <c r="AE7" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="AF7" s="11"/>
       <c r="AG7" s="11"/>
       <c r="AH7" s="11"/>
@@ -1158,7 +1166,7 @@
       <c r="B11" s="12"/>
       <c r="C11" s="9" t="n">
         <f aca="false">SUM(C4:C10)</f>
-        <v>10.5</v>
+        <v>21</v>
       </c>
       <c r="D11" s="9" t="n">
         <f aca="false">SUM(D4:D10)</f>
@@ -1203,7 +1211,7 @@
       <c r="P11" s="12"/>
       <c r="Q11" s="9" t="n">
         <f aca="false">SUM(Q4:Q10)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R11" s="9" t="n">
         <f aca="false">SUM(R4:R10)</f>
@@ -1397,7 +1405,9 @@
         <v>8</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="n">
+        <v>3</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1625,7 +1635,7 @@
       <c r="B24" s="12"/>
       <c r="C24" s="9" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D24" s="9" t="n">
         <f aca="false">SUM(D17:D23)</f>
@@ -1851,7 +1861,9 @@
         <v>8</v>
       </c>
       <c r="B30" s="10"/>
-      <c r="C30" s="8"/>
+      <c r="C30" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
@@ -2079,7 +2091,7 @@
       <c r="B37" s="12"/>
       <c r="C37" s="9" t="n">
         <f aca="false">SUM(C30:C36)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D37" s="9" t="n">
         <f aca="false">SUM(D30:D36)</f>
@@ -2306,7 +2318,7 @@
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="8" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -2535,7 +2547,7 @@
       <c r="B50" s="12"/>
       <c r="C50" s="9" t="n">
         <f aca="false">SUM(C43:C49)</f>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D50" s="9" t="n">
         <f aca="false">SUM(D43:D49)</f>

</xml_diff>

<commit_message>
lägg till timmar i tidsrapport
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,448 +5,443 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsrapport" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tidsplan" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="142">
   <si>
-    <t xml:space="preserve">HELA GRUPPEN – TID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DENNIS DERECICHEI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAMN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VECKONUMMER (NÄR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timmar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jakob Arvidsson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Måndag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juan Basaez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tisdag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Johan Can</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onsdag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dennis Derecichei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torsdag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emir Hadzisalihovic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fredag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yousef Hashem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lördag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noah Hellman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Söndag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summa timmar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAKOB ARVIDSSON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMIR HADZISALIHOVIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JUAN BASAEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YOUSEF HASHEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOHAN CAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOAH HELLMAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godkännande av </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projekt:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projektgrupp:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum: 2018-10-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granskad:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beställare: Mattias Krysander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version: 1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YH, JA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kurs: TSEA29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utfärdare: Jakob Arvidsson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OLIKA FASER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIDPLAN (när), veckonummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beskrivning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timmar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initialer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Totalt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designfas (v40 – v45)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utförandefas (v46 – v50)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESIGNFAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systemdesign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hårdvarudesign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mjukvarudesign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dokument</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rapporter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rita blockdiagram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rita kretsscheman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JB, EH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Övrigt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Möten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buffer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UTFÖRANDEFAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allmänt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Koppla och installera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD, EH, Alla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementera mjukvarubaser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NH, Alla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kommunikationsmodul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mjukvara för kommunikationsmodul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NH,EH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bildbearbetning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upptäcka kanter I bilder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NH, DD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upptäcka linjer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avgör felvärde, beräkna det från 2D kartan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autonom körning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position i karta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JB, JC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hitta kortaste säkra väg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reglera styrning utefter felvärde och följ vägfiler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JA,YH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navigera till bestämd stopplinje/parkeringsficka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Styrmodul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Driva bilen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensormodul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bearbeta sensorvärden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EH, JB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skicka ut värden till andra moduler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Användargränssnitt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kör och styr taxin från gränssnittet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JC,YH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inmatning till gränssnitt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visa info på gränssnitt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anslutningar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kommunikation via trådlös länk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD,JB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrationstester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helsystemtestning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YH, DD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teknisk dokumentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efterstudie och presentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JA, JC, DD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Användarmanual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EH, NH, JB, YH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tids- och statusrapporter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summa antal timmar:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MILSTOLPAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEADLINE (när), veckodag &amp; vecka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milstolpe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utvecklingsmiljöer för mikrokontroller och processorer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designspecifikationen är färdigställd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elektroniska komponenter är kopplade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MÅN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seriell kommunikation sker mellan moduler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mätvärden visas på användargränssnittet och reglerparametrar kan skickas till taxin under körning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxin kan fjärrstyras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kameran tar bilder och dessa behandlas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mata in karta och tolka den</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxin håller sig inom vägen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxin kan navigera kartan på ett säkert sätt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxin kan parkera i parkeringsfickor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxin utför sitt uppdrag 3 av 4 gånger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BESLUTSPUNKTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEADLINE (när), datum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godkännande av projektdirektiv, start av förstudier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godkännande av kravspecifikation, start av förberedelsefasen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godkännande av projektplanering, start av utförandefasen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godkännande av designspecifikation, fortsättning av utförandefasen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Används ej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godkännande av produktens funktionalitet, leverans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Godkännande av leverans, upplösning av projektgrupp</t>
+    <t>HELA GRUPPEN – TID</t>
+  </si>
+  <si>
+    <t>DENNIS DERECICHEI</t>
+  </si>
+  <si>
+    <t>NAMN</t>
+  </si>
+  <si>
+    <t>VECKONUMMER (NÄR)</t>
+  </si>
+  <si>
+    <t>Summa</t>
+  </si>
+  <si>
+    <t>timmar</t>
+  </si>
+  <si>
+    <t>Jakob Arvidsson</t>
+  </si>
+  <si>
+    <t>Måndag</t>
+  </si>
+  <si>
+    <t>Juan Basaez</t>
+  </si>
+  <si>
+    <t>Tisdag</t>
+  </si>
+  <si>
+    <t>Johan Can</t>
+  </si>
+  <si>
+    <t>Onsdag</t>
+  </si>
+  <si>
+    <t>Dennis Derecichei</t>
+  </si>
+  <si>
+    <t>Torsdag</t>
+  </si>
+  <si>
+    <t>Emir Hadzisalihovic</t>
+  </si>
+  <si>
+    <t>Fredag</t>
+  </si>
+  <si>
+    <t>Yousef Hashem</t>
+  </si>
+  <si>
+    <t>Lördag</t>
+  </si>
+  <si>
+    <t>Noah Hellman</t>
+  </si>
+  <si>
+    <t>Söndag</t>
+  </si>
+  <si>
+    <t>Summa timmar</t>
+  </si>
+  <si>
+    <t>JAKOB ARVIDSSON</t>
+  </si>
+  <si>
+    <t>EMIR HADZISALIHOVIC</t>
+  </si>
+  <si>
+    <t>JUAN BASAEZ</t>
+  </si>
+  <si>
+    <t>YOUSEF HASHEM</t>
+  </si>
+  <si>
+    <t>JOHAN CAN</t>
+  </si>
+  <si>
+    <t>NOAH HELLMAN</t>
+  </si>
+  <si>
+    <t>Godkännande av </t>
+  </si>
+  <si>
+    <t>Projekt:</t>
+  </si>
+  <si>
+    <t>Projektgrupp:</t>
+  </si>
+  <si>
+    <t>Datum: 2018-10-02</t>
+  </si>
+  <si>
+    <t>Granskad:</t>
+  </si>
+  <si>
+    <t>Beställare: Mattias Krysander</t>
+  </si>
+  <si>
+    <t>Version: 1.0</t>
+  </si>
+  <si>
+    <t>YH, JA</t>
+  </si>
+  <si>
+    <t>Kurs: TSEA29</t>
+  </si>
+  <si>
+    <t>Utfärdare: Jakob Arvidsson</t>
+  </si>
+  <si>
+    <t>OLIKA FASER</t>
+  </si>
+  <si>
+    <t>TID</t>
+  </si>
+  <si>
+    <t>VEM</t>
+  </si>
+  <si>
+    <t>TIDPLAN (när), veckonummer</t>
+  </si>
+  <si>
+    <t>Nr</t>
+  </si>
+  <si>
+    <t>Beskrivning</t>
+  </si>
+  <si>
+    <t>Timmar</t>
+  </si>
+  <si>
+    <t>Initialer</t>
+  </si>
+  <si>
+    <t>Totalt</t>
+  </si>
+  <si>
+    <t>Alla</t>
+  </si>
+  <si>
+    <t>Designfas (v40 – v45)</t>
+  </si>
+  <si>
+    <t>Utförandefas (v46 – v50)</t>
+  </si>
+  <si>
+    <t>DESIGNFAS</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Systemdesign</t>
+  </si>
+  <si>
+    <t>Hårdvarudesign</t>
+  </si>
+  <si>
+    <t>Mjukvarudesign</t>
+  </si>
+  <si>
+    <t>Dokument</t>
+  </si>
+  <si>
+    <t>Rapporter</t>
+  </si>
+  <si>
+    <t>Rita blockdiagram</t>
+  </si>
+  <si>
+    <t>Rita kretsscheman</t>
+  </si>
+  <si>
+    <t>JB, EH</t>
+  </si>
+  <si>
+    <t>Övrigt</t>
+  </si>
+  <si>
+    <t>Möten</t>
+  </si>
+  <si>
+    <t>Buffer</t>
+  </si>
+  <si>
+    <t>UTFÖRANDEFAS</t>
+  </si>
+  <si>
+    <t>Allmänt</t>
+  </si>
+  <si>
+    <t>Koppla och installera</t>
+  </si>
+  <si>
+    <t>DD, EH, Alla</t>
+  </si>
+  <si>
+    <t>Implementera mjukvarubaser</t>
+  </si>
+  <si>
+    <t>NH, Alla</t>
+  </si>
+  <si>
+    <t>Kommunikationsmodul</t>
+  </si>
+  <si>
+    <t>Mjukvara för kommunikationsmodul</t>
+  </si>
+  <si>
+    <t>NH,EH</t>
+  </si>
+  <si>
+    <t>Bildbearbetning</t>
+  </si>
+  <si>
+    <t>Upptäcka kanter I bilder</t>
+  </si>
+  <si>
+    <t>NH, DD</t>
+  </si>
+  <si>
+    <t>Upptäcka linjer</t>
+  </si>
+  <si>
+    <t>Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
+  </si>
+  <si>
+    <t>Avgör felvärde, beräkna det från 2D kartan</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>Autonom körning</t>
+  </si>
+  <si>
+    <t>Position i karta</t>
+  </si>
+  <si>
+    <t>JB, JC</t>
+  </si>
+  <si>
+    <t>Hitta kortaste säkra väg</t>
+  </si>
+  <si>
+    <t>EH</t>
+  </si>
+  <si>
+    <t>Reglera styrning utefter felvärde och följ vägfiler</t>
+  </si>
+  <si>
+    <t>JA,YH</t>
+  </si>
+  <si>
+    <t>Navigera till bestämd stopplinje/parkeringsficka</t>
+  </si>
+  <si>
+    <t>Styrmodul</t>
+  </si>
+  <si>
+    <t>Driva bilen</t>
+  </si>
+  <si>
+    <t>Sensormodul</t>
+  </si>
+  <si>
+    <t>Bearbeta sensorvärden</t>
+  </si>
+  <si>
+    <t>EH, JB</t>
+  </si>
+  <si>
+    <t>Skicka ut värden till andra moduler</t>
+  </si>
+  <si>
+    <t>Användargränssnitt</t>
+  </si>
+  <si>
+    <t>Kör och styr taxin från gränssnittet</t>
+  </si>
+  <si>
+    <t>JC,YH</t>
+  </si>
+  <si>
+    <t>Inmatning till gränssnitt</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>Visa info på gränssnitt</t>
+  </si>
+  <si>
+    <t>Anslutningar</t>
+  </si>
+  <si>
+    <t>Kommunikation via trådlös länk</t>
+  </si>
+  <si>
+    <t>DD,JB</t>
+  </si>
+  <si>
+    <t>Testning</t>
+  </si>
+  <si>
+    <t>Integrationstester</t>
+  </si>
+  <si>
+    <t>YH </t>
+  </si>
+  <si>
+    <t>Helsystemtestning</t>
+  </si>
+  <si>
+    <t>YH, DD</t>
+  </si>
+  <si>
+    <t>Teknisk dokumentation</t>
+  </si>
+  <si>
+    <t>Efterstudie och presentation</t>
+  </si>
+  <si>
+    <t>JA, JC, DD</t>
+  </si>
+  <si>
+    <t>Användarmanual</t>
+  </si>
+  <si>
+    <t>EH, NH, JB, YH</t>
+  </si>
+  <si>
+    <t>Tids- och statusrapporter</t>
+  </si>
+  <si>
+    <t>Summa antal timmar:</t>
+  </si>
+  <si>
+    <t>MILSTOLPAR</t>
+  </si>
+  <si>
+    <t>DEADLINE (när), veckodag &amp; vecka</t>
+  </si>
+  <si>
+    <t>Milstolpe</t>
+  </si>
+  <si>
+    <t>Utvecklingsmiljöer för mikrokontroller och processorer</t>
+  </si>
+  <si>
+    <t>ONS</t>
+  </si>
+  <si>
+    <t>Designspecifikationen är färdigställd</t>
+  </si>
+  <si>
+    <t>TIS</t>
+  </si>
+  <si>
+    <t>Elektroniska komponenter är kopplade</t>
+  </si>
+  <si>
+    <t>MÅN</t>
+  </si>
+  <si>
+    <t>Seriell kommunikation sker mellan moduler</t>
+  </si>
+  <si>
+    <t>Mätvärden visas på användargränssnittet och reglerparametrar kan skickas till taxin under körning</t>
+  </si>
+  <si>
+    <t>Taxin kan fjärrstyras</t>
+  </si>
+  <si>
+    <t>Kameran tar bilder och dessa behandlas</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>Mata in karta och tolka den</t>
+  </si>
+  <si>
+    <t>Taxin håller sig inom vägen</t>
+  </si>
+  <si>
+    <t>Taxin kan navigera kartan på ett säkert sätt</t>
+  </si>
+  <si>
+    <t>FRE</t>
+  </si>
+  <si>
+    <t>Taxin kan parkera i parkeringsfickor</t>
+  </si>
+  <si>
+    <t>Taxin utför sitt uppdrag 3 av 4 gånger</t>
+  </si>
+  <si>
+    <t>BESLUTSPUNKTER</t>
+  </si>
+  <si>
+    <t>DEADLINE (när), datum</t>
+  </si>
+  <si>
+    <t>Godkännande av projektdirektiv, start av förstudier</t>
+  </si>
+  <si>
+    <t>Godkännande av kravspecifikation, start av förberedelsefasen</t>
+  </si>
+  <si>
+    <t>Godkännande av projektplanering, start av utförandefasen</t>
+  </si>
+  <si>
+    <t>Godkännande av designspecifikation, fortsättning av utförandefasen </t>
+  </si>
+  <si>
+    <t>Används ej</t>
+  </si>
+  <si>
+    <t>Godkännande av produktens funktionalitet, leverans</t>
+  </si>
+  <si>
+    <t>Godkännande av leverans, upplösning av projektgrupp</t>
   </si>
 </sst>
 </file>
@@ -454,7 +449,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -926,21 +921,21 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
+        <sz val="10"/>
+        <color rgb="FF9C0006"/>
         <name val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF9C0006"/>
-        <sz val="10"/>
       </font>
       <fill>
         <patternFill>
@@ -950,11 +945,11 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="10"/>
+        <color rgb="FF006100"/>
         <name val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF006100"/>
-        <sz val="10"/>
       </font>
       <fill>
         <patternFill>
@@ -999,12 +994,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFC6EFCE"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFC7CE"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1033,24 +1028,24 @@
   </sheetPr>
   <dimension ref="A1:AO50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q33" activeCellId="0" sqref="Q33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="1" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="17" style="1" width="5.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="7.49"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="31" style="1" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="6.01"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="42" style="1" width="11.5"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.66836734693878"/>
+    <col collapsed="false" hidden="false" max="12" min="3" style="1" width="5.01020408163265"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.5"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="26" min="17" style="1" width="5.83163265306122"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.48979591836735"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="11.5"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="1" width="9"/>
+    <col collapsed="false" hidden="false" max="40" min="31" style="1" width="13.1683673469388"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="6.01020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="42" style="1" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,7 +1234,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D4" s="8" t="n">
         <f aca="false">SUM(D17:D23)</f>
@@ -1279,7 +1274,7 @@
       </c>
       <c r="M4" s="9" t="n">
         <f aca="false">SUM(C4:L4)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>7</v>
@@ -1787,7 +1782,7 @@
       <c r="B11" s="11"/>
       <c r="C11" s="9" t="n">
         <f aca="false">SUM(C4:C10)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D11" s="9" t="n">
         <f aca="false">SUM(D4:D10)</f>
@@ -1885,6 +1880,62 @@
       <c r="AN11" s="0"/>
       <c r="AO11" s="0"/>
     </row>
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
+      <c r="T12" s="0"/>
+      <c r="U12" s="0"/>
+      <c r="V12" s="0"/>
+      <c r="W12" s="0"/>
+      <c r="X12" s="0"/>
+      <c r="Y12" s="0"/>
+      <c r="Z12" s="0"/>
+      <c r="AA12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
+      <c r="V13" s="0"/>
+      <c r="W13" s="0"/>
+      <c r="X13" s="0"/>
+      <c r="Y13" s="0"/>
+      <c r="Z13" s="0"/>
+      <c r="AA13" s="0"/>
+    </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>21</v>
@@ -2062,7 +2113,9 @@
         <v>9</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -2089,12 +2142,14 @@
       <c r="Z18" s="8"/>
       <c r="AA18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="8" t="n">
+        <v>0</v>
+      </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -2256,7 +2311,7 @@
       <c r="B24" s="11"/>
       <c r="C24" s="9" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D24" s="9" t="n">
         <f aca="false">SUM(D17:D23)</f>
@@ -2340,6 +2395,62 @@
         <v>0</v>
       </c>
       <c r="AA24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="I25" s="0"/>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
+      <c r="O25" s="0"/>
+      <c r="P25" s="0"/>
+      <c r="Q25" s="0"/>
+      <c r="R25" s="0"/>
+      <c r="S25" s="0"/>
+      <c r="T25" s="0"/>
+      <c r="U25" s="0"/>
+      <c r="V25" s="0"/>
+      <c r="W25" s="0"/>
+      <c r="X25" s="0"/>
+      <c r="Y25" s="0"/>
+      <c r="Z25" s="0"/>
+      <c r="AA25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="G26" s="0"/>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
+      <c r="M26" s="0"/>
+      <c r="O26" s="0"/>
+      <c r="P26" s="0"/>
+      <c r="Q26" s="0"/>
+      <c r="R26" s="0"/>
+      <c r="S26" s="0"/>
+      <c r="T26" s="0"/>
+      <c r="U26" s="0"/>
+      <c r="V26" s="0"/>
+      <c r="W26" s="0"/>
+      <c r="X26" s="0"/>
+      <c r="Y26" s="0"/>
+      <c r="Z26" s="0"/>
+      <c r="AA26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
@@ -2581,7 +2692,7 @@
       <c r="Z32" s="8"/>
       <c r="AA32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
         <v>13</v>
       </c>
@@ -2800,6 +2911,62 @@
         <v>0</v>
       </c>
       <c r="AA37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
+      <c r="J38" s="0"/>
+      <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
+      <c r="M38" s="0"/>
+      <c r="O38" s="0"/>
+      <c r="P38" s="0"/>
+      <c r="Q38" s="0"/>
+      <c r="R38" s="0"/>
+      <c r="S38" s="0"/>
+      <c r="T38" s="0"/>
+      <c r="U38" s="0"/>
+      <c r="V38" s="0"/>
+      <c r="W38" s="0"/>
+      <c r="X38" s="0"/>
+      <c r="Y38" s="0"/>
+      <c r="Z38" s="0"/>
+      <c r="AA38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
+      <c r="O39" s="0"/>
+      <c r="P39" s="0"/>
+      <c r="Q39" s="0"/>
+      <c r="R39" s="0"/>
+      <c r="S39" s="0"/>
+      <c r="T39" s="0"/>
+      <c r="U39" s="0"/>
+      <c r="V39" s="0"/>
+      <c r="W39" s="0"/>
+      <c r="X39" s="0"/>
+      <c r="Y39" s="0"/>
+      <c r="Z39" s="0"/>
+      <c r="AA39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
@@ -3359,7 +3526,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3374,22 +3541,22 @@
   </sheetPr>
   <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="8" style="0" width="5.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="22" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="11.57"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.14285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.87755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.56632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8571428571429"/>
+    <col collapsed="false" hidden="false" max="21" min="8" style="0" width="5.55102040816327"/>
+    <col collapsed="false" hidden="false" max="1014" min="22" style="0" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6521,17 +6688,9 @@
     <mergeCell ref="B87:G87"/>
     <mergeCell ref="B88:G88"/>
   </mergeCells>
-  <conditionalFormatting sqref="V62:V63 V28:V29 V31 V33:V36 V38:V41 V43 V45:V46 V48:V50 V52 V54:V55 V57:V60">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("FALSE",V28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="1">
-      <formula>NOT(ISERROR(SEARCH("TRUE",V28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
log time for everyone
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,443 +5,451 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsrapport" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tidsplan" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="142">
-  <si>
-    <t>HELA GRUPPEN – TID</t>
-  </si>
-  <si>
-    <t>DENNIS DERECICHEI</t>
-  </si>
-  <si>
-    <t>NAMN</t>
-  </si>
-  <si>
-    <t>VECKONUMMER (NÄR)</t>
-  </si>
-  <si>
-    <t>Summa</t>
-  </si>
-  <si>
-    <t>timmar</t>
-  </si>
-  <si>
-    <t>Jakob Arvidsson</t>
-  </si>
-  <si>
-    <t>Måndag</t>
-  </si>
-  <si>
-    <t>Juan Basaez</t>
-  </si>
-  <si>
-    <t>Tisdag</t>
-  </si>
-  <si>
-    <t>Johan Can</t>
-  </si>
-  <si>
-    <t>Onsdag</t>
-  </si>
-  <si>
-    <t>Dennis Derecichei</t>
-  </si>
-  <si>
-    <t>Torsdag</t>
-  </si>
-  <si>
-    <t>Emir Hadzisalihovic</t>
-  </si>
-  <si>
-    <t>Fredag</t>
-  </si>
-  <si>
-    <t>Yousef Hashem</t>
-  </si>
-  <si>
-    <t>Lördag</t>
-  </si>
-  <si>
-    <t>Noah Hellman</t>
-  </si>
-  <si>
-    <t>Söndag</t>
-  </si>
-  <si>
-    <t>Summa timmar</t>
-  </si>
-  <si>
-    <t>JAKOB ARVIDSSON</t>
-  </si>
-  <si>
-    <t>EMIR HADZISALIHOVIC</t>
-  </si>
-  <si>
-    <t>JUAN BASAEZ</t>
-  </si>
-  <si>
-    <t>YOUSEF HASHEM</t>
-  </si>
-  <si>
-    <t>JOHAN CAN</t>
-  </si>
-  <si>
-    <t>NOAH HELLMAN</t>
-  </si>
-  <si>
-    <t>Godkännande av </t>
-  </si>
-  <si>
-    <t>Projekt:</t>
-  </si>
-  <si>
-    <t>Projektgrupp:</t>
-  </si>
-  <si>
-    <t>Datum: 2018-10-02</t>
-  </si>
-  <si>
-    <t>Granskad:</t>
-  </si>
-  <si>
-    <t>Beställare: Mattias Krysander</t>
-  </si>
-  <si>
-    <t>Version: 1.0</t>
-  </si>
-  <si>
-    <t>YH, JA</t>
-  </si>
-  <si>
-    <t>Kurs: TSEA29</t>
-  </si>
-  <si>
-    <t>Utfärdare: Jakob Arvidsson</t>
-  </si>
-  <si>
-    <t>OLIKA FASER</t>
-  </si>
-  <si>
-    <t>TID</t>
-  </si>
-  <si>
-    <t>VEM</t>
-  </si>
-  <si>
-    <t>TIDPLAN (när), veckonummer</t>
-  </si>
-  <si>
-    <t>Nr</t>
-  </si>
-  <si>
-    <t>Beskrivning</t>
-  </si>
-  <si>
-    <t>Timmar</t>
-  </si>
-  <si>
-    <t>Initialer</t>
-  </si>
-  <si>
-    <t>Totalt</t>
-  </si>
-  <si>
-    <t>Alla</t>
-  </si>
-  <si>
-    <t>Designfas (v40 – v45)</t>
-  </si>
-  <si>
-    <t>Utförandefas (v46 – v50)</t>
-  </si>
-  <si>
-    <t>DESIGNFAS</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Systemdesign</t>
-  </si>
-  <si>
-    <t>Hårdvarudesign</t>
-  </si>
-  <si>
-    <t>Mjukvarudesign</t>
-  </si>
-  <si>
-    <t>Dokument</t>
-  </si>
-  <si>
-    <t>Rapporter</t>
-  </si>
-  <si>
-    <t>Rita blockdiagram</t>
-  </si>
-  <si>
-    <t>Rita kretsscheman</t>
-  </si>
-  <si>
-    <t>JB, EH</t>
-  </si>
-  <si>
-    <t>Övrigt</t>
-  </si>
-  <si>
-    <t>Möten</t>
-  </si>
-  <si>
-    <t>Buffer</t>
-  </si>
-  <si>
-    <t>UTFÖRANDEFAS</t>
-  </si>
-  <si>
-    <t>Allmänt</t>
-  </si>
-  <si>
-    <t>Koppla och installera</t>
-  </si>
-  <si>
-    <t>DD, EH, Alla</t>
-  </si>
-  <si>
-    <t>Implementera mjukvarubaser</t>
-  </si>
-  <si>
-    <t>NH, Alla</t>
-  </si>
-  <si>
-    <t>Kommunikationsmodul</t>
-  </si>
-  <si>
-    <t>Mjukvara för kommunikationsmodul</t>
-  </si>
-  <si>
-    <t>NH,EH</t>
-  </si>
-  <si>
-    <t>Bildbearbetning</t>
-  </si>
-  <si>
-    <t>Upptäcka kanter I bilder</t>
-  </si>
-  <si>
-    <t>NH, DD</t>
-  </si>
-  <si>
-    <t>Upptäcka linjer</t>
-  </si>
-  <si>
-    <t>Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
-  </si>
-  <si>
-    <t>Avgör felvärde, beräkna det från 2D kartan</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>Autonom körning</t>
-  </si>
-  <si>
-    <t>Position i karta</t>
-  </si>
-  <si>
-    <t>JB, JC</t>
-  </si>
-  <si>
-    <t>Hitta kortaste säkra väg</t>
-  </si>
-  <si>
-    <t>EH</t>
-  </si>
-  <si>
-    <t>Reglera styrning utefter felvärde och följ vägfiler</t>
-  </si>
-  <si>
-    <t>JA,YH</t>
-  </si>
-  <si>
-    <t>Navigera till bestämd stopplinje/parkeringsficka</t>
-  </si>
-  <si>
-    <t>Styrmodul</t>
-  </si>
-  <si>
-    <t>Driva bilen</t>
-  </si>
-  <si>
-    <t>Sensormodul</t>
-  </si>
-  <si>
-    <t>Bearbeta sensorvärden</t>
-  </si>
-  <si>
-    <t>EH, JB</t>
-  </si>
-  <si>
-    <t>Skicka ut värden till andra moduler</t>
-  </si>
-  <si>
-    <t>Användargränssnitt</t>
-  </si>
-  <si>
-    <t>Kör och styr taxin från gränssnittet</t>
-  </si>
-  <si>
-    <t>JC,YH</t>
-  </si>
-  <si>
-    <t>Inmatning till gränssnitt</t>
-  </si>
-  <si>
-    <t>JC</t>
-  </si>
-  <si>
-    <t>Visa info på gränssnitt</t>
-  </si>
-  <si>
-    <t>Anslutningar</t>
-  </si>
-  <si>
-    <t>Kommunikation via trådlös länk</t>
-  </si>
-  <si>
-    <t>DD,JB</t>
-  </si>
-  <si>
-    <t>Testning</t>
-  </si>
-  <si>
-    <t>Integrationstester</t>
-  </si>
-  <si>
-    <t>YH </t>
-  </si>
-  <si>
-    <t>Helsystemtestning</t>
-  </si>
-  <si>
-    <t>YH, DD</t>
-  </si>
-  <si>
-    <t>Teknisk dokumentation</t>
-  </si>
-  <si>
-    <t>Efterstudie och presentation</t>
-  </si>
-  <si>
-    <t>JA, JC, DD</t>
-  </si>
-  <si>
-    <t>Användarmanual</t>
-  </si>
-  <si>
-    <t>EH, NH, JB, YH</t>
-  </si>
-  <si>
-    <t>Tids- och statusrapporter</t>
-  </si>
-  <si>
-    <t>Summa antal timmar:</t>
-  </si>
-  <si>
-    <t>MILSTOLPAR</t>
-  </si>
-  <si>
-    <t>DEADLINE (när), veckodag &amp; vecka</t>
-  </si>
-  <si>
-    <t>Milstolpe</t>
-  </si>
-  <si>
-    <t>Utvecklingsmiljöer för mikrokontroller och processorer</t>
-  </si>
-  <si>
-    <t>ONS</t>
-  </si>
-  <si>
-    <t>Designspecifikationen är färdigställd</t>
-  </si>
-  <si>
-    <t>TIS</t>
-  </si>
-  <si>
-    <t>Elektroniska komponenter är kopplade</t>
-  </si>
-  <si>
-    <t>MÅN</t>
-  </si>
-  <si>
-    <t>Seriell kommunikation sker mellan moduler</t>
-  </si>
-  <si>
-    <t>Mätvärden visas på användargränssnittet och reglerparametrar kan skickas till taxin under körning</t>
-  </si>
-  <si>
-    <t>Taxin kan fjärrstyras</t>
-  </si>
-  <si>
-    <t>Kameran tar bilder och dessa behandlas</t>
-  </si>
-  <si>
-    <t>TOR</t>
-  </si>
-  <si>
-    <t>Mata in karta och tolka den</t>
-  </si>
-  <si>
-    <t>Taxin håller sig inom vägen</t>
-  </si>
-  <si>
-    <t>Taxin kan navigera kartan på ett säkert sätt</t>
-  </si>
-  <si>
-    <t>FRE</t>
-  </si>
-  <si>
-    <t>Taxin kan parkera i parkeringsfickor</t>
-  </si>
-  <si>
-    <t>Taxin utför sitt uppdrag 3 av 4 gånger</t>
-  </si>
-  <si>
-    <t>BESLUTSPUNKTER</t>
-  </si>
-  <si>
-    <t>DEADLINE (när), datum</t>
-  </si>
-  <si>
-    <t>Godkännande av projektdirektiv, start av förstudier</t>
-  </si>
-  <si>
-    <t>Godkännande av kravspecifikation, start av förberedelsefasen</t>
-  </si>
-  <si>
-    <t>Godkännande av projektplanering, start av utförandefasen</t>
-  </si>
-  <si>
-    <t>Godkännande av designspecifikation, fortsättning av utförandefasen </t>
-  </si>
-  <si>
-    <t>Används ej</t>
-  </si>
-  <si>
-    <t>Godkännande av produktens funktionalitet, leverans</t>
-  </si>
-  <si>
-    <t>Godkännande av leverans, upplösning av projektgrupp</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
+  <si>
+    <t xml:space="preserve">HELA GRUPPEN – TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENNIS DERECICHEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAMN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VECKONUMMER (NÄR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakob Arvidsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Måndag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan Basaez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tisdag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johan Can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onsdag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dennis Derecichei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torsdag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emir Hadzisalihovic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fredag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yousef Hashem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lördag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noah Hellman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Söndag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summa timmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JAKOB ARVIDSSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMIR HADZISALIHOVIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUAN BASAEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOUSEF HASHEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHAN CAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOAH HELLMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projekt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projektgrupp:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum: 2018-10-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granskad:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beställare: Mattias Krysander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YH, JA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurs: TSEA29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utfärdare: Jakob Arvidsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLIKA FASER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIDPLAN (när), veckonummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beskrivning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designfas (v40 – v45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utförandefas (v46 – v50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESIGNFAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systemdesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hårdvarudesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mjukvarudesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dokument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rita blockdiagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rita kretsscheman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JB, EH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Övrigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Möten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTFÖRANDEFAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allmänt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koppla och installera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD, EH, Alla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementera mjukvarubaser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH, Alla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommunikationsmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mjukvara för kommunikationsmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH,EH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bildbearbetning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upptäcka kanter I bilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH, DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upptäcka linjer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avgör felvärde, beräkna det från 2D kartan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autonom körning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position i karta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JB, JC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hitta kortaste säkra väg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reglera styrning utefter felvärde och följ vägfiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA,YH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigera till bestämd stopplinje/parkeringsficka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Styrmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driva bilen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensormodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bearbeta sensorvärden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH, JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skicka ut värden till andra moduler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Användargränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kör och styr taxin från gränssnittet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC,YH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inmatning till gränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visa info på gränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anslutningar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommunikation via trådlös länk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD,JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrationstester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helsystemtestning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YH, DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teknisk dokumentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efterstudie och presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA, JC, DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Användarmanual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH, NH, JB, YH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tids- och statusrapporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summa antal timmar:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILSTOLPAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE (när), veckodag &amp; vecka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milstolpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utvecklingsmiljöer för mikrokontroller och processorer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designspecifikationen är färdigställd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elektroniska komponenter är kopplade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MÅN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seriell kommunikation sker mellan moduler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mätvärden visas på användargränssnittet och reglerparametrar kan skickas till taxin under körning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin kan fjärrstyras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kameran tar bilder och dessa behandlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mata in karta och tolka den</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin håller sig inom vägen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin kan navigera kartan på ett säkert sätt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin kan parkera i parkeringsfickor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin utför sitt uppdrag 3 av 4 gånger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BESLUTSPUNKTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE (när), datum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av projektdirektiv, start av förstudier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av kravspecifikation, start av förberedelsefasen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av projektplanering, start av utförandefasen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av designspecifikation, fortsättning av utförandefasen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Används ej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av produktens funktionalitet, leverans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av leverans, upplösning av projektgrupp</t>
   </si>
 </sst>
 </file>
@@ -449,7 +457,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -921,21 +929,21 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
         <sz val="10"/>
-        <color rgb="FF9C0006"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -945,11 +953,11 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF006100"/>
         <sz val="10"/>
-        <color rgb="FF006100"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -994,12 +1002,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFC6EFCE"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFC7CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1028,24 +1036,24 @@
   </sheetPr>
   <dimension ref="A1:AO50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.66836734693878"/>
-    <col collapsed="false" hidden="false" max="12" min="3" style="1" width="5.01020408163265"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.5"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="8.8265306122449"/>
-    <col collapsed="false" hidden="false" max="26" min="17" style="1" width="5.83163265306122"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.48979591836735"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="11.5"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="1" width="9"/>
-    <col collapsed="false" hidden="false" max="40" min="31" style="1" width="13.1683673469388"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="6.01020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="42" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="1" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="17" style="1" width="5.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="7.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="31" style="1" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="6.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="42" style="1" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,7 +1242,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" s="8" t="n">
         <f aca="false">SUM(D17:D23)</f>
@@ -1274,7 +1282,7 @@
       </c>
       <c r="M4" s="9" t="n">
         <f aca="false">SUM(C4:L4)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>7</v>
@@ -1314,7 +1322,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="n">
         <f aca="false">SUM(C30:C36)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D5" s="8" t="n">
         <f aca="false">SUM(D30:D36)</f>
@@ -1354,13 +1362,15 @@
       </c>
       <c r="M5" s="9" t="n">
         <f aca="false">SUM(C5:L5)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="P5" s="10"/>
-      <c r="Q5" s="8"/>
+      <c r="Q5" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
@@ -1392,7 +1402,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="n">
         <f aca="false">SUM(C43:C49)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" s="8" t="n">
         <f aca="false">SUM(D43:D49)</f>
@@ -1432,7 +1442,7 @@
       </c>
       <c r="M6" s="9" t="n">
         <f aca="false">SUM(C6:L6)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>11</v>
@@ -1470,7 +1480,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="n">
         <f aca="false">SUM(Q4:Q10)</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D7" s="8" t="n">
         <f aca="false">SUM(R4:R10)</f>
@@ -1510,13 +1520,15 @@
       </c>
       <c r="M7" s="9" t="n">
         <f aca="false">SUM(C7:L7)</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="P7" s="10"/>
-      <c r="Q7" s="8"/>
+      <c r="Q7" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
@@ -1548,7 +1560,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="n">
         <f aca="false">SUM(Q17:Q23)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D8" s="8" t="n">
         <f aca="false">SUM(R17:R23)</f>
@@ -1588,7 +1600,7 @@
       </c>
       <c r="M8" s="9" t="n">
         <f aca="false">SUM(C8:L8)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="O8" s="10" t="s">
         <v>15</v>
@@ -1626,7 +1638,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="n">
         <f aca="false">SUM(Q30:Q36)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8" t="n">
         <f aca="false">SUM(R30:R36)</f>
@@ -1666,7 +1678,7 @@
       </c>
       <c r="M9" s="9" t="n">
         <f aca="false">SUM(C9:L9)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="O9" s="10" t="s">
         <v>17</v>
@@ -1704,7 +1716,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="n">
         <f aca="false">SUM(Q43:Q49)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D10" s="8" t="n">
         <f aca="false">SUM(R43:R49)</f>
@@ -1744,7 +1756,7 @@
       </c>
       <c r="M10" s="9" t="n">
         <f aca="false">SUM(C10:L10)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="O10" s="10" t="s">
         <v>19</v>
@@ -1782,7 +1794,7 @@
       <c r="B11" s="11"/>
       <c r="C11" s="9" t="n">
         <f aca="false">SUM(C4:C10)</f>
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="D11" s="9" t="n">
         <f aca="false">SUM(D4:D10)</f>
@@ -1827,7 +1839,7 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="9" t="n">
         <f aca="false">SUM(Q4:Q10)</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="R11" s="9" t="n">
         <f aca="false">SUM(R4:R10)</f>
@@ -1880,62 +1892,6 @@
       <c r="AN11" s="0"/>
       <c r="AO11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-      <c r="G12" s="0"/>
-      <c r="H12" s="0"/>
-      <c r="I12" s="0"/>
-      <c r="J12" s="0"/>
-      <c r="K12" s="0"/>
-      <c r="L12" s="0"/>
-      <c r="M12" s="0"/>
-      <c r="O12" s="0"/>
-      <c r="P12" s="0"/>
-      <c r="Q12" s="0"/>
-      <c r="R12" s="0"/>
-      <c r="S12" s="0"/>
-      <c r="T12" s="0"/>
-      <c r="U12" s="0"/>
-      <c r="V12" s="0"/>
-      <c r="W12" s="0"/>
-      <c r="X12" s="0"/>
-      <c r="Y12" s="0"/>
-      <c r="Z12" s="0"/>
-      <c r="AA12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="0"/>
-      <c r="H13" s="0"/>
-      <c r="I13" s="0"/>
-      <c r="J13" s="0"/>
-      <c r="K13" s="0"/>
-      <c r="L13" s="0"/>
-      <c r="M13" s="0"/>
-      <c r="O13" s="0"/>
-      <c r="P13" s="0"/>
-      <c r="Q13" s="0"/>
-      <c r="R13" s="0"/>
-      <c r="S13" s="0"/>
-      <c r="T13" s="0"/>
-      <c r="U13" s="0"/>
-      <c r="V13" s="0"/>
-      <c r="W13" s="0"/>
-      <c r="X13" s="0"/>
-      <c r="Y13" s="0"/>
-      <c r="Z13" s="0"/>
-      <c r="AA13" s="0"/>
-    </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>21</v>
@@ -1968,7 +1924,7 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -2004,7 +1960,7 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="n">
@@ -2147,9 +2103,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="8" t="n">
-        <v>0</v>
-      </c>
+      <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -2164,7 +2118,9 @@
         <v>11</v>
       </c>
       <c r="P19" s="10"/>
-      <c r="Q19" s="8"/>
+      <c r="Q19" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
@@ -2176,12 +2132,14 @@
       <c r="Z19" s="8"/>
       <c r="AA19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="8"/>
+      <c r="C20" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -2196,7 +2154,9 @@
         <v>13</v>
       </c>
       <c r="P20" s="10"/>
-      <c r="Q20" s="8"/>
+      <c r="Q20" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
@@ -2311,7 +2271,7 @@
       <c r="B24" s="11"/>
       <c r="C24" s="9" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D24" s="9" t="n">
         <f aca="false">SUM(D17:D23)</f>
@@ -2356,7 +2316,7 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="9" t="n">
         <f aca="false">SUM(Q17:Q23)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="R24" s="9" t="n">
         <f aca="false">SUM(R17:R23)</f>
@@ -2395,62 +2355,6 @@
         <v>0</v>
       </c>
       <c r="AA24" s="6"/>
-    </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
-      <c r="E25" s="0"/>
-      <c r="F25" s="0"/>
-      <c r="G25" s="0"/>
-      <c r="H25" s="0"/>
-      <c r="I25" s="0"/>
-      <c r="J25" s="0"/>
-      <c r="K25" s="0"/>
-      <c r="L25" s="0"/>
-      <c r="M25" s="0"/>
-      <c r="O25" s="0"/>
-      <c r="P25" s="0"/>
-      <c r="Q25" s="0"/>
-      <c r="R25" s="0"/>
-      <c r="S25" s="0"/>
-      <c r="T25" s="0"/>
-      <c r="U25" s="0"/>
-      <c r="V25" s="0"/>
-      <c r="W25" s="0"/>
-      <c r="X25" s="0"/>
-      <c r="Y25" s="0"/>
-      <c r="Z25" s="0"/>
-      <c r="AA25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="0"/>
-      <c r="F26" s="0"/>
-      <c r="G26" s="0"/>
-      <c r="H26" s="0"/>
-      <c r="I26" s="0"/>
-      <c r="J26" s="0"/>
-      <c r="K26" s="0"/>
-      <c r="L26" s="0"/>
-      <c r="M26" s="0"/>
-      <c r="O26" s="0"/>
-      <c r="P26" s="0"/>
-      <c r="Q26" s="0"/>
-      <c r="R26" s="0"/>
-      <c r="S26" s="0"/>
-      <c r="T26" s="0"/>
-      <c r="U26" s="0"/>
-      <c r="V26" s="0"/>
-      <c r="W26" s="0"/>
-      <c r="X26" s="0"/>
-      <c r="Y26" s="0"/>
-      <c r="Z26" s="0"/>
-      <c r="AA26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
@@ -2629,7 +2533,9 @@
         <v>9</v>
       </c>
       <c r="B31" s="10"/>
-      <c r="C31" s="8"/>
+      <c r="C31" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
@@ -2692,12 +2598,14 @@
       <c r="Z32" s="8"/>
       <c r="AA32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B33" s="10"/>
-      <c r="C33" s="8"/>
+      <c r="C33" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -2712,7 +2620,9 @@
         <v>13</v>
       </c>
       <c r="P33" s="10"/>
-      <c r="Q33" s="8"/>
+      <c r="Q33" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
       <c r="T33" s="8"/>
@@ -2827,7 +2737,7 @@
       <c r="B37" s="11"/>
       <c r="C37" s="9" t="n">
         <f aca="false">SUM(C30:C36)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D37" s="9" t="n">
         <f aca="false">SUM(D30:D36)</f>
@@ -2872,7 +2782,7 @@
       <c r="P37" s="11"/>
       <c r="Q37" s="9" t="n">
         <f aca="false">SUM(Q30:Q36)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="R37" s="9" t="n">
         <f aca="false">SUM(R30:R36)</f>
@@ -2911,62 +2821,6 @@
         <v>0</v>
       </c>
       <c r="AA37" s="6"/>
-    </row>
-    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="0"/>
-      <c r="E38" s="0"/>
-      <c r="F38" s="0"/>
-      <c r="G38" s="0"/>
-      <c r="H38" s="0"/>
-      <c r="I38" s="0"/>
-      <c r="J38" s="0"/>
-      <c r="K38" s="0"/>
-      <c r="L38" s="0"/>
-      <c r="M38" s="0"/>
-      <c r="O38" s="0"/>
-      <c r="P38" s="0"/>
-      <c r="Q38" s="0"/>
-      <c r="R38" s="0"/>
-      <c r="S38" s="0"/>
-      <c r="T38" s="0"/>
-      <c r="U38" s="0"/>
-      <c r="V38" s="0"/>
-      <c r="W38" s="0"/>
-      <c r="X38" s="0"/>
-      <c r="Y38" s="0"/>
-      <c r="Z38" s="0"/>
-      <c r="AA38" s="0"/>
-    </row>
-    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
-      <c r="D39" s="0"/>
-      <c r="E39" s="0"/>
-      <c r="F39" s="0"/>
-      <c r="G39" s="0"/>
-      <c r="H39" s="0"/>
-      <c r="I39" s="0"/>
-      <c r="J39" s="0"/>
-      <c r="K39" s="0"/>
-      <c r="L39" s="0"/>
-      <c r="M39" s="0"/>
-      <c r="O39" s="0"/>
-      <c r="P39" s="0"/>
-      <c r="Q39" s="0"/>
-      <c r="R39" s="0"/>
-      <c r="S39" s="0"/>
-      <c r="T39" s="0"/>
-      <c r="U39" s="0"/>
-      <c r="V39" s="0"/>
-      <c r="W39" s="0"/>
-      <c r="X39" s="0"/>
-      <c r="Y39" s="0"/>
-      <c r="Z39" s="0"/>
-      <c r="AA39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
@@ -3162,7 +3016,9 @@
         <v>9</v>
       </c>
       <c r="P44" s="10"/>
-      <c r="Q44" s="8"/>
+      <c r="Q44" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
       <c r="T44" s="8"/>
@@ -3211,7 +3067,9 @@
         <v>13</v>
       </c>
       <c r="B46" s="10"/>
-      <c r="C46" s="8"/>
+      <c r="C46" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
@@ -3226,7 +3084,9 @@
         <v>13</v>
       </c>
       <c r="P46" s="10"/>
-      <c r="Q46" s="8"/>
+      <c r="Q46" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
       <c r="T46" s="8"/>
@@ -3341,7 +3201,7 @@
       <c r="B50" s="11"/>
       <c r="C50" s="9" t="n">
         <f aca="false">SUM(C43:C49)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D50" s="9" t="n">
         <f aca="false">SUM(D43:D49)</f>
@@ -3386,7 +3246,7 @@
       <c r="P50" s="11"/>
       <c r="Q50" s="9" t="n">
         <f aca="false">SUM(Q43:Q49)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="R50" s="9" t="n">
         <f aca="false">SUM(R43:R49)</f>
@@ -3526,7 +3386,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3539,24 +3399,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U88"/>
+  <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.14285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.87755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.56632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="8" style="0" width="5.55102040816327"/>
-    <col collapsed="false" hidden="false" max="1014" min="22" style="0" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="11.5714285714286"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="8" style="0" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="22" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,10 +3528,13 @@
       <c r="S4" s="24"/>
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
+      <c r="V4" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
@@ -3679,7 +3542,7 @@
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
       <c r="G5" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -3698,20 +3561,20 @@
     </row>
     <row r="6" s="29" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -3729,19 +3592,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
       <c r="F7" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H7" s="32" t="n">
         <v>40</v>
@@ -3787,7 +3650,7 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32"/>
       <c r="B8" s="34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
@@ -3796,7 +3659,7 @@
         <v>1120</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" s="35" t="n">
         <v>40</v>
@@ -3837,7 +3700,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32"/>
       <c r="B9" s="34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -3846,7 +3709,7 @@
         <v>220</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H9" s="35" t="n">
         <v>40</v>
@@ -3875,7 +3738,7 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32"/>
       <c r="B10" s="34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
@@ -3884,7 +3747,7 @@
         <v>900</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
@@ -3918,20 +3781,20 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
@@ -3949,19 +3812,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
       <c r="F12" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H12" s="32" t="n">
         <v>40</v>
@@ -4007,7 +3870,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="32"/>
       <c r="B13" s="30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -4034,7 +3897,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="34"/>
@@ -4043,7 +3906,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H14" s="35" t="n">
         <v>10</v>
@@ -4072,7 +3935,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
@@ -4081,7 +3944,7 @@
         <v>40</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H15" s="35" t="n">
         <v>20</v>
@@ -4110,7 +3973,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
@@ -4119,7 +3982,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H16" s="35"/>
       <c r="I16" s="35" t="n">
@@ -4146,7 +4009,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="32"/>
       <c r="B17" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -4173,7 +4036,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
@@ -4182,7 +4045,7 @@
         <v>40</v>
       </c>
       <c r="G18" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H18" s="35"/>
       <c r="I18" s="35" t="n">
@@ -4211,7 +4074,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
@@ -4249,7 +4112,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="34"/>
       <c r="D20" s="34"/>
@@ -4258,7 +4121,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H20" s="35"/>
       <c r="I20" s="35" t="n">
@@ -4285,7 +4148,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="32"/>
       <c r="B21" s="30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -4312,7 +4175,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -4321,7 +4184,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H22" s="35" t="n">
         <v>7</v>
@@ -4350,7 +4213,7 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="32"/>
       <c r="B23" s="34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
@@ -4390,7 +4253,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="32"/>
       <c r="B24" s="34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
@@ -4429,20 +4292,20 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
       <c r="E25" s="28"/>
       <c r="F25" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I25" s="28"/>
       <c r="J25" s="28"/>
@@ -4460,19 +4323,19 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
       <c r="F26" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H26" s="32" t="n">
         <v>40</v>
@@ -4518,7 +4381,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="32"/>
       <c r="B27" s="30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -4545,7 +4408,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C28" s="34"/>
       <c r="D28" s="34"/>
@@ -4554,7 +4417,7 @@
         <v>55</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H28" s="38"/>
       <c r="I28" s="38"/>
@@ -4583,7 +4446,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" s="34"/>
       <c r="D29" s="34"/>
@@ -4592,7 +4455,7 @@
         <v>60</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H29" s="38"/>
       <c r="I29" s="38"/>
@@ -4619,7 +4482,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="32"/>
       <c r="B30" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="30"/>
@@ -4646,7 +4509,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
@@ -4655,7 +4518,7 @@
         <v>40</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H31" s="38"/>
       <c r="I31" s="38"/>
@@ -4682,7 +4545,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="32"/>
       <c r="B32" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
@@ -4709,7 +4572,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" s="42"/>
       <c r="D33" s="42"/>
@@ -4718,7 +4581,7 @@
         <v>25</v>
       </c>
       <c r="G33" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H33" s="38"/>
       <c r="I33" s="38"/>
@@ -4745,7 +4608,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34" s="42"/>
       <c r="D34" s="42"/>
@@ -4754,7 +4617,7 @@
         <v>25</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H34" s="38"/>
       <c r="I34" s="38"/>
@@ -4783,7 +4646,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" s="42"/>
       <c r="D35" s="42"/>
@@ -4792,7 +4655,7 @@
         <v>20</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H35" s="38"/>
       <c r="I35" s="38"/>
@@ -4819,7 +4682,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="42"/>
@@ -4828,7 +4691,7 @@
         <v>20</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H36" s="38"/>
       <c r="I36" s="38"/>
@@ -4853,7 +4716,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="32"/>
       <c r="B37" s="30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="30"/>
@@ -4880,7 +4743,7 @@
         <v>15</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C38" s="42"/>
       <c r="D38" s="42"/>
@@ -4889,7 +4752,7 @@
         <v>30</v>
       </c>
       <c r="G38" s="35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H38" s="38"/>
       <c r="I38" s="38"/>
@@ -4916,7 +4779,7 @@
         <v>16</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="42"/>
@@ -4925,7 +4788,7 @@
         <v>20</v>
       </c>
       <c r="G39" s="35" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H39" s="38"/>
       <c r="I39" s="38"/>
@@ -4952,7 +4815,7 @@
         <v>17</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C40" s="42"/>
       <c r="D40" s="42"/>
@@ -4961,7 +4824,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H40" s="38"/>
       <c r="I40" s="38"/>
@@ -4990,7 +4853,7 @@
         <v>18</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="42"/>
@@ -4999,7 +4862,7 @@
         <v>40</v>
       </c>
       <c r="G41" s="35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H41" s="38"/>
       <c r="I41" s="38"/>
@@ -5026,7 +4889,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="32"/>
       <c r="B42" s="30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C42" s="30"/>
       <c r="D42" s="30"/>
@@ -5053,7 +4916,7 @@
         <v>19</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C43" s="42"/>
       <c r="D43" s="42"/>
@@ -5062,7 +4925,7 @@
         <v>40</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H43" s="38"/>
       <c r="I43" s="38"/>
@@ -5087,7 +4950,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="32"/>
       <c r="B44" s="30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44" s="30"/>
       <c r="D44" s="30"/>
@@ -5114,7 +4977,7 @@
         <v>20</v>
       </c>
       <c r="B45" s="42" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C45" s="42"/>
       <c r="D45" s="42"/>
@@ -5123,7 +4986,7 @@
         <v>40</v>
       </c>
       <c r="G45" s="35" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H45" s="38"/>
       <c r="I45" s="38"/>
@@ -5152,7 +5015,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C46" s="42"/>
       <c r="D46" s="42"/>
@@ -5161,7 +5024,7 @@
         <v>20</v>
       </c>
       <c r="G46" s="35" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H46" s="38"/>
       <c r="I46" s="38"/>
@@ -5188,7 +5051,7 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="32"/>
       <c r="B47" s="30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C47" s="30"/>
       <c r="D47" s="30"/>
@@ -5215,7 +5078,7 @@
         <v>22</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C48" s="42"/>
       <c r="D48" s="42"/>
@@ -5224,7 +5087,7 @@
         <v>15</v>
       </c>
       <c r="G48" s="35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H48" s="38"/>
       <c r="I48" s="38"/>
@@ -5251,7 +5114,7 @@
         <v>23</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="42"/>
@@ -5260,7 +5123,7 @@
         <v>30</v>
       </c>
       <c r="G49" s="35" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H49" s="38"/>
       <c r="I49" s="38"/>
@@ -5289,7 +5152,7 @@
         <v>24</v>
       </c>
       <c r="B50" s="42" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C50" s="42"/>
       <c r="D50" s="42"/>
@@ -5298,7 +5161,7 @@
         <v>30</v>
       </c>
       <c r="G50" s="35" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H50" s="38"/>
       <c r="I50" s="38"/>
@@ -5325,7 +5188,7 @@
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="32"/>
       <c r="B51" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
@@ -5352,7 +5215,7 @@
         <v>25</v>
       </c>
       <c r="B52" s="42" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C52" s="42"/>
       <c r="D52" s="42"/>
@@ -5361,7 +5224,7 @@
         <v>20</v>
       </c>
       <c r="G52" s="35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H52" s="38"/>
       <c r="I52" s="38"/>
@@ -5386,7 +5249,7 @@
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="32"/>
       <c r="B53" s="30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C53" s="30"/>
       <c r="D53" s="30"/>
@@ -5413,7 +5276,7 @@
         <v>26</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
@@ -5422,7 +5285,7 @@
         <v>10</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H54" s="38"/>
       <c r="I54" s="38"/>
@@ -5449,7 +5312,7 @@
         <v>27</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C55" s="42"/>
       <c r="D55" s="42"/>
@@ -5458,7 +5321,7 @@
         <v>30</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H55" s="38"/>
       <c r="I55" s="38"/>
@@ -5483,7 +5346,7 @@
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="32"/>
       <c r="B56" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C56" s="30"/>
       <c r="D56" s="30"/>
@@ -5510,7 +5373,7 @@
         <v>28</v>
       </c>
       <c r="B57" s="42" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C57" s="42"/>
       <c r="D57" s="42"/>
@@ -5519,7 +5382,7 @@
         <v>70</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H57" s="38"/>
       <c r="I57" s="38"/>
@@ -5546,7 +5409,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="42" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
@@ -5555,7 +5418,7 @@
         <v>20</v>
       </c>
       <c r="G58" s="34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H58" s="38"/>
       <c r="I58" s="38"/>
@@ -5582,7 +5445,7 @@
         <v>30</v>
       </c>
       <c r="B59" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C59" s="42"/>
       <c r="D59" s="42"/>
@@ -5591,7 +5454,7 @@
         <v>20</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H59" s="38"/>
       <c r="I59" s="38"/>
@@ -5620,7 +5483,7 @@
         <v>33</v>
       </c>
       <c r="B60" s="42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C60" s="42"/>
       <c r="D60" s="42"/>
@@ -5629,7 +5492,7 @@
         <v>20</v>
       </c>
       <c r="G60" s="43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H60" s="38"/>
       <c r="I60" s="38"/>
@@ -5662,7 +5525,7 @@
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="32"/>
       <c r="B61" s="30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C61" s="30"/>
       <c r="D61" s="30"/>
@@ -5689,7 +5552,7 @@
         <v>32</v>
       </c>
       <c r="B62" s="42" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C62" s="42"/>
       <c r="D62" s="42"/>
@@ -5698,7 +5561,7 @@
         <v>35</v>
       </c>
       <c r="G62" s="43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H62" s="38"/>
       <c r="I62" s="38"/>
@@ -5731,7 +5594,7 @@
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="32"/>
       <c r="B63" s="44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C63" s="44"/>
       <c r="D63" s="44"/>
@@ -5780,7 +5643,7 @@
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="32"/>
       <c r="B64" s="42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C64" s="42"/>
       <c r="D64" s="42"/>
@@ -5829,7 +5692,7 @@
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="32"/>
       <c r="B65" s="45" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C65" s="45"/>
       <c r="D65" s="45"/>
@@ -5877,7 +5740,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B66" s="28"/>
       <c r="C66" s="28"/>
@@ -5886,7 +5749,7 @@
       <c r="F66" s="28"/>
       <c r="G66" s="28"/>
       <c r="H66" s="28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I66" s="28"/>
       <c r="J66" s="28"/>
@@ -5904,10 +5767,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B67" s="47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C67" s="47"/>
       <c r="D67" s="47"/>
@@ -5960,7 +5823,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C68" s="48"/>
       <c r="D68" s="48"/>
@@ -5972,7 +5835,7 @@
       <c r="J68" s="49"/>
       <c r="K68" s="49"/>
       <c r="L68" s="49" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M68" s="49"/>
       <c r="N68" s="8"/>
@@ -5989,7 +5852,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="48" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C69" s="48"/>
       <c r="D69" s="48"/>
@@ -6002,7 +5865,7 @@
       <c r="K69" s="49"/>
       <c r="L69" s="49"/>
       <c r="M69" s="49" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N69" s="8"/>
       <c r="O69" s="8"/>
@@ -6018,7 +5881,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C70" s="48"/>
       <c r="D70" s="48"/>
@@ -6033,7 +5896,7 @@
       <c r="M70" s="49"/>
       <c r="N70" s="8"/>
       <c r="O70" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P70" s="8"/>
       <c r="Q70" s="8"/>
@@ -6047,7 +5910,7 @@
         <v>4</v>
       </c>
       <c r="B71" s="48" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C71" s="48"/>
       <c r="D71" s="48"/>
@@ -6063,7 +5926,7 @@
       <c r="N71" s="8"/>
       <c r="O71" s="8"/>
       <c r="P71" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
@@ -6076,7 +5939,7 @@
         <v>5</v>
       </c>
       <c r="B72" s="48" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C72" s="48"/>
       <c r="D72" s="48"/>
@@ -6092,7 +5955,7 @@
       <c r="N72" s="50"/>
       <c r="O72" s="50"/>
       <c r="P72" s="50" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Q72" s="50"/>
       <c r="R72" s="50"/>
@@ -6105,7 +5968,7 @@
         <v>6</v>
       </c>
       <c r="B73" s="48" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C73" s="48"/>
       <c r="D73" s="48"/>
@@ -6121,7 +5984,7 @@
       <c r="N73" s="8"/>
       <c r="O73" s="8"/>
       <c r="P73" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
@@ -6134,7 +5997,7 @@
         <v>7</v>
       </c>
       <c r="B74" s="48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C74" s="48"/>
       <c r="D74" s="48"/>
@@ -6150,7 +6013,7 @@
       <c r="N74" s="50"/>
       <c r="O74" s="50"/>
       <c r="P74" s="50" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q74" s="50"/>
       <c r="R74" s="50"/>
@@ -6163,7 +6026,7 @@
         <v>8</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C75" s="48"/>
       <c r="D75" s="48"/>
@@ -6180,7 +6043,7 @@
       <c r="O75" s="50"/>
       <c r="P75" s="50"/>
       <c r="Q75" s="50" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="R75" s="50"/>
       <c r="S75" s="49"/>
@@ -6192,7 +6055,7 @@
         <v>9</v>
       </c>
       <c r="B76" s="48" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C76" s="48"/>
       <c r="D76" s="48"/>
@@ -6209,7 +6072,7 @@
       <c r="O76" s="50"/>
       <c r="P76" s="50"/>
       <c r="Q76" s="50" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="R76" s="50"/>
       <c r="S76" s="49"/>
@@ -6221,7 +6084,7 @@
         <v>10</v>
       </c>
       <c r="B77" s="48" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C77" s="48"/>
       <c r="D77" s="48"/>
@@ -6238,7 +6101,7 @@
       <c r="O77" s="50"/>
       <c r="P77" s="50"/>
       <c r="Q77" s="50" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="R77" s="50"/>
       <c r="S77" s="49"/>
@@ -6250,7 +6113,7 @@
         <v>11</v>
       </c>
       <c r="B78" s="48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C78" s="48"/>
       <c r="D78" s="48"/>
@@ -6268,7 +6131,7 @@
       <c r="P78" s="8"/>
       <c r="Q78" s="8"/>
       <c r="R78" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="S78" s="49"/>
       <c r="T78" s="49"/>
@@ -6279,7 +6142,7 @@
         <v>12</v>
       </c>
       <c r="B79" s="48" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C79" s="48"/>
       <c r="D79" s="48"/>
@@ -6297,7 +6160,7 @@
       <c r="P79" s="8"/>
       <c r="Q79" s="8"/>
       <c r="R79" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="S79" s="49"/>
       <c r="T79" s="49"/>
@@ -6305,20 +6168,20 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B80" s="28"/>
       <c r="C80" s="28"/>
       <c r="D80" s="28"/>
       <c r="E80" s="28"/>
       <c r="F80" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G80" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H80" s="28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I80" s="28"/>
       <c r="J80" s="28"/>
@@ -6336,10 +6199,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B81" s="47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C81" s="47"/>
       <c r="D81" s="47"/>
@@ -6392,7 +6255,7 @@
         <v>0</v>
       </c>
       <c r="B82" s="48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C82" s="48"/>
       <c r="D82" s="48"/>
@@ -6419,7 +6282,7 @@
         <v>1</v>
       </c>
       <c r="B83" s="48" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C83" s="48"/>
       <c r="D83" s="48"/>
@@ -6446,7 +6309,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="48" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C84" s="48"/>
       <c r="D84" s="48"/>
@@ -6455,7 +6318,7 @@
       <c r="G84" s="48"/>
       <c r="H84" s="49"/>
       <c r="I84" s="49" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J84" s="49"/>
       <c r="K84" s="49"/>
@@ -6475,7 +6338,7 @@
         <v>3</v>
       </c>
       <c r="B85" s="48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C85" s="48"/>
       <c r="D85" s="48"/>
@@ -6488,7 +6351,7 @@
       <c r="K85" s="49"/>
       <c r="L85" s="49"/>
       <c r="M85" s="49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="N85" s="8"/>
       <c r="O85" s="8"/>
@@ -6504,7 +6367,7 @@
         <v>4</v>
       </c>
       <c r="B86" s="54" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C86" s="54"/>
       <c r="D86" s="54"/>
@@ -6531,7 +6394,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="48" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C87" s="48"/>
       <c r="D87" s="48"/>
@@ -6549,7 +6412,7 @@
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
       <c r="R87" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="S87" s="49"/>
       <c r="T87" s="49"/>
@@ -6560,7 +6423,7 @@
         <v>6</v>
       </c>
       <c r="B88" s="48" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C88" s="48"/>
       <c r="D88" s="48"/>
@@ -6579,7 +6442,7 @@
       <c r="Q88" s="49"/>
       <c r="R88" s="49"/>
       <c r="S88" s="49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="T88" s="49"/>
       <c r="U88" s="52"/>
@@ -6688,9 +6551,17 @@
     <mergeCell ref="B87:G87"/>
     <mergeCell ref="B88:G88"/>
   </mergeCells>
+  <conditionalFormatting sqref="V62:V63 V28:V29 V31 V33:V36 V38:V41 V43 V45:V46 V48:V50 V52 V54:V55 V57:V60">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("FALSE",V28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="1">
+      <formula>NOT(ISERROR(SEARCH("TRUE",V28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
fix new time plan
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsrapport" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="147">
   <si>
     <t xml:space="preserve">HELA GRUPPEN – TID</t>
   </si>
@@ -227,7 +227,7 @@
     <t xml:space="preserve">Implementera mjukvarubaser</t>
   </si>
   <si>
-    <t xml:space="preserve">NH, Alla</t>
+    <t xml:space="preserve">NH, EH, DD, JC</t>
   </si>
   <si>
     <t xml:space="preserve">Kommunikationsmodul</t>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">Mjukvara för kommunikationsmodul</t>
   </si>
   <si>
-    <t xml:space="preserve">NH,EH</t>
+    <t xml:space="preserve">NH, JC</t>
   </si>
   <si>
     <t xml:space="preserve">Bildbearbetning</t>
@@ -245,19 +245,22 @@
     <t xml:space="preserve">Upptäcka kanter I bilder</t>
   </si>
   <si>
+    <t xml:space="preserve">Upptäcka linjer</t>
+  </si>
+  <si>
     <t xml:space="preserve">NH, DD</t>
   </si>
   <si>
-    <t xml:space="preserve">Upptäcka linjer</t>
-  </si>
-  <si>
     <t xml:space="preserve">Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
   </si>
   <si>
+    <t xml:space="preserve">JC, DD, JB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Avgör felvärde, beräkna det från 2D kartan</t>
   </si>
   <si>
-    <t xml:space="preserve">NH</t>
+    <t xml:space="preserve">NH, JB</t>
   </si>
   <si>
     <t xml:space="preserve">Autonom körning</t>
@@ -266,7 +269,7 @@
     <t xml:space="preserve">Position i karta</t>
   </si>
   <si>
-    <t xml:space="preserve">JB, JC</t>
+    <t xml:space="preserve">JB, JC, DD</t>
   </si>
   <si>
     <t xml:space="preserve">Hitta kortaste säkra väg</t>
@@ -284,6 +287,9 @@
     <t xml:space="preserve">Navigera till bestämd stopplinje/parkeringsficka</t>
   </si>
   <si>
+    <t xml:space="preserve">NH, JA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Styrmodul</t>
   </si>
   <si>
@@ -314,19 +320,22 @@
     <t xml:space="preserve">Inmatning till gränssnitt</t>
   </si>
   <si>
-    <t xml:space="preserve">JC</t>
+    <t xml:space="preserve">JC, EH, JB</t>
   </si>
   <si>
     <t xml:space="preserve">Visa info på gränssnitt</t>
   </si>
   <si>
+    <t xml:space="preserve">JC, DD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anslutningar</t>
   </si>
   <si>
     <t xml:space="preserve">Kommunikation via trådlös länk</t>
   </si>
   <si>
-    <t xml:space="preserve">DD,JB</t>
+    <t xml:space="preserve">DD,YH</t>
   </si>
   <si>
     <t xml:space="preserve">Testning</t>
@@ -335,16 +344,19 @@
     <t xml:space="preserve">Integrationstester</t>
   </si>
   <si>
-    <t xml:space="preserve">YH </t>
+    <t xml:space="preserve">EH </t>
   </si>
   <si>
     <t xml:space="preserve">Helsystemtestning</t>
   </si>
   <si>
-    <t xml:space="preserve">YH, DD</t>
+    <t xml:space="preserve">YH, JC</t>
   </si>
   <si>
     <t xml:space="preserve">Teknisk dokumentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH, DD, JB, JA</t>
   </si>
   <si>
     <t xml:space="preserve">Efterstudie och presentation</t>
@@ -1036,7 +1048,7 @@
   </sheetPr>
   <dimension ref="A1:AO50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3401,8 +3413,8 @@
   </sheetPr>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4581,7 +4593,7 @@
         <v>25</v>
       </c>
       <c r="G33" s="35" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="H33" s="38"/>
       <c r="I33" s="38"/>
@@ -4608,7 +4620,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="42"/>
       <c r="D34" s="42"/>
@@ -4617,7 +4629,7 @@
         <v>25</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H34" s="38"/>
       <c r="I34" s="38"/>
@@ -4655,7 +4667,7 @@
         <v>20</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H35" s="38"/>
       <c r="I35" s="38"/>
@@ -4682,7 +4694,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="42"/>
@@ -4691,7 +4703,7 @@
         <v>20</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H36" s="38"/>
       <c r="I36" s="38"/>
@@ -4716,7 +4728,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="32"/>
       <c r="B37" s="30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="30"/>
@@ -4743,7 +4755,7 @@
         <v>15</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C38" s="42"/>
       <c r="D38" s="42"/>
@@ -4752,7 +4764,7 @@
         <v>30</v>
       </c>
       <c r="G38" s="35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H38" s="38"/>
       <c r="I38" s="38"/>
@@ -4779,7 +4791,7 @@
         <v>16</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="42"/>
@@ -4788,7 +4800,7 @@
         <v>20</v>
       </c>
       <c r="G39" s="35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H39" s="38"/>
       <c r="I39" s="38"/>
@@ -4815,7 +4827,7 @@
         <v>17</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C40" s="42"/>
       <c r="D40" s="42"/>
@@ -4824,7 +4836,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H40" s="38"/>
       <c r="I40" s="38"/>
@@ -4853,7 +4865,7 @@
         <v>18</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="42"/>
@@ -4862,7 +4874,7 @@
         <v>40</v>
       </c>
       <c r="G41" s="35" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H41" s="38"/>
       <c r="I41" s="38"/>
@@ -4889,7 +4901,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="32"/>
       <c r="B42" s="30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C42" s="30"/>
       <c r="D42" s="30"/>
@@ -4916,7 +4928,7 @@
         <v>19</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C43" s="42"/>
       <c r="D43" s="42"/>
@@ -4925,7 +4937,7 @@
         <v>40</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H43" s="38"/>
       <c r="I43" s="38"/>
@@ -4950,7 +4962,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="32"/>
       <c r="B44" s="30" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C44" s="30"/>
       <c r="D44" s="30"/>
@@ -4977,7 +4989,7 @@
         <v>20</v>
       </c>
       <c r="B45" s="42" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45" s="42"/>
       <c r="D45" s="42"/>
@@ -4986,7 +4998,7 @@
         <v>40</v>
       </c>
       <c r="G45" s="35" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H45" s="38"/>
       <c r="I45" s="38"/>
@@ -5015,7 +5027,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C46" s="42"/>
       <c r="D46" s="42"/>
@@ -5024,7 +5036,7 @@
         <v>20</v>
       </c>
       <c r="G46" s="35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H46" s="38"/>
       <c r="I46" s="38"/>
@@ -5051,7 +5063,7 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="32"/>
       <c r="B47" s="30" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C47" s="30"/>
       <c r="D47" s="30"/>
@@ -5078,7 +5090,7 @@
         <v>22</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C48" s="42"/>
       <c r="D48" s="42"/>
@@ -5087,7 +5099,7 @@
         <v>15</v>
       </c>
       <c r="G48" s="35" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H48" s="38"/>
       <c r="I48" s="38"/>
@@ -5114,7 +5126,7 @@
         <v>23</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="42"/>
@@ -5123,7 +5135,7 @@
         <v>30</v>
       </c>
       <c r="G49" s="35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H49" s="38"/>
       <c r="I49" s="38"/>
@@ -5152,7 +5164,7 @@
         <v>24</v>
       </c>
       <c r="B50" s="42" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C50" s="42"/>
       <c r="D50" s="42"/>
@@ -5161,7 +5173,7 @@
         <v>30</v>
       </c>
       <c r="G50" s="35" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="H50" s="38"/>
       <c r="I50" s="38"/>
@@ -5188,7 +5200,7 @@
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="32"/>
       <c r="B51" s="30" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="30"/>
@@ -5215,7 +5227,7 @@
         <v>25</v>
       </c>
       <c r="B52" s="42" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C52" s="42"/>
       <c r="D52" s="42"/>
@@ -5224,7 +5236,7 @@
         <v>20</v>
       </c>
       <c r="G52" s="35" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H52" s="38"/>
       <c r="I52" s="38"/>
@@ -5249,7 +5261,7 @@
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="32"/>
       <c r="B53" s="30" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C53" s="30"/>
       <c r="D53" s="30"/>
@@ -5276,7 +5288,7 @@
         <v>26</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
@@ -5285,7 +5297,7 @@
         <v>10</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H54" s="38"/>
       <c r="I54" s="38"/>
@@ -5312,7 +5324,7 @@
         <v>27</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C55" s="42"/>
       <c r="D55" s="42"/>
@@ -5321,7 +5333,7 @@
         <v>30</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H55" s="38"/>
       <c r="I55" s="38"/>
@@ -5373,7 +5385,7 @@
         <v>28</v>
       </c>
       <c r="B57" s="42" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C57" s="42"/>
       <c r="D57" s="42"/>
@@ -5382,7 +5394,7 @@
         <v>70</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="H57" s="38"/>
       <c r="I57" s="38"/>
@@ -5409,7 +5421,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="42" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
@@ -5418,7 +5430,7 @@
         <v>20</v>
       </c>
       <c r="G58" s="34" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H58" s="38"/>
       <c r="I58" s="38"/>
@@ -5445,7 +5457,7 @@
         <v>30</v>
       </c>
       <c r="B59" s="42" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C59" s="42"/>
       <c r="D59" s="42"/>
@@ -5454,7 +5466,7 @@
         <v>20</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H59" s="38"/>
       <c r="I59" s="38"/>
@@ -5483,7 +5495,7 @@
         <v>33</v>
       </c>
       <c r="B60" s="42" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C60" s="42"/>
       <c r="D60" s="42"/>
@@ -5692,7 +5704,7 @@
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="32"/>
       <c r="B65" s="45" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C65" s="45"/>
       <c r="D65" s="45"/>
@@ -5740,7 +5752,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B66" s="28"/>
       <c r="C66" s="28"/>
@@ -5749,7 +5761,7 @@
       <c r="F66" s="28"/>
       <c r="G66" s="28"/>
       <c r="H66" s="28" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I66" s="28"/>
       <c r="J66" s="28"/>
@@ -5770,7 +5782,7 @@
         <v>42</v>
       </c>
       <c r="B67" s="47" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C67" s="47"/>
       <c r="D67" s="47"/>
@@ -5823,7 +5835,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C68" s="48"/>
       <c r="D68" s="48"/>
@@ -5835,7 +5847,7 @@
       <c r="J68" s="49"/>
       <c r="K68" s="49"/>
       <c r="L68" s="49" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="M68" s="49"/>
       <c r="N68" s="8"/>
@@ -5852,7 +5864,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="48" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C69" s="48"/>
       <c r="D69" s="48"/>
@@ -5865,7 +5877,7 @@
       <c r="K69" s="49"/>
       <c r="L69" s="49"/>
       <c r="M69" s="49" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="N69" s="8"/>
       <c r="O69" s="8"/>
@@ -5881,7 +5893,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="48" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C70" s="48"/>
       <c r="D70" s="48"/>
@@ -5896,7 +5908,7 @@
       <c r="M70" s="49"/>
       <c r="N70" s="8"/>
       <c r="O70" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="P70" s="8"/>
       <c r="Q70" s="8"/>
@@ -5910,7 +5922,7 @@
         <v>4</v>
       </c>
       <c r="B71" s="48" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C71" s="48"/>
       <c r="D71" s="48"/>
@@ -5926,7 +5938,7 @@
       <c r="N71" s="8"/>
       <c r="O71" s="8"/>
       <c r="P71" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
@@ -5939,7 +5951,7 @@
         <v>5</v>
       </c>
       <c r="B72" s="48" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C72" s="48"/>
       <c r="D72" s="48"/>
@@ -5955,7 +5967,7 @@
       <c r="N72" s="50"/>
       <c r="O72" s="50"/>
       <c r="P72" s="50" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="Q72" s="50"/>
       <c r="R72" s="50"/>
@@ -5968,7 +5980,7 @@
         <v>6</v>
       </c>
       <c r="B73" s="48" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C73" s="48"/>
       <c r="D73" s="48"/>
@@ -5984,7 +5996,7 @@
       <c r="N73" s="8"/>
       <c r="O73" s="8"/>
       <c r="P73" s="8" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
@@ -5997,7 +6009,7 @@
         <v>7</v>
       </c>
       <c r="B74" s="48" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C74" s="48"/>
       <c r="D74" s="48"/>
@@ -6013,7 +6025,7 @@
       <c r="N74" s="50"/>
       <c r="O74" s="50"/>
       <c r="P74" s="50" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="Q74" s="50"/>
       <c r="R74" s="50"/>
@@ -6026,7 +6038,7 @@
         <v>8</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C75" s="48"/>
       <c r="D75" s="48"/>
@@ -6043,7 +6055,7 @@
       <c r="O75" s="50"/>
       <c r="P75" s="50"/>
       <c r="Q75" s="50" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="R75" s="50"/>
       <c r="S75" s="49"/>
@@ -6055,7 +6067,7 @@
         <v>9</v>
       </c>
       <c r="B76" s="48" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C76" s="48"/>
       <c r="D76" s="48"/>
@@ -6072,7 +6084,7 @@
       <c r="O76" s="50"/>
       <c r="P76" s="50"/>
       <c r="Q76" s="50" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="R76" s="50"/>
       <c r="S76" s="49"/>
@@ -6084,7 +6096,7 @@
         <v>10</v>
       </c>
       <c r="B77" s="48" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C77" s="48"/>
       <c r="D77" s="48"/>
@@ -6101,7 +6113,7 @@
       <c r="O77" s="50"/>
       <c r="P77" s="50"/>
       <c r="Q77" s="50" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="R77" s="50"/>
       <c r="S77" s="49"/>
@@ -6113,7 +6125,7 @@
         <v>11</v>
       </c>
       <c r="B78" s="48" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C78" s="48"/>
       <c r="D78" s="48"/>
@@ -6131,7 +6143,7 @@
       <c r="P78" s="8"/>
       <c r="Q78" s="8"/>
       <c r="R78" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="S78" s="49"/>
       <c r="T78" s="49"/>
@@ -6142,7 +6154,7 @@
         <v>12</v>
       </c>
       <c r="B79" s="48" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C79" s="48"/>
       <c r="D79" s="48"/>
@@ -6160,7 +6172,7 @@
       <c r="P79" s="8"/>
       <c r="Q79" s="8"/>
       <c r="R79" s="8" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="S79" s="49"/>
       <c r="T79" s="49"/>
@@ -6168,7 +6180,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B80" s="28"/>
       <c r="C80" s="28"/>
@@ -6181,7 +6193,7 @@
         <v>40</v>
       </c>
       <c r="H80" s="28" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="I80" s="28"/>
       <c r="J80" s="28"/>
@@ -6202,7 +6214,7 @@
         <v>42</v>
       </c>
       <c r="B81" s="47" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C81" s="47"/>
       <c r="D81" s="47"/>
@@ -6255,7 +6267,7 @@
         <v>0</v>
       </c>
       <c r="B82" s="48" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C82" s="48"/>
       <c r="D82" s="48"/>
@@ -6282,7 +6294,7 @@
         <v>1</v>
       </c>
       <c r="B83" s="48" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C83" s="48"/>
       <c r="D83" s="48"/>
@@ -6309,7 +6321,7 @@
         <v>2</v>
       </c>
       <c r="B84" s="48" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C84" s="48"/>
       <c r="D84" s="48"/>
@@ -6318,7 +6330,7 @@
       <c r="G84" s="48"/>
       <c r="H84" s="49"/>
       <c r="I84" s="49" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="J84" s="49"/>
       <c r="K84" s="49"/>
@@ -6338,7 +6350,7 @@
         <v>3</v>
       </c>
       <c r="B85" s="48" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C85" s="48"/>
       <c r="D85" s="48"/>
@@ -6351,7 +6363,7 @@
       <c r="K85" s="49"/>
       <c r="L85" s="49"/>
       <c r="M85" s="49" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="N85" s="8"/>
       <c r="O85" s="8"/>
@@ -6367,7 +6379,7 @@
         <v>4</v>
       </c>
       <c r="B86" s="54" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C86" s="54"/>
       <c r="D86" s="54"/>
@@ -6394,7 +6406,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="48" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C87" s="48"/>
       <c r="D87" s="48"/>
@@ -6412,7 +6424,7 @@
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
       <c r="R87" s="8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="S87" s="49"/>
       <c r="T87" s="49"/>
@@ -6423,7 +6435,7 @@
         <v>6</v>
       </c>
       <c r="B88" s="48" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C88" s="48"/>
       <c r="D88" s="48"/>
@@ -6442,7 +6454,7 @@
       <c r="Q88" s="49"/>
       <c r="R88" s="49"/>
       <c r="S88" s="49" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="T88" s="49"/>
       <c r="U88" s="52"/>

</xml_diff>

<commit_message>
log time for NH, JA, DD, EH, YH
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsrapport" sheetId="1" state="visible" r:id="rId2"/>
@@ -1048,8 +1048,8 @@
   </sheetPr>
   <dimension ref="A1:AO50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q48" activeCellId="0" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1254,7 +1254,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4" s="8" t="n">
         <f aca="false">SUM(D17:D23)</f>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="M4" s="9" t="n">
         <f aca="false">SUM(C4:L4)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>7</v>
@@ -1492,7 +1492,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="n">
         <f aca="false">SUM(Q4:Q10)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D7" s="8" t="n">
         <f aca="false">SUM(R4:R10)</f>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="M7" s="9" t="n">
         <f aca="false">SUM(C7:L7)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>13</v>
@@ -1572,7 +1572,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="n">
         <f aca="false">SUM(Q17:Q23)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D8" s="8" t="n">
         <f aca="false">SUM(R17:R23)</f>
@@ -1612,13 +1612,15 @@
       </c>
       <c r="M8" s="9" t="n">
         <f aca="false">SUM(C8:L8)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="O8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="P8" s="10"/>
-      <c r="Q8" s="8"/>
+      <c r="Q8" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
@@ -1650,7 +1652,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="n">
         <f aca="false">SUM(Q30:Q36)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D9" s="8" t="n">
         <f aca="false">SUM(R30:R36)</f>
@@ -1690,7 +1692,7 @@
       </c>
       <c r="M9" s="9" t="n">
         <f aca="false">SUM(C9:L9)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="O9" s="10" t="s">
         <v>17</v>
@@ -1728,7 +1730,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="n">
         <f aca="false">SUM(Q43:Q49)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D10" s="8" t="n">
         <f aca="false">SUM(R43:R49)</f>
@@ -1768,7 +1770,7 @@
       </c>
       <c r="M10" s="9" t="n">
         <f aca="false">SUM(C10:L10)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="O10" s="10" t="s">
         <v>19</v>
@@ -1806,7 +1808,7 @@
       <c r="B11" s="11"/>
       <c r="C11" s="9" t="n">
         <f aca="false">SUM(C4:C10)</f>
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D11" s="9" t="n">
         <f aca="false">SUM(D4:D10)</f>
@@ -1851,7 +1853,7 @@
       <c r="P11" s="11"/>
       <c r="Q11" s="9" t="n">
         <f aca="false">SUM(Q4:Q10)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="R11" s="9" t="n">
         <f aca="false">SUM(R4:R10)</f>
@@ -2185,7 +2187,9 @@
         <v>15</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="8"/>
+      <c r="C21" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -2200,7 +2204,9 @@
         <v>15</v>
       </c>
       <c r="P21" s="10"/>
-      <c r="Q21" s="8"/>
+      <c r="Q21" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
@@ -2283,7 +2289,7 @@
       <c r="B24" s="11"/>
       <c r="C24" s="9" t="n">
         <f aca="false">SUM(C17:C23)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D24" s="9" t="n">
         <f aca="false">SUM(D17:D23)</f>
@@ -2328,7 +2334,7 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="9" t="n">
         <f aca="false">SUM(Q17:Q23)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="R24" s="9" t="n">
         <f aca="false">SUM(R17:R23)</f>
@@ -2666,7 +2672,9 @@
         <v>15</v>
       </c>
       <c r="P34" s="10"/>
-      <c r="Q34" s="8"/>
+      <c r="Q34" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
@@ -2794,7 +2802,7 @@
       <c r="P37" s="11"/>
       <c r="Q37" s="9" t="n">
         <f aca="false">SUM(Q30:Q36)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="R37" s="9" t="n">
         <f aca="false">SUM(R30:R36)</f>
@@ -3130,7 +3138,9 @@
         <v>15</v>
       </c>
       <c r="P47" s="10"/>
-      <c r="Q47" s="8"/>
+      <c r="Q47" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="R47" s="8"/>
       <c r="S47" s="8"/>
       <c r="T47" s="8"/>
@@ -3258,7 +3268,7 @@
       <c r="P50" s="11"/>
       <c r="Q50" s="9" t="n">
         <f aca="false">SUM(Q43:Q49)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="R50" s="9" t="n">
         <f aca="false">SUM(R43:R49)</f>
@@ -3413,7 +3423,7 @@
   </sheetPr>
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G49" activeCellId="0" sqref="G49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update timeplan for the week
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsrapport" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="145">
   <si>
     <t xml:space="preserve">HELA GRUPPEN – TID</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t xml:space="preserve">Utfärdare: Jakob Arvidsson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s</t>
   </si>
   <si>
     <t xml:space="preserve">OLIKA FASER</t>
@@ -715,7 +712,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -864,6 +861,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -934,12 +935,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1011,8 +1012,8 @@
   </sheetPr>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U9" activeCellId="0" sqref="U9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB26" activeCellId="0" sqref="AB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3322,10 +3323,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V88"/>
+  <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V9" activeCellId="0" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3478,26 +3479,23 @@
       <c r="S5" s="23"/>
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
-      <c r="V5" s="0" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="6" s="28" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
       <c r="F6" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="H6" s="27" t="s">
         <v>40</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>41</v>
       </c>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
@@ -3515,19 +3513,19 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>43</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>45</v>
       </c>
       <c r="H7" s="31" t="n">
         <v>40</v>
@@ -3570,10 +3568,10 @@
       </c>
       <c r="U7" s="32"/>
     </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31"/>
       <c r="B8" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
@@ -3582,7 +3580,7 @@
         <v>1120</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="34" t="n">
         <v>0</v>
@@ -3597,21 +3595,20 @@
       <c r="L8" s="36" t="n">
         <v>43</v>
       </c>
-      <c r="M8" s="34" t="n">
-        <f aca="false">SUM(M13:M23,M27:M63)</f>
-        <v>34</v>
+      <c r="M8" s="37" t="n">
+        <v>77</v>
       </c>
       <c r="N8" s="34" t="n">
         <f aca="false">SUM(N13:N23,N27:N63)</f>
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="O8" s="34" t="n">
         <f aca="false">SUM(O13:O23,O27:O63)</f>
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="P8" s="34" t="n">
         <f aca="false">SUM(P13:P23,P27:P63)</f>
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="Q8" s="34" t="n">
         <f aca="false">SUM(Q13:Q23,Q27:Q63)</f>
@@ -3625,7 +3622,7 @@
         <f aca="false">SUM(S13:S23,S27:S63)</f>
         <v>22</v>
       </c>
-      <c r="T8" s="37"/>
+      <c r="T8" s="38"/>
       <c r="U8" s="32" t="n">
         <f aca="false">SUM(H8:S8)</f>
         <v>1120</v>
@@ -3634,7 +3631,7 @@
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31"/>
       <c r="B9" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
@@ -3643,7 +3640,7 @@
         <v>220</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" s="34" t="n">
         <v>40</v>
@@ -3652,8 +3649,8 @@
         <v>110</v>
       </c>
       <c r="J9" s="34"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
       <c r="M9" s="34" t="n">
         <v>70</v>
       </c>
@@ -3663,7 +3660,7 @@
       <c r="Q9" s="34"/>
       <c r="R9" s="34"/>
       <c r="S9" s="34"/>
-      <c r="T9" s="37"/>
+      <c r="T9" s="38"/>
       <c r="U9" s="32" t="n">
         <f aca="false">SUM(H9:S9)</f>
         <v>220</v>
@@ -3672,7 +3669,7 @@
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31"/>
       <c r="B10" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
@@ -3681,22 +3678,22 @@
         <v>900</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" s="34"/>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
       <c r="M10" s="34"/>
       <c r="N10" s="34" t="n">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="O10" s="34" t="n">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="P10" s="34" t="n">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="Q10" s="34" t="n">
         <v>180</v>
@@ -3707,28 +3704,28 @@
       <c r="S10" s="34" t="n">
         <v>22</v>
       </c>
-      <c r="T10" s="37"/>
+      <c r="T10" s="38"/>
       <c r="U10" s="32" t="n">
         <f aca="false">SUM(H10:S10)</f>
-        <v>900</v>
+        <v>857</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="H11" s="27" t="s">
         <v>40</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>41</v>
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
@@ -3746,19 +3743,19 @@
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="30" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>43</v>
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
       <c r="F12" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>45</v>
       </c>
       <c r="H12" s="31" t="n">
         <v>40</v>
@@ -3804,12 +3801,12 @@
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="31"/>
       <c r="B13" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
-      <c r="F13" s="40"/>
+      <c r="F13" s="41"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
@@ -3818,12 +3815,12 @@
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="38"/>
       <c r="U13" s="29"/>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3831,7 +3828,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
@@ -3840,7 +3837,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H14" s="34" t="n">
         <v>10</v>
@@ -3849,16 +3846,16 @@
         <v>10</v>
       </c>
       <c r="J14" s="34"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
       <c r="U14" s="32" t="n">
         <f aca="false">SUM(H14:T14)</f>
         <v>20</v>
@@ -3869,7 +3866,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
@@ -3878,7 +3875,7 @@
         <v>40</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" s="34" t="n">
         <v>20</v>
@@ -3887,16 +3884,16 @@
         <v>20</v>
       </c>
       <c r="J15" s="34"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="40"/>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="38"/>
       <c r="U15" s="32" t="n">
         <f aca="false">SUM(H15:T15)</f>
         <v>40</v>
@@ -3907,7 +3904,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -3916,23 +3913,23 @@
         <v>40</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H16" s="34"/>
       <c r="I16" s="34" t="n">
         <v>20</v>
       </c>
       <c r="J16" s="34"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="37"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="38"/>
       <c r="U16" s="32" t="n">
         <f aca="false">SUM(H16:T16)</f>
         <v>20</v>
@@ -3941,12 +3938,12 @@
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="31"/>
       <c r="B17" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
-      <c r="F17" s="40"/>
+      <c r="F17" s="41"/>
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
@@ -3955,12 +3952,12 @@
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="37"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
       <c r="U17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3968,7 +3965,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
@@ -3977,25 +3974,25 @@
         <v>40</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="34" t="n">
         <v>20</v>
       </c>
       <c r="J18" s="34"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="40"/>
       <c r="M18" s="34" t="n">
         <v>24</v>
       </c>
       <c r="N18" s="34"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
       <c r="U18" s="32" t="n">
         <f aca="false">SUM(H18:T18)</f>
         <v>44</v>
@@ -4006,7 +4003,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
@@ -4022,16 +4019,16 @@
         <v>10</v>
       </c>
       <c r="J19" s="34"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="40"/>
       <c r="M19" s="34"/>
       <c r="N19" s="34"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37"/>
-      <c r="T19" s="37"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
       <c r="U19" s="32" t="n">
         <f aca="false">SUM(H19:T19)</f>
         <v>10</v>
@@ -4042,7 +4039,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
@@ -4051,23 +4048,23 @@
         <v>20</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="34" t="n">
         <v>10</v>
       </c>
       <c r="J20" s="34"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="40"/>
       <c r="M20" s="34"/>
       <c r="N20" s="34"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
       <c r="U20" s="32" t="n">
         <f aca="false">SUM(H20:T20)</f>
         <v>10</v>
@@ -4076,34 +4073,34 @@
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="31"/>
       <c r="B21" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="40"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="41"/>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="31" t="n">
         <v>7</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
@@ -4112,7 +4109,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H22" s="34" t="n">
         <v>7</v>
@@ -4121,18 +4118,18 @@
         <v>7</v>
       </c>
       <c r="J22" s="34"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="40"/>
       <c r="M22" s="34" t="n">
         <v>7</v>
       </c>
       <c r="N22" s="34"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="37"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="38"/>
+      <c r="T22" s="38"/>
       <c r="U22" s="32" t="n">
         <f aca="false">SUM(H22:T22)</f>
         <v>21</v>
@@ -4141,7 +4138,7 @@
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31"/>
       <c r="B23" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
@@ -4167,12 +4164,12 @@
         <v>3</v>
       </c>
       <c r="N23" s="34"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="37"/>
-      <c r="T23" s="37"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="38"/>
       <c r="U23" s="32" t="n">
         <f aca="false">SUM(H23:T23)</f>
         <v>19</v>
@@ -4181,7 +4178,7 @@
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="31"/>
       <c r="B24" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
@@ -4207,33 +4204,33 @@
         <v>34</v>
       </c>
       <c r="N24" s="34"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="37"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
       <c r="U24" s="32" t="n">
         <f aca="false">SUM(H8:M8)</f>
-        <v>220</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="H25" s="27" t="s">
         <v>40</v>
-      </c>
-      <c r="H25" s="27" t="s">
-        <v>41</v>
       </c>
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
@@ -4251,19 +4248,19 @@
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="30" t="s">
         <v>42</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>43</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
       <c r="F26" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>45</v>
       </c>
       <c r="H26" s="31" t="n">
         <v>40</v>
@@ -4309,34 +4306,34 @@
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="31"/>
       <c r="B27" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="40"/>
-      <c r="S27" s="40"/>
-      <c r="T27" s="37"/>
-      <c r="U27" s="40"/>
-    </row>
-    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="41"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="31" t="n">
         <v>8</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
@@ -4345,13 +4342,13 @@
         <v>55</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
+        <v>65</v>
+      </c>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
       <c r="M28" s="34"/>
       <c r="N28" s="34" t="n">
         <v>40</v>
@@ -4363,7 +4360,7 @@
       <c r="Q28" s="34"/>
       <c r="R28" s="34"/>
       <c r="S28" s="36"/>
-      <c r="T28" s="37"/>
+      <c r="T28" s="38"/>
       <c r="U28" s="32" t="n">
         <f aca="false">SUM(H28:S28)</f>
         <v>55</v>
@@ -4374,7 +4371,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
@@ -4383,16 +4380,16 @@
         <v>60</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
+        <v>67</v>
+      </c>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
       <c r="M29" s="34"/>
       <c r="N29" s="34" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="O29" s="34" t="n">
         <v>20</v>
@@ -4401,70 +4398,70 @@
       <c r="Q29" s="34"/>
       <c r="R29" s="34"/>
       <c r="S29" s="36"/>
-      <c r="T29" s="37"/>
+      <c r="T29" s="38"/>
       <c r="U29" s="32" t="n">
         <f aca="false">SUM(H29:S29)</f>
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="31"/>
       <c r="B30" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="40"/>
-      <c r="R30" s="40"/>
-      <c r="S30" s="40"/>
-      <c r="T30" s="37"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="38"/>
       <c r="U30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="43" t="n">
+        <v>40</v>
+      </c>
+      <c r="G31" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="42" t="n">
-        <v>40</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42" t="n">
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43" t="n">
         <v>10</v>
       </c>
-      <c r="O31" s="42" t="n">
+      <c r="O31" s="43" t="n">
         <v>30</v>
       </c>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
       <c r="S31" s="36"/>
-      <c r="T31" s="37"/>
+      <c r="T31" s="38"/>
       <c r="U31" s="32" t="n">
         <f aca="false">SUM(H31:S31)</f>
         <v>40</v>
@@ -4473,133 +4470,133 @@
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="31"/>
       <c r="B32" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="40"/>
-      <c r="O32" s="40"/>
-      <c r="P32" s="40"/>
-      <c r="Q32" s="40"/>
-      <c r="R32" s="40"/>
-      <c r="S32" s="40"/>
-      <c r="T32" s="37"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="38"/>
       <c r="U32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="B33" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="42" t="n">
+      <c r="B33" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="43" t="n">
         <v>25</v>
       </c>
       <c r="G33" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="42" t="n">
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43" t="n">
         <v>25</v>
       </c>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="42"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
       <c r="S33" s="36"/>
-      <c r="T33" s="37"/>
+      <c r="T33" s="38"/>
       <c r="U33" s="32" t="n">
         <f aca="false">SUM(H33:S33)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="43" t="n">
+        <v>25</v>
+      </c>
+      <c r="G34" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="42" t="n">
-        <v>25</v>
-      </c>
-      <c r="G34" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42" t="n">
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="43" t="n">
+        <v>10</v>
+      </c>
+      <c r="P34" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="P34" s="42" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="42"/>
+      <c r="Q34" s="43"/>
+      <c r="R34" s="43"/>
       <c r="S34" s="36"/>
-      <c r="T34" s="37"/>
+      <c r="T34" s="38"/>
       <c r="U34" s="32" t="n">
         <f aca="false">SUM(H34:S34)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="31" t="n">
         <v>13</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="43" t="n">
+        <v>20</v>
+      </c>
+      <c r="G35" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="42" t="n">
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="43" t="n">
         <v>20</v>
       </c>
-      <c r="G35" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q35" s="42"/>
-      <c r="R35" s="42"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="43"/>
       <c r="S35" s="36"/>
-      <c r="T35" s="37"/>
+      <c r="T35" s="38"/>
       <c r="U35" s="32" t="n">
         <f aca="false">SUM(H35:S35)</f>
         <v>20</v>
@@ -4609,33 +4606,33 @@
       <c r="A36" s="31" t="n">
         <v>14</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="43" t="n">
+        <v>20</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="42" t="n">
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43" t="n">
         <v>20</v>
       </c>
-      <c r="G36" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q36" s="42"/>
-      <c r="R36" s="42"/>
+      <c r="Q36" s="43"/>
+      <c r="R36" s="43"/>
       <c r="S36" s="36"/>
-      <c r="T36" s="37"/>
+      <c r="T36" s="38"/>
       <c r="U36" s="32" t="n">
         <f aca="false">SUM(H36:S36)</f>
         <v>20</v>
@@ -4644,59 +4641,59 @@
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="31"/>
       <c r="B37" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="40"/>
-      <c r="N37" s="40"/>
-      <c r="O37" s="40"/>
-      <c r="P37" s="40"/>
-      <c r="Q37" s="40"/>
-      <c r="R37" s="40"/>
-      <c r="S37" s="40"/>
-      <c r="T37" s="37"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="41"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="41"/>
+      <c r="T37" s="38"/>
       <c r="U37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="43" t="n">
+        <v>30</v>
+      </c>
+      <c r="G38" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="42" t="n">
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="43"/>
+      <c r="Q38" s="43" t="n">
         <v>30</v>
       </c>
-      <c r="G38" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="42"/>
-      <c r="O38" s="42"/>
-      <c r="P38" s="42"/>
-      <c r="Q38" s="42" t="n">
-        <v>30</v>
-      </c>
-      <c r="R38" s="42"/>
+      <c r="R38" s="43"/>
       <c r="S38" s="36"/>
-      <c r="T38" s="37"/>
+      <c r="T38" s="38"/>
       <c r="U38" s="32" t="n">
         <f aca="false">SUM(H38:S38)</f>
         <v>30</v>
@@ -4706,33 +4703,33 @@
       <c r="A39" s="31" t="n">
         <v>16</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="43" t="n">
+        <v>20</v>
+      </c>
+      <c r="G39" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="42" t="n">
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="43"/>
+      <c r="P39" s="43"/>
+      <c r="Q39" s="43" t="n">
         <v>20</v>
       </c>
-      <c r="G39" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="42"/>
-      <c r="N39" s="42"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="42"/>
-      <c r="Q39" s="42" t="n">
-        <v>20</v>
-      </c>
-      <c r="R39" s="42"/>
+      <c r="R39" s="43"/>
       <c r="S39" s="36"/>
-      <c r="T39" s="37"/>
+      <c r="T39" s="38"/>
       <c r="U39" s="32" t="n">
         <f aca="false">SUM(H39:S39)</f>
         <v>20</v>
@@ -4742,73 +4739,73 @@
       <c r="A40" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="43" t="n">
+        <v>70</v>
+      </c>
+      <c r="G40" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="42" t="n">
-        <v>70</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="42" t="n">
-        <v>45</v>
-      </c>
-      <c r="Q40" s="42" t="n">
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="43"/>
+      <c r="P40" s="43" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q40" s="43" t="n">
         <v>25</v>
       </c>
-      <c r="R40" s="42"/>
+      <c r="R40" s="43"/>
       <c r="S40" s="36"/>
-      <c r="T40" s="37"/>
+      <c r="T40" s="38"/>
       <c r="U40" s="32" t="n">
         <f aca="false">SUM(H40:S40)</f>
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="43" t="n">
+        <v>40</v>
+      </c>
+      <c r="G41" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="42" t="n">
-        <v>40</v>
-      </c>
-      <c r="G41" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="37"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="42"/>
-      <c r="Q41" s="42" t="n">
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="43"/>
+      <c r="P41" s="43"/>
+      <c r="Q41" s="43" t="n">
         <v>25</v>
       </c>
-      <c r="R41" s="42" t="n">
+      <c r="R41" s="43" t="n">
         <v>15</v>
       </c>
       <c r="S41" s="36"/>
-      <c r="T41" s="37"/>
+      <c r="T41" s="38"/>
       <c r="U41" s="32" t="n">
         <f aca="false">SUM(H41:S41)</f>
         <v>40</v>
@@ -4817,122 +4814,122 @@
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="31"/>
       <c r="B42" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="37"/>
-      <c r="L42" s="37"/>
-      <c r="M42" s="40"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
-      <c r="P42" s="40"/>
-      <c r="Q42" s="40"/>
-      <c r="R42" s="40"/>
-      <c r="S42" s="40"/>
-      <c r="T42" s="37"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="41"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="41"/>
+      <c r="T42" s="38"/>
       <c r="U42" s="32"/>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="B43" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="42" t="n">
+      <c r="B43" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="43" t="n">
         <v>40</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="37"/>
-      <c r="L43" s="37"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42" t="n">
-        <v>40</v>
-      </c>
-      <c r="O43" s="42"/>
-      <c r="P43" s="42"/>
-      <c r="Q43" s="42"/>
-      <c r="R43" s="42"/>
+        <v>85</v>
+      </c>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="43"/>
+      <c r="N43" s="43" t="n">
+        <v>37</v>
+      </c>
+      <c r="O43" s="43"/>
+      <c r="P43" s="43"/>
+      <c r="Q43" s="43"/>
+      <c r="R43" s="43"/>
       <c r="S43" s="36"/>
-      <c r="T43" s="37"/>
+      <c r="T43" s="38"/>
       <c r="U43" s="32" t="n">
         <f aca="false">SUM(H43:S43)</f>
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="31"/>
       <c r="B44" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="37"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="40"/>
-      <c r="N44" s="40"/>
-      <c r="O44" s="40"/>
-      <c r="P44" s="40"/>
-      <c r="Q44" s="40"/>
-      <c r="R44" s="40"/>
-      <c r="S44" s="40"/>
-      <c r="T44" s="37"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="41"/>
+      <c r="P44" s="41"/>
+      <c r="Q44" s="41"/>
+      <c r="R44" s="41"/>
+      <c r="S44" s="41"/>
+      <c r="T44" s="38"/>
       <c r="U44" s="32"/>
     </row>
-    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="43" t="n">
+        <v>40</v>
+      </c>
+      <c r="G45" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="42" t="n">
-        <v>40</v>
-      </c>
-      <c r="G45" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="37"/>
-      <c r="L45" s="37"/>
-      <c r="M45" s="42"/>
-      <c r="N45" s="42" t="n">
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="43" t="n">
         <v>20</v>
       </c>
-      <c r="O45" s="42" t="n">
+      <c r="O45" s="43" t="n">
         <v>20</v>
       </c>
-      <c r="P45" s="42"/>
-      <c r="Q45" s="42"/>
-      <c r="R45" s="42"/>
+      <c r="P45" s="43"/>
+      <c r="Q45" s="43"/>
+      <c r="R45" s="43"/>
       <c r="S45" s="36"/>
-      <c r="T45" s="37"/>
+      <c r="T45" s="38"/>
       <c r="U45" s="32" t="n">
         <f aca="false">SUM(H45:S45)</f>
         <v>40</v>
@@ -4942,35 +4939,35 @@
       <c r="A46" s="31" t="n">
         <v>21</v>
       </c>
-      <c r="B46" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="42" t="n">
+      <c r="B46" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="43" t="n">
         <v>20</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="37"/>
-      <c r="L46" s="37"/>
-      <c r="M46" s="42"/>
-      <c r="N46" s="42"/>
-      <c r="O46" s="42" t="n">
+        <v>83</v>
+      </c>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="43"/>
+      <c r="O46" s="43" t="n">
         <v>10</v>
       </c>
-      <c r="P46" s="42" t="n">
+      <c r="P46" s="43" t="n">
         <v>10</v>
       </c>
-      <c r="Q46" s="42"/>
-      <c r="R46" s="42"/>
+      <c r="Q46" s="43"/>
+      <c r="R46" s="43"/>
       <c r="S46" s="36"/>
-      <c r="T46" s="37"/>
+      <c r="T46" s="38"/>
       <c r="U46" s="32" t="n">
         <f aca="false">SUM(H46:S46)</f>
         <v>20</v>
@@ -4979,59 +4976,59 @@
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="31"/>
       <c r="B47" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C47" s="29"/>
       <c r="D47" s="29"/>
       <c r="E47" s="29"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="37"/>
-      <c r="L47" s="37"/>
-      <c r="M47" s="40"/>
-      <c r="N47" s="40"/>
-      <c r="O47" s="40"/>
-      <c r="P47" s="40"/>
-      <c r="Q47" s="40"/>
-      <c r="R47" s="40"/>
-      <c r="S47" s="40"/>
-      <c r="T47" s="37"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="41"/>
+      <c r="O47" s="41"/>
+      <c r="P47" s="41"/>
+      <c r="Q47" s="41"/>
+      <c r="R47" s="41"/>
+      <c r="S47" s="41"/>
+      <c r="T47" s="38"/>
       <c r="U47" s="32"/>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="31" t="n">
         <v>22</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="43" t="n">
+        <v>15</v>
+      </c>
+      <c r="G48" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="42" t="n">
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="43"/>
+      <c r="N48" s="43"/>
+      <c r="O48" s="43"/>
+      <c r="P48" s="43"/>
+      <c r="Q48" s="43" t="n">
         <v>15</v>
       </c>
-      <c r="G48" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="42"/>
-      <c r="N48" s="42"/>
-      <c r="O48" s="42"/>
-      <c r="P48" s="42"/>
-      <c r="Q48" s="42" t="n">
-        <v>15</v>
-      </c>
-      <c r="R48" s="42"/>
+      <c r="R48" s="43"/>
       <c r="S48" s="36"/>
-      <c r="T48" s="37"/>
+      <c r="T48" s="38"/>
       <c r="U48" s="32" t="n">
         <f aca="false">SUM(H48:S48)</f>
         <v>15</v>
@@ -5041,35 +5038,35 @@
       <c r="A49" s="31" t="n">
         <v>23</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="43" t="n">
+        <v>30</v>
+      </c>
+      <c r="G49" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="42" t="n">
-        <v>30</v>
-      </c>
-      <c r="G49" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="42"/>
-      <c r="N49" s="42"/>
-      <c r="O49" s="42"/>
-      <c r="P49" s="42" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q49" s="42" t="n">
-        <v>15</v>
-      </c>
-      <c r="R49" s="42"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="43"/>
+      <c r="O49" s="43"/>
+      <c r="P49" s="43" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q49" s="43" t="n">
+        <v>10</v>
+      </c>
+      <c r="R49" s="43"/>
       <c r="S49" s="36"/>
-      <c r="T49" s="37"/>
+      <c r="T49" s="38"/>
       <c r="U49" s="32" t="n">
         <f aca="false">SUM(H49:S49)</f>
         <v>30</v>
@@ -5079,35 +5076,35 @@
       <c r="A50" s="31" t="n">
         <v>24</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="43" t="n">
+        <v>30</v>
+      </c>
+      <c r="G50" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="42" t="n">
-        <v>30</v>
-      </c>
-      <c r="G50" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="37"/>
-      <c r="L50" s="37"/>
-      <c r="M50" s="42"/>
-      <c r="N50" s="42"/>
-      <c r="O50" s="42"/>
-      <c r="P50" s="42" t="n">
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="38"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="43"/>
+      <c r="N50" s="43"/>
+      <c r="O50" s="43"/>
+      <c r="P50" s="43" t="n">
         <v>10</v>
       </c>
-      <c r="Q50" s="42" t="n">
+      <c r="Q50" s="43" t="n">
         <v>20</v>
       </c>
-      <c r="R50" s="42"/>
+      <c r="R50" s="43"/>
       <c r="S50" s="36"/>
-      <c r="T50" s="37"/>
+      <c r="T50" s="38"/>
       <c r="U50" s="32" t="n">
         <f aca="false">SUM(H50:S50)</f>
         <v>30</v>
@@ -5116,120 +5113,120 @@
     <row r="51" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="31"/>
       <c r="B51" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51" s="29"/>
       <c r="D51" s="29"/>
       <c r="E51" s="29"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="37"/>
-      <c r="J51" s="37"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
-      <c r="M51" s="40"/>
-      <c r="N51" s="40"/>
-      <c r="O51" s="40"/>
-      <c r="P51" s="40"/>
-      <c r="Q51" s="40"/>
-      <c r="R51" s="40"/>
-      <c r="S51" s="40"/>
-      <c r="T51" s="37"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
+      <c r="K51" s="38"/>
+      <c r="L51" s="38"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="41"/>
+      <c r="P51" s="41"/>
+      <c r="Q51" s="41"/>
+      <c r="R51" s="41"/>
+      <c r="S51" s="41"/>
+      <c r="T51" s="38"/>
       <c r="U51" s="32"/>
     </row>
     <row r="52" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="B52" s="41" t="s">
+      <c r="B52" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="43" t="n">
+        <v>20</v>
+      </c>
+      <c r="G52" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="42" t="n">
-        <v>20</v>
-      </c>
-      <c r="G52" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="H52" s="37"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="37"/>
-      <c r="M52" s="42"/>
-      <c r="N52" s="42"/>
-      <c r="O52" s="42" t="n">
-        <v>20</v>
-      </c>
-      <c r="P52" s="42"/>
-      <c r="Q52" s="42"/>
-      <c r="R52" s="42"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="43"/>
+      <c r="N52" s="43"/>
+      <c r="O52" s="43" t="n">
+        <v>10</v>
+      </c>
+      <c r="P52" s="43"/>
+      <c r="Q52" s="43"/>
+      <c r="R52" s="43"/>
       <c r="S52" s="36"/>
-      <c r="T52" s="37"/>
+      <c r="T52" s="38"/>
       <c r="U52" s="32" t="n">
         <f aca="false">SUM(H52:S52)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="31"/>
       <c r="B53" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C53" s="29"/>
       <c r="D53" s="29"/>
       <c r="E53" s="29"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="37"/>
-      <c r="M53" s="40"/>
-      <c r="N53" s="40"/>
-      <c r="O53" s="40"/>
-      <c r="P53" s="40"/>
-      <c r="Q53" s="40"/>
-      <c r="R53" s="40"/>
-      <c r="S53" s="40"/>
-      <c r="T53" s="37"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="38"/>
+      <c r="M53" s="41"/>
+      <c r="N53" s="41"/>
+      <c r="O53" s="41"/>
+      <c r="P53" s="41"/>
+      <c r="Q53" s="41"/>
+      <c r="R53" s="41"/>
+      <c r="S53" s="41"/>
+      <c r="T53" s="38"/>
       <c r="U53" s="32"/>
     </row>
     <row r="54" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="31" t="n">
         <v>26</v>
       </c>
-      <c r="B54" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="42" t="n">
+      <c r="B54" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="43" t="n">
         <v>10</v>
       </c>
       <c r="G54" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="37"/>
-      <c r="L54" s="37"/>
-      <c r="M54" s="42"/>
-      <c r="N54" s="42"/>
-      <c r="O54" s="42"/>
-      <c r="P54" s="42" t="n">
+        <v>83</v>
+      </c>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="38"/>
+      <c r="K54" s="38"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="43"/>
+      <c r="N54" s="43"/>
+      <c r="O54" s="43"/>
+      <c r="P54" s="43" t="n">
         <v>10</v>
       </c>
-      <c r="Q54" s="42"/>
-      <c r="R54" s="42"/>
+      <c r="Q54" s="43"/>
+      <c r="R54" s="43"/>
       <c r="S54" s="36"/>
-      <c r="T54" s="37"/>
+      <c r="T54" s="38"/>
       <c r="U54" s="32" t="n">
         <f aca="false">SUM(H54:S54)</f>
         <v>10</v>
@@ -5239,33 +5236,33 @@
       <c r="A55" s="31" t="n">
         <v>27</v>
       </c>
-      <c r="B55" s="41" t="s">
+      <c r="B55" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="43" t="n">
+        <v>30</v>
+      </c>
+      <c r="G55" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="42" t="n">
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
+      <c r="L55" s="38"/>
+      <c r="M55" s="43"/>
+      <c r="N55" s="43"/>
+      <c r="O55" s="43"/>
+      <c r="P55" s="43"/>
+      <c r="Q55" s="43"/>
+      <c r="R55" s="43" t="n">
         <v>30</v>
       </c>
-      <c r="G55" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="H55" s="37"/>
-      <c r="I55" s="37"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="37"/>
-      <c r="L55" s="37"/>
-      <c r="M55" s="42"/>
-      <c r="N55" s="42"/>
-      <c r="O55" s="42"/>
-      <c r="P55" s="42"/>
-      <c r="Q55" s="42"/>
-      <c r="R55" s="42" t="n">
-        <v>30</v>
-      </c>
       <c r="S55" s="36"/>
-      <c r="T55" s="37"/>
+      <c r="T55" s="38"/>
       <c r="U55" s="32" t="n">
         <f aca="false">SUM(H55:S55)</f>
         <v>30</v>
@@ -5274,59 +5271,59 @@
     <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="31"/>
       <c r="B56" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" s="29"/>
       <c r="D56" s="29"/>
       <c r="E56" s="29"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
-      <c r="L56" s="37"/>
-      <c r="M56" s="40"/>
-      <c r="N56" s="40"/>
-      <c r="O56" s="40"/>
-      <c r="P56" s="40"/>
-      <c r="Q56" s="40"/>
-      <c r="R56" s="40"/>
-      <c r="S56" s="40"/>
-      <c r="T56" s="37"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
+      <c r="L56" s="38"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="41"/>
+      <c r="P56" s="41"/>
+      <c r="Q56" s="41"/>
+      <c r="R56" s="41"/>
+      <c r="S56" s="41"/>
+      <c r="T56" s="38"/>
       <c r="U56" s="32"/>
     </row>
     <row r="57" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="31" t="n">
         <v>28</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="43" t="n">
+        <v>70</v>
+      </c>
+      <c r="G57" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="42" t="n">
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
+      <c r="L57" s="38"/>
+      <c r="M57" s="43"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="43"/>
+      <c r="P57" s="43"/>
+      <c r="Q57" s="43"/>
+      <c r="R57" s="43" t="n">
         <v>70</v>
       </c>
-      <c r="G57" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="37"/>
-      <c r="M57" s="42"/>
-      <c r="N57" s="42"/>
-      <c r="O57" s="42"/>
-      <c r="P57" s="42"/>
-      <c r="Q57" s="42"/>
-      <c r="R57" s="42" t="n">
-        <v>70</v>
-      </c>
       <c r="S57" s="36"/>
-      <c r="T57" s="37"/>
+      <c r="T57" s="38"/>
       <c r="U57" s="32" t="n">
         <f aca="false">SUM(H57:S57)</f>
         <v>70</v>
@@ -5336,33 +5333,33 @@
       <c r="A58" s="31" t="n">
         <v>29</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="43" t="n">
+        <v>20</v>
+      </c>
+      <c r="G58" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
-      <c r="E58" s="41"/>
-      <c r="F58" s="42" t="n">
-        <v>20</v>
-      </c>
-      <c r="G58" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="37"/>
-      <c r="L58" s="37"/>
-      <c r="M58" s="42"/>
-      <c r="N58" s="42"/>
-      <c r="O58" s="42"/>
-      <c r="P58" s="42"/>
-      <c r="Q58" s="42"/>
-      <c r="R58" s="42"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="38"/>
+      <c r="K58" s="38"/>
+      <c r="L58" s="38"/>
+      <c r="M58" s="43"/>
+      <c r="N58" s="43"/>
+      <c r="O58" s="43"/>
+      <c r="P58" s="43"/>
+      <c r="Q58" s="43"/>
+      <c r="R58" s="43"/>
       <c r="S58" s="36" t="n">
         <v>20</v>
       </c>
-      <c r="T58" s="37"/>
+      <c r="T58" s="38"/>
       <c r="U58" s="32" t="n">
         <f aca="false">SUM(H58:S58)</f>
         <v>20</v>
@@ -5372,35 +5369,35 @@
       <c r="A59" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="43" t="n">
+        <v>20</v>
+      </c>
+      <c r="G59" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="41"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="42" t="n">
-        <v>20</v>
-      </c>
-      <c r="G59" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="37"/>
-      <c r="L59" s="37"/>
-      <c r="M59" s="42"/>
-      <c r="N59" s="42"/>
-      <c r="O59" s="42"/>
-      <c r="P59" s="42"/>
-      <c r="Q59" s="42" t="n">
+      <c r="H59" s="38"/>
+      <c r="I59" s="38"/>
+      <c r="J59" s="38"/>
+      <c r="K59" s="38"/>
+      <c r="L59" s="38"/>
+      <c r="M59" s="43"/>
+      <c r="N59" s="43"/>
+      <c r="O59" s="43"/>
+      <c r="P59" s="43"/>
+      <c r="Q59" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="R59" s="42" t="n">
+      <c r="R59" s="43" t="n">
         <v>15</v>
       </c>
       <c r="S59" s="36"/>
-      <c r="T59" s="37"/>
+      <c r="T59" s="38"/>
       <c r="U59" s="32" t="n">
         <f aca="false">SUM(H59:S59)</f>
         <v>20</v>
@@ -5410,41 +5407,41 @@
       <c r="A60" s="31" t="n">
         <v>33</v>
       </c>
-      <c r="B60" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="42" t="n">
+      <c r="B60" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="42"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="43" t="n">
         <v>20</v>
       </c>
-      <c r="G60" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H60" s="37"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="37"/>
-      <c r="L60" s="37"/>
-      <c r="M60" s="42"/>
-      <c r="N60" s="42" t="n">
+      <c r="G60" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
+      <c r="K60" s="38"/>
+      <c r="L60" s="38"/>
+      <c r="M60" s="43"/>
+      <c r="N60" s="43" t="n">
         <v>4</v>
       </c>
-      <c r="O60" s="42" t="n">
+      <c r="O60" s="43" t="n">
         <v>4</v>
       </c>
-      <c r="P60" s="42" t="n">
+      <c r="P60" s="43" t="n">
         <v>4</v>
       </c>
-      <c r="Q60" s="42" t="n">
+      <c r="Q60" s="43" t="n">
         <v>4</v>
       </c>
-      <c r="R60" s="42" t="n">
+      <c r="R60" s="43" t="n">
         <v>4</v>
       </c>
       <c r="S60" s="36"/>
-      <c r="T60" s="37"/>
+      <c r="T60" s="38"/>
       <c r="U60" s="32" t="n">
         <f aca="false">SUM(H60:S60)</f>
         <v>20</v>
@@ -5453,67 +5450,67 @@
     <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="31"/>
       <c r="B61" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C61" s="29"/>
       <c r="D61" s="29"/>
       <c r="E61" s="29"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="37"/>
-      <c r="L61" s="37"/>
-      <c r="M61" s="40"/>
-      <c r="N61" s="40"/>
-      <c r="O61" s="40"/>
-      <c r="P61" s="40"/>
-      <c r="Q61" s="40"/>
-      <c r="R61" s="40"/>
-      <c r="S61" s="40"/>
-      <c r="T61" s="37"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
+      <c r="J61" s="38"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="38"/>
+      <c r="M61" s="41"/>
+      <c r="N61" s="41"/>
+      <c r="O61" s="41"/>
+      <c r="P61" s="41"/>
+      <c r="Q61" s="41"/>
+      <c r="R61" s="41"/>
+      <c r="S61" s="41"/>
+      <c r="T61" s="38"/>
       <c r="U61" s="32"/>
     </row>
     <row r="62" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="31" t="n">
         <v>32</v>
       </c>
-      <c r="B62" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" s="41"/>
-      <c r="D62" s="41"/>
-      <c r="E62" s="41"/>
-      <c r="F62" s="42" t="n">
+      <c r="B62" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="43" t="n">
         <v>35</v>
       </c>
-      <c r="G62" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="37"/>
-      <c r="L62" s="37"/>
-      <c r="M62" s="42"/>
-      <c r="N62" s="42" t="n">
+      <c r="G62" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="38"/>
+      <c r="K62" s="38"/>
+      <c r="L62" s="38"/>
+      <c r="M62" s="43"/>
+      <c r="N62" s="43" t="n">
         <v>7</v>
       </c>
-      <c r="O62" s="42" t="n">
+      <c r="O62" s="43" t="n">
         <v>7</v>
       </c>
-      <c r="P62" s="42" t="n">
+      <c r="P62" s="43" t="n">
         <v>7</v>
       </c>
-      <c r="Q62" s="42" t="n">
+      <c r="Q62" s="43" t="n">
         <v>7</v>
       </c>
-      <c r="R62" s="42" t="n">
+      <c r="R62" s="43" t="n">
         <v>7</v>
       </c>
       <c r="S62" s="36"/>
-      <c r="T62" s="37"/>
+      <c r="T62" s="38"/>
       <c r="U62" s="32" t="n">
         <f aca="false">SUM(H62:S62)</f>
         <v>35</v>
@@ -5521,48 +5518,48 @@
     </row>
     <row r="63" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="31"/>
-      <c r="B63" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="42" t="n">
+      <c r="B63" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="43" t="n">
         <f aca="false">(900-SUM(F28:F62))</f>
         <v>95</v>
       </c>
-      <c r="G63" s="42"/>
-      <c r="H63" s="37"/>
-      <c r="I63" s="37"/>
-      <c r="J63" s="37"/>
-      <c r="K63" s="37"/>
-      <c r="L63" s="37"/>
-      <c r="M63" s="42"/>
-      <c r="N63" s="42" t="n">
-        <f aca="false">SUM(H9:M9,N10)-SUM(H8:M8)-SUM(N27:N62)</f>
+      <c r="G63" s="43"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="38"/>
+      <c r="L63" s="38"/>
+      <c r="M63" s="43"/>
+      <c r="N63" s="43" t="n">
+        <f aca="false">N10-SUM(N27:N62)</f>
         <v>19</v>
       </c>
-      <c r="O63" s="42" t="n">
-        <f aca="false">SUM(H9:N9,N10:O10)-SUM(I8:N8)-SUM(O27:O62)</f>
-        <v>24</v>
-      </c>
-      <c r="P63" s="42" t="n">
-        <f aca="false">SUM(H9:O9,N10:P10)-SUM(H8:O8)-SUM(P27:P62)</f>
+      <c r="O63" s="43" t="n">
+        <f aca="false">O10-SUM(O27:O62)</f>
         <v>19</v>
       </c>
-      <c r="Q63" s="42" t="n">
-        <f aca="false">SUM(H9:P9,N10:Q10)-SUM(H8:P8)-SUM(Q27:Q62)</f>
-        <v>14</v>
-      </c>
-      <c r="R63" s="42" t="n">
-        <f aca="false">SUM(H9:Q9,N10:R10)-SUM(H8:Q8)-SUM(R27:R62)</f>
+      <c r="P63" s="43" t="n">
+        <f aca="false">P10-SUM(P27:P62)</f>
+        <v>19</v>
+      </c>
+      <c r="Q63" s="43" t="n">
+        <f aca="false">Q10-SUM(Q27:Q62)</f>
+        <v>19</v>
+      </c>
+      <c r="R63" s="43" t="n">
+        <f aca="false">R10-SUM(R27:R62)</f>
         <v>17</v>
       </c>
-      <c r="S63" s="42" t="n">
-        <f aca="false">SUM(H9:R9,N10:S10)-SUM(H8:R8)-SUM(S27:S62)</f>
+      <c r="S63" s="43" t="n">
+        <f aca="false">S10-SUM(S27:S62)</f>
         <v>2</v>
       </c>
-      <c r="T63" s="37"/>
+      <c r="T63" s="38"/>
       <c r="U63" s="32" t="n">
         <f aca="false">SUM(H63:S63)</f>
         <v>95</v>
@@ -5570,108 +5567,108 @@
     </row>
     <row r="64" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="31"/>
-      <c r="B64" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
-      <c r="F64" s="42" t="n">
+      <c r="B64" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="43" t="n">
         <f aca="false">SUM(F28:F63)</f>
         <v>900</v>
       </c>
-      <c r="G64" s="42"/>
-      <c r="H64" s="37"/>
-      <c r="I64" s="37"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="37"/>
-      <c r="L64" s="37"/>
-      <c r="M64" s="42"/>
-      <c r="N64" s="42" t="n">
+      <c r="G64" s="43"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="43"/>
+      <c r="N64" s="43" t="n">
         <f aca="false">SUM(N28:N63)</f>
-        <v>180</v>
-      </c>
-      <c r="O64" s="42" t="n">
+        <v>167</v>
+      </c>
+      <c r="O64" s="43" t="n">
         <f aca="false">SUM(O28:O63)</f>
-        <v>180</v>
-      </c>
-      <c r="P64" s="42" t="n">
+        <v>170</v>
+      </c>
+      <c r="P64" s="43" t="n">
         <f aca="false">SUM(P28:P63)</f>
-        <v>180</v>
-      </c>
-      <c r="Q64" s="42" t="n">
+        <v>160</v>
+      </c>
+      <c r="Q64" s="43" t="n">
         <f aca="false">SUM(Q28:Q63)</f>
         <v>180</v>
       </c>
-      <c r="R64" s="42" t="n">
+      <c r="R64" s="43" t="n">
         <f aca="false">SUM(R28:R63)</f>
         <v>158</v>
       </c>
-      <c r="S64" s="42" t="n">
+      <c r="S64" s="43" t="n">
         <f aca="false">SUM(S28:S63)</f>
         <v>22</v>
       </c>
-      <c r="T64" s="37"/>
+      <c r="T64" s="38"/>
       <c r="U64" s="32" t="n">
         <f aca="false">SUM(H64:S64)</f>
-        <v>900</v>
+        <v>857</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="31"/>
-      <c r="B65" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="C65" s="44"/>
-      <c r="D65" s="44"/>
-      <c r="E65" s="44"/>
-      <c r="F65" s="45" t="n">
+      <c r="B65" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="46" t="n">
         <f aca="false">SUM(F24,F64)</f>
         <v>1120</v>
       </c>
-      <c r="G65" s="45"/>
-      <c r="H65" s="37"/>
-      <c r="I65" s="37"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="37"/>
-      <c r="L65" s="37"/>
-      <c r="M65" s="45" t="n">
+      <c r="G65" s="46"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
+      <c r="K65" s="38"/>
+      <c r="L65" s="38"/>
+      <c r="M65" s="46" t="n">
         <f aca="false">SUM(M13:M23,M27:M63)</f>
         <v>34</v>
       </c>
-      <c r="N65" s="45" t="n">
+      <c r="N65" s="46" t="n">
         <f aca="false">SUM(N13:N23,N27:N63)</f>
-        <v>180</v>
-      </c>
-      <c r="O65" s="45" t="n">
+        <v>167</v>
+      </c>
+      <c r="O65" s="46" t="n">
         <f aca="false">SUM(O13:O23,O27:O63)</f>
-        <v>180</v>
-      </c>
-      <c r="P65" s="45" t="n">
+        <v>170</v>
+      </c>
+      <c r="P65" s="46" t="n">
         <f aca="false">SUM(P13:P23,P27:P63)</f>
-        <v>180</v>
-      </c>
-      <c r="Q65" s="45" t="n">
+        <v>160</v>
+      </c>
+      <c r="Q65" s="46" t="n">
         <f aca="false">SUM(Q13:Q23,Q27:Q63)</f>
         <v>180</v>
       </c>
-      <c r="R65" s="45" t="n">
+      <c r="R65" s="46" t="n">
         <f aca="false">SUM(R13:R23,R27:R63)</f>
         <v>158</v>
       </c>
-      <c r="S65" s="45" t="n">
+      <c r="S65" s="46" t="n">
         <f aca="false">SUM(S13:S23,S27:S63)</f>
         <v>22</v>
       </c>
-      <c r="T65" s="37"/>
+      <c r="T65" s="38"/>
       <c r="U65" s="32" t="n">
         <f aca="false">SUM(H65:S65)</f>
-        <v>934</v>
+        <v>891</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B66" s="27"/>
       <c r="C66" s="27"/>
@@ -5680,7 +5677,7 @@
       <c r="F66" s="27"/>
       <c r="G66" s="27"/>
       <c r="H66" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I66" s="27"/>
       <c r="J66" s="27"/>
@@ -5698,16 +5695,16 @@
     </row>
     <row r="67" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B67" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="C67" s="46"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="46"/>
-      <c r="G67" s="46"/>
+        <v>41</v>
+      </c>
+      <c r="B67" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
       <c r="H67" s="31" t="n">
         <v>40</v>
       </c>
@@ -5753,366 +5750,366 @@
       <c r="A68" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="B68" s="47" t="s">
+      <c r="B68" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="48"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="49"/>
+      <c r="L68" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-      <c r="H68" s="48"/>
-      <c r="I68" s="48"/>
-      <c r="J68" s="48"/>
-      <c r="K68" s="48"/>
-      <c r="L68" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="M68" s="48"/>
+      <c r="M68" s="49"/>
       <c r="N68" s="8"/>
       <c r="O68" s="8"/>
       <c r="P68" s="8"/>
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
-      <c r="S68" s="48"/>
-      <c r="T68" s="48"/>
-      <c r="U68" s="40"/>
+      <c r="S68" s="49"/>
+      <c r="T68" s="49"/>
+      <c r="U68" s="41"/>
     </row>
     <row r="69" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="B69" s="47" t="s">
+      <c r="B69" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="48"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="48"/>
+      <c r="H69" s="49"/>
+      <c r="I69" s="49"/>
+      <c r="J69" s="49"/>
+      <c r="K69" s="49"/>
+      <c r="L69" s="49"/>
+      <c r="M69" s="49" t="s">
         <v>122</v>
-      </c>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="48"/>
-      <c r="I69" s="48"/>
-      <c r="J69" s="48"/>
-      <c r="K69" s="48"/>
-      <c r="L69" s="48"/>
-      <c r="M69" s="48" t="s">
-        <v>123</v>
       </c>
       <c r="N69" s="8"/>
       <c r="O69" s="8"/>
       <c r="P69" s="8"/>
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
-      <c r="S69" s="48"/>
-      <c r="T69" s="48"/>
+      <c r="S69" s="49"/>
+      <c r="T69" s="49"/>
       <c r="U69" s="32"/>
     </row>
     <row r="70" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="B70" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C70" s="47"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="48"/>
-      <c r="I70" s="48"/>
-      <c r="J70" s="48"/>
-      <c r="K70" s="48"/>
-      <c r="L70" s="48"/>
-      <c r="M70" s="48"/>
+      <c r="B70" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="48"/>
+      <c r="G70" s="48"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="49"/>
+      <c r="L70" s="49"/>
+      <c r="M70" s="49"/>
       <c r="N70" s="8"/>
       <c r="O70" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P70" s="8"/>
       <c r="Q70" s="8"/>
       <c r="R70" s="8"/>
-      <c r="S70" s="48"/>
-      <c r="T70" s="48"/>
+      <c r="S70" s="49"/>
+      <c r="T70" s="49"/>
       <c r="U70" s="32"/>
     </row>
     <row r="71" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="B71" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="47"/>
-      <c r="F71" s="47"/>
-      <c r="G71" s="47"/>
-      <c r="H71" s="48"/>
-      <c r="I71" s="48"/>
-      <c r="J71" s="48"/>
-      <c r="K71" s="48"/>
-      <c r="L71" s="48"/>
-      <c r="M71" s="48"/>
+      <c r="B71" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C71" s="48"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
+      <c r="F71" s="48"/>
+      <c r="G71" s="48"/>
+      <c r="H71" s="49"/>
+      <c r="I71" s="49"/>
+      <c r="J71" s="49"/>
+      <c r="K71" s="49"/>
+      <c r="L71" s="49"/>
+      <c r="M71" s="49"/>
       <c r="N71" s="8"/>
       <c r="O71" s="8"/>
       <c r="P71" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
-      <c r="S71" s="48"/>
-      <c r="T71" s="48"/>
-      <c r="U71" s="40"/>
+      <c r="S71" s="49"/>
+      <c r="T71" s="49"/>
+      <c r="U71" s="41"/>
     </row>
     <row r="72" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="B72" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
-      <c r="F72" s="47"/>
-      <c r="G72" s="47"/>
-      <c r="H72" s="48"/>
-      <c r="I72" s="48"/>
-      <c r="J72" s="48"/>
-      <c r="K72" s="48"/>
-      <c r="L72" s="48"/>
-      <c r="M72" s="48"/>
-      <c r="N72" s="49"/>
-      <c r="O72" s="49"/>
-      <c r="P72" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q72" s="49"/>
-      <c r="R72" s="49"/>
-      <c r="S72" s="48"/>
-      <c r="T72" s="48"/>
+      <c r="B72" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="48"/>
+      <c r="F72" s="48"/>
+      <c r="G72" s="48"/>
+      <c r="H72" s="49"/>
+      <c r="I72" s="49"/>
+      <c r="J72" s="49"/>
+      <c r="K72" s="49"/>
+      <c r="L72" s="49"/>
+      <c r="M72" s="49"/>
+      <c r="N72" s="50"/>
+      <c r="O72" s="50"/>
+      <c r="P72" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q72" s="50"/>
+      <c r="R72" s="50"/>
+      <c r="S72" s="49"/>
+      <c r="T72" s="49"/>
       <c r="U72" s="32"/>
     </row>
     <row r="73" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="B73" s="47" t="s">
-        <v>128</v>
-      </c>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
-      <c r="E73" s="47"/>
-      <c r="F73" s="47"/>
-      <c r="G73" s="47"/>
-      <c r="H73" s="48"/>
-      <c r="I73" s="48"/>
-      <c r="J73" s="48"/>
-      <c r="K73" s="48"/>
-      <c r="L73" s="48"/>
-      <c r="M73" s="48"/>
+      <c r="B73" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="48"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="49"/>
+      <c r="I73" s="49"/>
+      <c r="J73" s="49"/>
+      <c r="K73" s="49"/>
+      <c r="L73" s="49"/>
+      <c r="M73" s="49"/>
       <c r="N73" s="8"/>
       <c r="O73" s="8"/>
       <c r="P73" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
-      <c r="S73" s="48"/>
-      <c r="T73" s="48"/>
-      <c r="U73" s="40"/>
+      <c r="S73" s="49"/>
+      <c r="T73" s="49"/>
+      <c r="U73" s="41"/>
     </row>
     <row r="74" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="B74" s="47" t="s">
+      <c r="B74" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C74" s="48"/>
+      <c r="D74" s="48"/>
+      <c r="E74" s="48"/>
+      <c r="F74" s="48"/>
+      <c r="G74" s="48"/>
+      <c r="H74" s="49"/>
+      <c r="I74" s="49"/>
+      <c r="J74" s="49"/>
+      <c r="K74" s="49"/>
+      <c r="L74" s="49"/>
+      <c r="M74" s="49"/>
+      <c r="N74" s="50"/>
+      <c r="O74" s="50"/>
+      <c r="P74" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
-      <c r="F74" s="47"/>
-      <c r="G74" s="47"/>
-      <c r="H74" s="48"/>
-      <c r="I74" s="48"/>
-      <c r="J74" s="48"/>
-      <c r="K74" s="48"/>
-      <c r="L74" s="48"/>
-      <c r="M74" s="48"/>
-      <c r="N74" s="49"/>
-      <c r="O74" s="49"/>
-      <c r="P74" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q74" s="49"/>
-      <c r="R74" s="49"/>
-      <c r="S74" s="48"/>
-      <c r="T74" s="48"/>
+      <c r="Q74" s="50"/>
+      <c r="R74" s="50"/>
+      <c r="S74" s="49"/>
+      <c r="T74" s="49"/>
       <c r="U74" s="32"/>
     </row>
     <row r="75" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="B75" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="47"/>
-      <c r="H75" s="48"/>
-      <c r="I75" s="48"/>
-      <c r="J75" s="48"/>
-      <c r="K75" s="48"/>
-      <c r="L75" s="48"/>
-      <c r="M75" s="48"/>
-      <c r="N75" s="49"/>
-      <c r="O75" s="49"/>
-      <c r="P75" s="49"/>
-      <c r="Q75" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="R75" s="49"/>
-      <c r="S75" s="48"/>
-      <c r="T75" s="48"/>
+      <c r="B75" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C75" s="48"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="48"/>
+      <c r="H75" s="49"/>
+      <c r="I75" s="49"/>
+      <c r="J75" s="49"/>
+      <c r="K75" s="49"/>
+      <c r="L75" s="49"/>
+      <c r="M75" s="49"/>
+      <c r="N75" s="50"/>
+      <c r="O75" s="50"/>
+      <c r="P75" s="50"/>
+      <c r="Q75" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="R75" s="50"/>
+      <c r="S75" s="49"/>
+      <c r="T75" s="49"/>
       <c r="U75" s="32"/>
     </row>
     <row r="76" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="B76" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="C76" s="47"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
-      <c r="H76" s="48"/>
-      <c r="I76" s="48"/>
-      <c r="J76" s="48"/>
-      <c r="K76" s="48"/>
-      <c r="L76" s="48"/>
-      <c r="M76" s="48"/>
-      <c r="N76" s="49"/>
-      <c r="O76" s="49"/>
-      <c r="P76" s="49"/>
-      <c r="Q76" s="49" t="s">
-        <v>121</v>
-      </c>
-      <c r="R76" s="49"/>
-      <c r="S76" s="48"/>
-      <c r="T76" s="48"/>
+      <c r="B76" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C76" s="48"/>
+      <c r="D76" s="48"/>
+      <c r="E76" s="48"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="48"/>
+      <c r="H76" s="49"/>
+      <c r="I76" s="49"/>
+      <c r="J76" s="49"/>
+      <c r="K76" s="49"/>
+      <c r="L76" s="49"/>
+      <c r="M76" s="49"/>
+      <c r="N76" s="50"/>
+      <c r="O76" s="50"/>
+      <c r="P76" s="50"/>
+      <c r="Q76" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="R76" s="50"/>
+      <c r="S76" s="49"/>
+      <c r="T76" s="49"/>
       <c r="U76" s="32"/>
     </row>
     <row r="77" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="B77" s="47" t="s">
+      <c r="B77" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" s="48"/>
+      <c r="D77" s="48"/>
+      <c r="E77" s="48"/>
+      <c r="F77" s="48"/>
+      <c r="G77" s="48"/>
+      <c r="H77" s="49"/>
+      <c r="I77" s="49"/>
+      <c r="J77" s="49"/>
+      <c r="K77" s="49"/>
+      <c r="L77" s="49"/>
+      <c r="M77" s="49"/>
+      <c r="N77" s="50"/>
+      <c r="O77" s="50"/>
+      <c r="P77" s="50"/>
+      <c r="Q77" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="C77" s="47"/>
-      <c r="D77" s="47"/>
-      <c r="E77" s="47"/>
-      <c r="F77" s="47"/>
-      <c r="G77" s="47"/>
-      <c r="H77" s="48"/>
-      <c r="I77" s="48"/>
-      <c r="J77" s="48"/>
-      <c r="K77" s="48"/>
-      <c r="L77" s="48"/>
-      <c r="M77" s="48"/>
-      <c r="N77" s="49"/>
-      <c r="O77" s="49"/>
-      <c r="P77" s="49"/>
-      <c r="Q77" s="49" t="s">
-        <v>134</v>
-      </c>
-      <c r="R77" s="49"/>
-      <c r="S77" s="48"/>
-      <c r="T77" s="48"/>
+      <c r="R77" s="50"/>
+      <c r="S77" s="49"/>
+      <c r="T77" s="49"/>
       <c r="U77" s="32"/>
     </row>
     <row r="78" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="31" t="n">
         <v>11</v>
       </c>
-      <c r="B78" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="C78" s="47"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="47"/>
-      <c r="G78" s="47"/>
-      <c r="H78" s="48"/>
-      <c r="I78" s="48"/>
-      <c r="J78" s="48"/>
-      <c r="K78" s="48"/>
-      <c r="L78" s="48"/>
-      <c r="M78" s="48"/>
+      <c r="B78" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C78" s="48"/>
+      <c r="D78" s="48"/>
+      <c r="E78" s="48"/>
+      <c r="F78" s="48"/>
+      <c r="G78" s="48"/>
+      <c r="H78" s="49"/>
+      <c r="I78" s="49"/>
+      <c r="J78" s="49"/>
+      <c r="K78" s="49"/>
+      <c r="L78" s="49"/>
+      <c r="M78" s="49"/>
       <c r="N78" s="8"/>
       <c r="O78" s="8"/>
       <c r="P78" s="8"/>
       <c r="Q78" s="8"/>
       <c r="R78" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="S78" s="48"/>
-      <c r="T78" s="48"/>
-      <c r="U78" s="40"/>
+        <v>124</v>
+      </c>
+      <c r="S78" s="49"/>
+      <c r="T78" s="49"/>
+      <c r="U78" s="41"/>
     </row>
     <row r="79" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="31" t="n">
         <v>12</v>
       </c>
-      <c r="B79" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="C79" s="47"/>
-      <c r="D79" s="47"/>
-      <c r="E79" s="47"/>
-      <c r="F79" s="47"/>
-      <c r="G79" s="47"/>
-      <c r="H79" s="48"/>
-      <c r="I79" s="48"/>
-      <c r="J79" s="48"/>
-      <c r="K79" s="48"/>
-      <c r="L79" s="48"/>
-      <c r="M79" s="48"/>
+      <c r="B79" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="C79" s="48"/>
+      <c r="D79" s="48"/>
+      <c r="E79" s="48"/>
+      <c r="F79" s="48"/>
+      <c r="G79" s="48"/>
+      <c r="H79" s="49"/>
+      <c r="I79" s="49"/>
+      <c r="J79" s="49"/>
+      <c r="K79" s="49"/>
+      <c r="L79" s="49"/>
+      <c r="M79" s="49"/>
       <c r="N79" s="8"/>
       <c r="O79" s="8"/>
       <c r="P79" s="8"/>
       <c r="Q79" s="8"/>
       <c r="R79" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="S79" s="48"/>
-      <c r="T79" s="48"/>
+        <v>120</v>
+      </c>
+      <c r="S79" s="49"/>
+      <c r="T79" s="49"/>
       <c r="U79" s="32"/>
     </row>
     <row r="80" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B80" s="27"/>
       <c r="C80" s="27"/>
       <c r="D80" s="27"/>
       <c r="E80" s="27"/>
       <c r="F80" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G80" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G80" s="27" t="s">
-        <v>40</v>
-      </c>
       <c r="H80" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I80" s="27"/>
       <c r="J80" s="27"/>
@@ -6130,253 +6127,253 @@
     </row>
     <row r="81" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B81" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C81" s="47"/>
+      <c r="D81" s="47"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="47"/>
+      <c r="G81" s="47"/>
+      <c r="H81" s="51" t="n">
+        <v>40</v>
+      </c>
+      <c r="I81" s="51" t="n">
+        <v>41</v>
+      </c>
+      <c r="J81" s="51" t="n">
         <v>42</v>
       </c>
-      <c r="B81" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="C81" s="46"/>
-      <c r="D81" s="46"/>
-      <c r="E81" s="46"/>
-      <c r="F81" s="46"/>
-      <c r="G81" s="46"/>
-      <c r="H81" s="50" t="n">
-        <v>40</v>
-      </c>
-      <c r="I81" s="50" t="n">
-        <v>41</v>
-      </c>
-      <c r="J81" s="50" t="n">
-        <v>42</v>
-      </c>
-      <c r="K81" s="50" t="n">
+      <c r="K81" s="51" t="n">
         <v>43</v>
       </c>
-      <c r="L81" s="50" t="n">
+      <c r="L81" s="51" t="n">
         <v>44</v>
       </c>
-      <c r="M81" s="50" t="n">
+      <c r="M81" s="51" t="n">
         <v>45</v>
       </c>
-      <c r="N81" s="50" t="n">
+      <c r="N81" s="51" t="n">
         <v>46</v>
       </c>
-      <c r="O81" s="50" t="n">
+      <c r="O81" s="51" t="n">
         <v>47</v>
       </c>
-      <c r="P81" s="50" t="n">
+      <c r="P81" s="51" t="n">
         <v>48</v>
       </c>
-      <c r="Q81" s="50" t="n">
+      <c r="Q81" s="51" t="n">
         <v>49</v>
       </c>
-      <c r="R81" s="50" t="n">
+      <c r="R81" s="51" t="n">
         <v>50</v>
       </c>
-      <c r="S81" s="50" t="n">
+      <c r="S81" s="51" t="n">
         <v>51</v>
       </c>
-      <c r="T81" s="50" t="n">
+      <c r="T81" s="51" t="n">
         <v>52</v>
       </c>
-      <c r="U81" s="51"/>
+      <c r="U81" s="52"/>
     </row>
     <row r="82" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="31" t="n">
         <v>0</v>
       </c>
-      <c r="B82" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C82" s="47"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
-      <c r="F82" s="47"/>
-      <c r="G82" s="47"/>
-      <c r="H82" s="48"/>
-      <c r="I82" s="48"/>
-      <c r="J82" s="48"/>
-      <c r="K82" s="48"/>
-      <c r="L82" s="48"/>
-      <c r="M82" s="48"/>
+      <c r="B82" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C82" s="48"/>
+      <c r="D82" s="48"/>
+      <c r="E82" s="48"/>
+      <c r="F82" s="48"/>
+      <c r="G82" s="48"/>
+      <c r="H82" s="49"/>
+      <c r="I82" s="49"/>
+      <c r="J82" s="49"/>
+      <c r="K82" s="49"/>
+      <c r="L82" s="49"/>
+      <c r="M82" s="49"/>
       <c r="N82" s="8"/>
       <c r="O82" s="8"/>
       <c r="P82" s="8"/>
       <c r="Q82" s="8"/>
       <c r="R82" s="8"/>
-      <c r="S82" s="48"/>
-      <c r="T82" s="48"/>
-      <c r="U82" s="52"/>
+      <c r="S82" s="49"/>
+      <c r="T82" s="49"/>
+      <c r="U82" s="53"/>
     </row>
     <row r="83" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="B83" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="C83" s="47"/>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47"/>
-      <c r="F83" s="47"/>
-      <c r="G83" s="47"/>
-      <c r="H83" s="48"/>
-      <c r="I83" s="48"/>
-      <c r="J83" s="48"/>
-      <c r="K83" s="48"/>
-      <c r="L83" s="48"/>
-      <c r="M83" s="48"/>
+      <c r="B83" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C83" s="48"/>
+      <c r="D83" s="48"/>
+      <c r="E83" s="48"/>
+      <c r="F83" s="48"/>
+      <c r="G83" s="48"/>
+      <c r="H83" s="49"/>
+      <c r="I83" s="49"/>
+      <c r="J83" s="49"/>
+      <c r="K83" s="49"/>
+      <c r="L83" s="49"/>
+      <c r="M83" s="49"/>
       <c r="N83" s="8"/>
       <c r="O83" s="8"/>
       <c r="P83" s="8"/>
       <c r="Q83" s="8"/>
       <c r="R83" s="8"/>
-      <c r="S83" s="48"/>
-      <c r="T83" s="48"/>
-      <c r="U83" s="51"/>
+      <c r="S83" s="49"/>
+      <c r="T83" s="49"/>
+      <c r="U83" s="52"/>
     </row>
     <row r="84" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="B84" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="C84" s="47"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
-      <c r="F84" s="47"/>
-      <c r="G84" s="47"/>
-      <c r="H84" s="48"/>
-      <c r="I84" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="J84" s="48"/>
-      <c r="K84" s="48"/>
-      <c r="L84" s="48"/>
-      <c r="M84" s="48"/>
+      <c r="B84" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C84" s="48"/>
+      <c r="D84" s="48"/>
+      <c r="E84" s="48"/>
+      <c r="F84" s="48"/>
+      <c r="G84" s="48"/>
+      <c r="H84" s="49"/>
+      <c r="I84" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="J84" s="49"/>
+      <c r="K84" s="49"/>
+      <c r="L84" s="49"/>
+      <c r="M84" s="49"/>
       <c r="N84" s="8"/>
       <c r="O84" s="8"/>
       <c r="P84" s="8"/>
       <c r="Q84" s="8"/>
       <c r="R84" s="8"/>
-      <c r="S84" s="48"/>
-      <c r="T84" s="48"/>
-      <c r="U84" s="51"/>
+      <c r="S84" s="49"/>
+      <c r="T84" s="49"/>
+      <c r="U84" s="52"/>
     </row>
     <row r="85" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="B85" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="C85" s="47"/>
-      <c r="D85" s="47"/>
-      <c r="E85" s="47"/>
-      <c r="F85" s="47"/>
-      <c r="G85" s="47"/>
-      <c r="H85" s="48"/>
-      <c r="I85" s="48"/>
-      <c r="J85" s="48"/>
-      <c r="K85" s="48"/>
-      <c r="L85" s="48"/>
-      <c r="M85" s="48" t="s">
-        <v>134</v>
+      <c r="B85" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C85" s="48"/>
+      <c r="D85" s="48"/>
+      <c r="E85" s="48"/>
+      <c r="F85" s="48"/>
+      <c r="G85" s="48"/>
+      <c r="H85" s="49"/>
+      <c r="I85" s="49"/>
+      <c r="J85" s="49"/>
+      <c r="K85" s="49"/>
+      <c r="L85" s="49"/>
+      <c r="M85" s="49" t="s">
+        <v>133</v>
       </c>
       <c r="N85" s="8"/>
       <c r="O85" s="8"/>
       <c r="P85" s="8"/>
       <c r="Q85" s="8"/>
       <c r="R85" s="8"/>
-      <c r="S85" s="48"/>
-      <c r="T85" s="48"/>
-      <c r="U85" s="52"/>
+      <c r="S85" s="49"/>
+      <c r="T85" s="49"/>
+      <c r="U85" s="53"/>
     </row>
     <row r="86" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="B86" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="C86" s="53"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="53"/>
-      <c r="G86" s="53"/>
-      <c r="H86" s="48"/>
-      <c r="I86" s="48"/>
-      <c r="J86" s="48"/>
-      <c r="K86" s="48"/>
-      <c r="L86" s="48"/>
-      <c r="M86" s="48"/>
-      <c r="N86" s="49"/>
-      <c r="O86" s="49"/>
-      <c r="P86" s="49"/>
-      <c r="Q86" s="49"/>
-      <c r="R86" s="49"/>
-      <c r="S86" s="48"/>
-      <c r="T86" s="48"/>
-      <c r="U86" s="51"/>
+      <c r="B86" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="C86" s="54"/>
+      <c r="D86" s="54"/>
+      <c r="E86" s="54"/>
+      <c r="F86" s="54"/>
+      <c r="G86" s="54"/>
+      <c r="H86" s="49"/>
+      <c r="I86" s="49"/>
+      <c r="J86" s="49"/>
+      <c r="K86" s="49"/>
+      <c r="L86" s="49"/>
+      <c r="M86" s="49"/>
+      <c r="N86" s="50"/>
+      <c r="O86" s="50"/>
+      <c r="P86" s="50"/>
+      <c r="Q86" s="50"/>
+      <c r="R86" s="50"/>
+      <c r="S86" s="49"/>
+      <c r="T86" s="49"/>
+      <c r="U86" s="52"/>
     </row>
     <row r="87" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="B87" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="C87" s="47"/>
-      <c r="D87" s="47"/>
-      <c r="E87" s="47"/>
-      <c r="F87" s="47"/>
-      <c r="G87" s="47"/>
-      <c r="H87" s="48"/>
-      <c r="I87" s="48"/>
-      <c r="J87" s="48"/>
-      <c r="K87" s="48"/>
-      <c r="L87" s="48"/>
-      <c r="M87" s="48"/>
+      <c r="B87" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C87" s="48"/>
+      <c r="D87" s="48"/>
+      <c r="E87" s="48"/>
+      <c r="F87" s="48"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="49"/>
+      <c r="I87" s="49"/>
+      <c r="J87" s="49"/>
+      <c r="K87" s="49"/>
+      <c r="L87" s="49"/>
+      <c r="M87" s="49"/>
       <c r="N87" s="8"/>
       <c r="O87" s="8"/>
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
       <c r="R87" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="S87" s="48"/>
-      <c r="T87" s="48"/>
-      <c r="U87" s="52"/>
+        <v>129</v>
+      </c>
+      <c r="S87" s="49"/>
+      <c r="T87" s="49"/>
+      <c r="U87" s="53"/>
     </row>
     <row r="88" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="B88" s="47" t="s">
-        <v>145</v>
-      </c>
-      <c r="C88" s="47"/>
-      <c r="D88" s="47"/>
-      <c r="E88" s="47"/>
-      <c r="F88" s="47"/>
-      <c r="G88" s="47"/>
-      <c r="H88" s="48"/>
-      <c r="I88" s="48"/>
-      <c r="J88" s="48"/>
-      <c r="K88" s="48"/>
-      <c r="L88" s="48"/>
-      <c r="M88" s="48"/>
-      <c r="N88" s="48"/>
-      <c r="O88" s="48"/>
-      <c r="P88" s="48"/>
-      <c r="Q88" s="48"/>
-      <c r="R88" s="48"/>
-      <c r="S88" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="T88" s="48"/>
-      <c r="U88" s="51"/>
+      <c r="B88" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88" s="48"/>
+      <c r="D88" s="48"/>
+      <c r="E88" s="48"/>
+      <c r="F88" s="48"/>
+      <c r="G88" s="48"/>
+      <c r="H88" s="49"/>
+      <c r="I88" s="49"/>
+      <c r="J88" s="49"/>
+      <c r="K88" s="49"/>
+      <c r="L88" s="49"/>
+      <c r="M88" s="49"/>
+      <c r="N88" s="49"/>
+      <c r="O88" s="49"/>
+      <c r="P88" s="49"/>
+      <c r="Q88" s="49"/>
+      <c r="R88" s="49"/>
+      <c r="S88" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="T88" s="49"/>
+      <c r="U88" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="101">

</xml_diff>

<commit_message>
log time JA, YH
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -1012,7 +1012,7 @@
   </sheetPr>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="V32" activeCellId="0" sqref="V32"/>
     </sheetView>
   </sheetViews>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="H4" s="8" t="n">
         <f aca="false">SUM(H17:H23)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I4" s="8" t="n">
         <f aca="false">SUM(I17:I23)</f>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="M4" s="9" t="n">
         <f aca="false">SUM(C4:L4)</f>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>7</v>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="H9" s="8" t="n">
         <f aca="false">SUM(V30:V36)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I9" s="8" t="n">
         <f aca="false">SUM(W30:W36)</f>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="M9" s="9" t="n">
         <f aca="false">SUM(C9:L9)</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O9" s="10" t="s">
         <v>17</v>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="H11" s="9" t="n">
         <f aca="false">SUM(H4:H10)</f>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I11" s="9" t="n">
         <f aca="false">SUM(I4:I10)</f>
@@ -1694,7 +1694,7 @@
       </c>
       <c r="M11" s="9" t="n">
         <f aca="false">SUM(C11:L11)</f>
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>20</v>
@@ -1938,7 +1938,9 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="H18" s="8" t="n">
+        <v>7</v>
+      </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -2171,7 +2173,7 @@
       </c>
       <c r="H24" s="9" t="n">
         <f aca="false">SUM(H17:H23)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I24" s="9" t="n">
         <f aca="false">SUM(I17:I23)</f>
@@ -2450,7 +2452,7 @@
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
       <c r="V31" s="8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W31" s="8"/>
       <c r="X31" s="8"/>
@@ -2708,7 +2710,7 @@
       </c>
       <c r="V37" s="9" t="n">
         <f aca="false">SUM(V30:V36)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W37" s="9" t="n">
         <f aca="false">SUM(W30:W36)</f>

</xml_diff>

<commit_message>
update time juan & yo
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -1012,8 +1012,8 @@
   </sheetPr>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V34" activeCellId="0" sqref="V34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="H5" s="8" t="n">
         <f aca="false">SUM(H30:H36)</f>
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="I5" s="8" t="n">
         <f aca="false">SUM(I30:I36)</f>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="M5" s="9" t="n">
         <f aca="false">SUM(C5:L5)</f>
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>9</v>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="H9" s="8" t="n">
         <f aca="false">SUM(V30:V36)</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I9" s="8" t="n">
         <f aca="false">SUM(W30:W36)</f>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="M9" s="9" t="n">
         <f aca="false">SUM(C9:L9)</f>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O9" s="10" t="s">
         <v>17</v>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="H11" s="9" t="n">
         <f aca="false">SUM(H4:H10)</f>
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="I11" s="9" t="n">
         <f aca="false">SUM(I4:I10)</f>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="M11" s="9" t="n">
         <f aca="false">SUM(C11:L11)</f>
-        <v>330</v>
+        <v>356</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>20</v>
@@ -2474,7 +2474,9 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="H32" s="8" t="n">
+        <v>8</v>
+      </c>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -2514,7 +2516,9 @@
       <c r="G33" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="H33" s="8"/>
+      <c r="H33" s="8" t="n">
+        <v>7</v>
+      </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
@@ -2556,7 +2560,9 @@
       <c r="G34" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="H34" s="8"/>
+      <c r="H34" s="8" t="n">
+        <v>6</v>
+      </c>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -2575,7 +2581,9 @@
       <c r="U34" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="V34" s="8"/>
+      <c r="V34" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
       <c r="Y34" s="8"/>
@@ -2673,7 +2681,7 @@
       </c>
       <c r="H37" s="9" t="n">
         <f aca="false">SUM(H30:H36)</f>
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="I37" s="9" t="n">
         <f aca="false">SUM(I30:I36)</f>
@@ -2718,7 +2726,7 @@
       </c>
       <c r="V37" s="9" t="n">
         <f aca="false">SUM(V30:V36)</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="W37" s="9" t="n">
         <f aca="false">SUM(W30:W36)</f>

</xml_diff>

<commit_message>
edit timeplan for the week
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsrapport" sheetId="1" state="visible" r:id="rId2"/>
@@ -935,12 +935,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1012,8 +1012,8 @@
   </sheetPr>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC37" activeCellId="0" sqref="AC37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V44" activeCellId="0" sqref="V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1237,7 +1237,7 @@
         <v>4</v>
       </c>
       <c r="V4" s="8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
@@ -1372,7 +1372,9 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
+      <c r="V6" s="8" t="n">
+        <v>6</v>
+      </c>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
@@ -1406,7 +1408,7 @@
       </c>
       <c r="H7" s="8" t="n">
         <f aca="false">SUM(V4:V10)</f>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="I7" s="8" t="n">
         <f aca="false">SUM(W4:W10)</f>
@@ -1426,7 +1428,7 @@
       </c>
       <c r="M7" s="9" t="n">
         <f aca="false">SUM(C7:L7)</f>
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>13</v>
@@ -1441,7 +1443,9 @@
       <c r="U7" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="V7" s="8"/>
+      <c r="V7" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
@@ -1512,7 +1516,9 @@
       <c r="U8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="V8" s="8"/>
+      <c r="V8" s="8" t="n">
+        <v>6</v>
+      </c>
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
@@ -1611,7 +1617,7 @@
       </c>
       <c r="H10" s="8" t="n">
         <f aca="false">SUM(V43:V49)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="8" t="n">
         <f aca="false">SUM(W43:W49)</f>
@@ -1631,7 +1637,7 @@
       </c>
       <c r="M10" s="9" t="n">
         <f aca="false">SUM(C10:L10)</f>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O10" s="10" t="s">
         <v>19</v>
@@ -1676,7 +1682,7 @@
       </c>
       <c r="H11" s="9" t="n">
         <f aca="false">SUM(H4:H10)</f>
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="I11" s="9" t="n">
         <f aca="false">SUM(I4:I10)</f>
@@ -1696,7 +1702,7 @@
       </c>
       <c r="M11" s="9" t="n">
         <f aca="false">SUM(C11:L11)</f>
-        <v>411</v>
+        <v>430</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>20</v>
@@ -1724,7 +1730,7 @@
       </c>
       <c r="V11" s="9" t="n">
         <f aca="false">SUM(V4:V10)</f>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="W11" s="9" t="n">
         <f aca="false">SUM(W4:W10)</f>
@@ -2936,7 +2942,7 @@
         <v>4</v>
       </c>
       <c r="V43" s="8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W43" s="8"/>
       <c r="X43" s="8"/>
@@ -3252,7 +3258,7 @@
       </c>
       <c r="V50" s="9" t="n">
         <f aca="false">SUM(V43:V49)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W50" s="9" t="n">
         <f aca="false">SUM(W43:W49)</f>
@@ -3387,17 +3393,17 @@
   </sheetPr>
   <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE46" activeCellId="0" sqref="AE46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="8" style="0" width="5.43"/>
@@ -3661,8 +3667,7 @@
         <v>77</v>
       </c>
       <c r="N8" s="34" t="n">
-        <f aca="false">SUM(N13:N23,N27:N63)</f>
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O8" s="34" t="n">
         <f aca="false">SUM(O13:O23,O27:O63)</f>
@@ -3670,7 +3675,7 @@
       </c>
       <c r="P8" s="34" t="n">
         <f aca="false">SUM(P13:P23,P27:P63)</f>
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="Q8" s="34" t="n">
         <f aca="false">SUM(Q13:Q23,Q27:Q63)</f>
@@ -3755,7 +3760,7 @@
         <v>170</v>
       </c>
       <c r="P10" s="34" t="n">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="Q10" s="34" t="n">
         <v>180</v>
@@ -3769,7 +3774,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="32" t="n">
         <f aca="false">SUM(H10:S10)</f>
-        <v>857</v>
+        <v>860</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5283,7 +5288,7 @@
       <c r="N54" s="43"/>
       <c r="O54" s="43"/>
       <c r="P54" s="43" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Q54" s="43"/>
       <c r="R54" s="43"/>
@@ -5291,7 +5296,7 @@
       <c r="T54" s="38"/>
       <c r="U54" s="32" t="n">
         <f aca="false">SUM(H54:S54)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5656,7 +5661,7 @@
       </c>
       <c r="P64" s="43" t="n">
         <f aca="false">SUM(P28:P63)</f>
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="Q64" s="43" t="n">
         <f aca="false">SUM(Q28:Q63)</f>
@@ -5673,7 +5678,7 @@
       <c r="T64" s="38"/>
       <c r="U64" s="32" t="n">
         <f aca="false">SUM(H64:S64)</f>
-        <v>857</v>
+        <v>860</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5708,7 +5713,7 @@
       </c>
       <c r="P65" s="46" t="n">
         <f aca="false">SUM(P13:P23,P27:P63)</f>
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="Q65" s="46" t="n">
         <f aca="false">SUM(Q13:Q23,Q27:Q63)</f>
@@ -5725,7 +5730,7 @@
       <c r="T65" s="38"/>
       <c r="U65" s="32" t="n">
         <f aca="false">SUM(H65:S65)</f>
-        <v>891</v>
+        <v>894</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
tidsrapport för mig sj och en 1timma möte för alla andra
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -1012,8 +1012,8 @@
   </sheetPr>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W31" activeCellId="0" sqref="W31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E35" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q64" activeCellId="0" sqref="Q64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="I4" s="8" t="n">
         <f aca="false">SUM(I17:I23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="8" t="n">
         <f aca="false">SUM(J17:J23)</f>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="M4" s="9" t="n">
         <f aca="false">SUM(C4:L4)</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>7</v>
@@ -1239,7 +1239,9 @@
       <c r="V4" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="W4" s="8"/>
+      <c r="W4" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
@@ -1276,7 +1278,7 @@
       </c>
       <c r="I5" s="8" t="n">
         <f aca="false">SUM(I30:I36)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="8" t="n">
         <f aca="false">SUM(J30:J36)</f>
@@ -1292,7 +1294,7 @@
       </c>
       <c r="M5" s="9" t="n">
         <f aca="false">SUM(C5:L5)</f>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O5" s="10" t="s">
         <v>9</v>
@@ -1345,7 +1347,7 @@
       </c>
       <c r="I6" s="8" t="n">
         <f aca="false">SUM(I43:I49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="8" t="n">
         <f aca="false">SUM(J43:J49)</f>
@@ -1361,7 +1363,7 @@
       </c>
       <c r="M6" s="9" t="n">
         <f aca="false">SUM(C6:L6)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>11</v>
@@ -1412,7 +1414,7 @@
       </c>
       <c r="I7" s="8" t="n">
         <f aca="false">SUM(W4:W10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="8" t="n">
         <f aca="false">SUM(X4:X10)</f>
@@ -1428,7 +1430,7 @@
       </c>
       <c r="M7" s="9" t="n">
         <f aca="false">SUM(C7:L7)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>13</v>
@@ -1483,7 +1485,7 @@
       </c>
       <c r="I8" s="8" t="n">
         <f aca="false">SUM(W17:W23)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J8" s="8" t="n">
         <f aca="false">SUM(X17:X23)</f>
@@ -1499,7 +1501,7 @@
       </c>
       <c r="M8" s="9" t="n">
         <f aca="false">SUM(C8:L8)</f>
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="O8" s="10" t="s">
         <v>15</v>
@@ -1621,7 +1623,7 @@
       </c>
       <c r="I10" s="8" t="n">
         <f aca="false">SUM(W43:W49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="8" t="n">
         <f aca="false">SUM(X43:X49)</f>
@@ -1637,7 +1639,7 @@
       </c>
       <c r="M10" s="9" t="n">
         <f aca="false">SUM(C10:L10)</f>
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O10" s="10" t="s">
         <v>19</v>
@@ -1686,7 +1688,7 @@
       </c>
       <c r="I11" s="9" t="n">
         <f aca="false">SUM(I4:I10)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J11" s="9" t="n">
         <f aca="false">SUM(J4:J10)</f>
@@ -1702,7 +1704,7 @@
       </c>
       <c r="M11" s="9" t="n">
         <f aca="false">SUM(C11:L11)</f>
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>20</v>
@@ -1734,7 +1736,7 @@
       </c>
       <c r="W11" s="9" t="n">
         <f aca="false">SUM(W4:W10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11" s="9" t="n">
         <f aca="false">SUM(X4:X10)</f>
@@ -1903,7 +1905,9 @@
       <c r="H17" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I17" s="8"/>
+      <c r="I17" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
@@ -1926,7 +1930,9 @@
       <c r="V17" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="W17" s="8"/>
+      <c r="W17" s="8" t="n">
+        <v>7</v>
+      </c>
       <c r="X17" s="8"/>
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
@@ -2201,7 +2207,7 @@
       </c>
       <c r="I24" s="9" t="n">
         <f aca="false">SUM(I17:I23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="9" t="n">
         <f aca="false">SUM(J17:J23)</f>
@@ -2246,7 +2252,7 @@
       </c>
       <c r="W24" s="9" t="n">
         <f aca="false">SUM(W17:W23)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="X24" s="9" t="n">
         <f aca="false">SUM(X17:X23)</f>
@@ -2417,7 +2423,9 @@
       <c r="H30" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I30" s="8"/>
+      <c r="I30" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
@@ -2707,7 +2715,7 @@
       </c>
       <c r="I37" s="9" t="n">
         <f aca="false">SUM(I30:I36)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="9" t="n">
         <f aca="false">SUM(J30:J36)</f>
@@ -2923,7 +2931,9 @@
       <c r="H43" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="I43" s="8"/>
+      <c r="I43" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
@@ -2946,7 +2956,9 @@
       <c r="V43" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="W43" s="8"/>
+      <c r="W43" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="X43" s="8"/>
       <c r="Y43" s="8"/>
       <c r="Z43" s="8"/>
@@ -3219,7 +3231,7 @@
       </c>
       <c r="I50" s="9" t="n">
         <f aca="false">SUM(I43:I49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" s="9" t="n">
         <f aca="false">SUM(J43:J49)</f>
@@ -3264,7 +3276,7 @@
       </c>
       <c r="W50" s="9" t="n">
         <f aca="false">SUM(W43:W49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X50" s="9" t="n">
         <f aca="false">SUM(X43:X49)</f>

</xml_diff>

<commit_message>
GUI select nodes for create edge
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\tsea29-taxi\doc\tidsrapport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\kurser\tsea29\tsea29-taxi\doc\tidsrapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -799,6 +799,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -808,11 +814,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -849,34 +877,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:AMK50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+      <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1249,78 +1249,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="O1" s="33" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="O1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
       <c r="M2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33" t="s">
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
       <c r="AA2" s="3"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="2">
         <v>41</v>
       </c>
@@ -1354,8 +1354,8 @@
       <c r="M3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
       <c r="Q3" s="2">
         <v>41</v>
       </c>
@@ -1386,13 +1386,13 @@
       <c r="Z3" s="4">
         <v>50</v>
       </c>
-      <c r="AA3" s="34"/>
+      <c r="AA3" s="36"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="6">
         <f t="shared" ref="C4:L4" si="0">SUM(C17:C23)</f>
         <v>15</v>
@@ -1437,10 +1437,10 @@
         <f t="shared" ref="M4:M11" si="1">SUM(C4:L4)</f>
         <v>95</v>
       </c>
-      <c r="O4" s="36" t="s">
+      <c r="O4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="36"/>
+      <c r="P4" s="34"/>
       <c r="Q4" s="6">
         <v>4</v>
       </c>
@@ -1461,13 +1461,13 @@
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-      <c r="AA4" s="34"/>
+      <c r="AA4" s="36"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="6">
         <f t="shared" ref="C5:L5" si="2">SUM(C30:C36)</f>
         <v>12</v>
@@ -1512,10 +1512,10 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="36"/>
+      <c r="P5" s="34"/>
       <c r="Q5" s="6">
         <v>4</v>
       </c>
@@ -1532,13 +1532,13 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-      <c r="AA5" s="34"/>
+      <c r="AA5" s="36"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="6">
         <f t="shared" ref="C6:L6" si="3">SUM(C43:C49)</f>
         <v>11</v>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="J6" s="6">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" si="3"/>
@@ -1581,12 +1581,12 @@
       </c>
       <c r="M6" s="7">
         <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="O6" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="36"/>
+      <c r="P6" s="34"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
@@ -1601,13 +1601,13 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="34"/>
+      <c r="AA6" s="36"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="35"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="6">
         <f t="shared" ref="C7:L7" si="4">SUM(Q4:Q10)</f>
         <v>17</v>
@@ -1652,10 +1652,10 @@
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="O7" s="36" t="s">
+      <c r="O7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="36"/>
+      <c r="P7" s="34"/>
       <c r="Q7" s="6">
         <v>5</v>
       </c>
@@ -1674,13 +1674,13 @@
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-      <c r="AA7" s="34"/>
+      <c r="AA7" s="36"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="35"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="6">
         <f t="shared" ref="C8:L8" si="5">SUM(Q17:Q23)</f>
         <v>11</v>
@@ -1725,10 +1725,10 @@
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="O8" s="36" t="s">
+      <c r="O8" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="36"/>
+      <c r="P8" s="34"/>
       <c r="Q8" s="6">
         <v>4</v>
       </c>
@@ -1749,13 +1749,13 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-      <c r="AA8" s="34"/>
+      <c r="AA8" s="36"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="6">
         <f t="shared" ref="C9:L9" si="6">SUM(Q30:Q36)</f>
         <v>14</v>
@@ -1800,10 +1800,10 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="O9" s="36" t="s">
+      <c r="O9" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="36"/>
+      <c r="P9" s="34"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
@@ -1814,13 +1814,13 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-      <c r="AA9" s="34"/>
+      <c r="AA9" s="36"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="6">
         <f t="shared" ref="C10:L10" si="7">SUM(Q43:Q49)</f>
         <v>16</v>
@@ -1865,10 +1865,10 @@
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="O10" s="36" t="s">
+      <c r="O10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="36"/>
+      <c r="P10" s="34"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
@@ -1879,13 +1879,13 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
-      <c r="AA10" s="34"/>
+      <c r="AA10" s="36"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="37"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="7">
         <f t="shared" ref="C11:L11" si="8">SUM(C4:C10)</f>
         <v>96</v>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="J11" s="7">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="8"/>
@@ -1928,12 +1928,12 @@
       </c>
       <c r="M11" s="7">
         <f t="shared" si="1"/>
-        <v>639</v>
-      </c>
-      <c r="O11" s="37" t="s">
+        <v>643</v>
+      </c>
+      <c r="O11" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="37"/>
+      <c r="P11" s="33"/>
       <c r="Q11" s="7">
         <f t="shared" ref="Q11:Z11" si="9">SUM(Q4:Q10)</f>
         <v>17</v>
@@ -1974,7 +1974,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA11" s="34"/>
+      <c r="AA11" s="36"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12"/>
@@ -2033,76 +2033,76 @@
       <c r="AA13"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="O14" s="33" t="s">
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="O14" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="33"/>
-      <c r="U14" s="33"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="33"/>
-      <c r="Y14" s="33"/>
-      <c r="Z14" s="33"/>
-      <c r="AA14" s="33"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
+      <c r="X14" s="35"/>
+      <c r="Y14" s="35"/>
+      <c r="Z14" s="35"/>
+      <c r="AA14" s="35"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33" t="s">
+      <c r="B15" s="35"/>
+      <c r="C15" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
       <c r="M15" s="3"/>
-      <c r="O15" s="33" t="s">
+      <c r="O15" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33" t="s">
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="R15" s="33"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
-      <c r="X15" s="33"/>
-      <c r="Y15" s="33"/>
-      <c r="Z15" s="33"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="35"/>
+      <c r="Z15" s="35"/>
       <c r="AA15" s="3"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="2">
         <v>41</v>
       </c>
@@ -2133,9 +2133,9 @@
       <c r="L16" s="4">
         <v>50</v>
       </c>
-      <c r="M16" s="34"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
+      <c r="M16" s="36"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
       <c r="Q16" s="2">
         <v>41</v>
       </c>
@@ -2166,13 +2166,13 @@
       <c r="Z16" s="4">
         <v>50</v>
       </c>
-      <c r="AA16" s="34"/>
+      <c r="AA16" s="36"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="6">
         <v>3</v>
       </c>
@@ -2191,11 +2191,11 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="34"/>
-      <c r="O17" s="36" t="s">
+      <c r="M17" s="36"/>
+      <c r="O17" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="P17" s="36"/>
+      <c r="P17" s="34"/>
       <c r="Q17" s="6">
         <v>2</v>
       </c>
@@ -2218,13 +2218,13 @@
       </c>
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
-      <c r="AA17" s="34"/>
+      <c r="AA17" s="36"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="36"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="6">
         <v>4</v>
       </c>
@@ -2243,11 +2243,11 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="34"/>
-      <c r="O18" s="36" t="s">
+      <c r="M18" s="36"/>
+      <c r="O18" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="P18" s="36"/>
+      <c r="P18" s="34"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -2266,13 +2266,13 @@
       </c>
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
-      <c r="AA18" s="34"/>
+      <c r="AA18" s="36"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -2287,11 +2287,11 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
-      <c r="M19" s="34"/>
-      <c r="O19" s="36" t="s">
+      <c r="M19" s="36"/>
+      <c r="O19" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="P19" s="36"/>
+      <c r="P19" s="34"/>
       <c r="Q19" s="6">
         <v>1</v>
       </c>
@@ -2308,13 +2308,13 @@
       <c r="X19" s="6"/>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
-      <c r="AA19" s="34"/>
+      <c r="AA19" s="36"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="36"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="6">
         <v>4</v>
       </c>
@@ -2333,11 +2333,11 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
-      <c r="M20" s="34"/>
-      <c r="O20" s="36" t="s">
+      <c r="M20" s="36"/>
+      <c r="O20" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="P20" s="36"/>
+      <c r="P20" s="34"/>
       <c r="Q20" s="6">
         <v>4</v>
       </c>
@@ -2358,13 +2358,13 @@
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
-      <c r="AA20" s="34"/>
+      <c r="AA20" s="36"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="36"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="6">
         <v>4</v>
       </c>
@@ -2383,11 +2383,11 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
-      <c r="M21" s="34"/>
-      <c r="O21" s="36" t="s">
+      <c r="M21" s="36"/>
+      <c r="O21" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="P21" s="36"/>
+      <c r="P21" s="34"/>
       <c r="Q21" s="6">
         <v>4</v>
       </c>
@@ -2404,13 +2404,13 @@
       <c r="X21" s="6"/>
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
-      <c r="AA21" s="34"/>
+      <c r="AA21" s="36"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="36"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -2421,11 +2421,11 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="34"/>
-      <c r="O22" s="36" t="s">
+      <c r="M22" s="36"/>
+      <c r="O22" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P22" s="36"/>
+      <c r="P22" s="34"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -2438,13 +2438,13 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
-      <c r="AA22" s="34"/>
+      <c r="AA22" s="36"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="36"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -2455,11 +2455,11 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="34"/>
-      <c r="O23" s="36" t="s">
+      <c r="M23" s="36"/>
+      <c r="O23" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P23" s="36"/>
+      <c r="P23" s="34"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
@@ -2472,13 +2472,13 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
-      <c r="AA23" s="34"/>
+      <c r="AA23" s="36"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="37"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="7">
         <f t="shared" ref="C24:L24" si="10">SUM(C17:C23)</f>
         <v>15</v>
@@ -2519,11 +2519,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M24" s="34"/>
-      <c r="O24" s="37" t="s">
+      <c r="M24" s="36"/>
+      <c r="O24" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="P24" s="37"/>
+      <c r="P24" s="33"/>
       <c r="Q24" s="7">
         <f t="shared" ref="Q24:Z24" si="11">SUM(Q17:Q23)</f>
         <v>11</v>
@@ -2564,7 +2564,7 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AA24" s="34"/>
+      <c r="AA24" s="36"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25"/>
@@ -2623,76 +2623,76 @@
       <c r="AA26"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="O27" s="33" t="s">
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="O27" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="33"/>
-      <c r="X27" s="33"/>
-      <c r="Y27" s="33"/>
-      <c r="Z27" s="33"/>
-      <c r="AA27" s="33"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="35"/>
+      <c r="X27" s="35"/>
+      <c r="Y27" s="35"/>
+      <c r="Z27" s="35"/>
+      <c r="AA27" s="35"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33" t="s">
+      <c r="B28" s="35"/>
+      <c r="C28" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
       <c r="M28" s="3"/>
-      <c r="O28" s="33" t="s">
+      <c r="O28" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33" t="s">
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="R28" s="33"/>
-      <c r="S28" s="33"/>
-      <c r="T28" s="33"/>
-      <c r="U28" s="33"/>
-      <c r="V28" s="33"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="33"/>
-      <c r="Y28" s="33"/>
-      <c r="Z28" s="33"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
+      <c r="X28" s="35"/>
+      <c r="Y28" s="35"/>
+      <c r="Z28" s="35"/>
       <c r="AA28" s="3"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="2">
         <v>41</v>
       </c>
@@ -2723,9 +2723,9 @@
       <c r="L29" s="4">
         <v>50</v>
       </c>
-      <c r="M29" s="34"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
+      <c r="M29" s="36"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="35"/>
       <c r="Q29" s="2">
         <v>41</v>
       </c>
@@ -2756,13 +2756,13 @@
       <c r="Z29" s="4">
         <v>50</v>
       </c>
-      <c r="AA29" s="34"/>
+      <c r="AA29" s="36"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="36"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="6">
         <v>4</v>
       </c>
@@ -2783,11 +2783,11 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
-      <c r="M30" s="34"/>
-      <c r="O30" s="36" t="s">
+      <c r="M30" s="36"/>
+      <c r="O30" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="P30" s="36"/>
+      <c r="P30" s="34"/>
       <c r="Q30" s="6">
         <v>2</v>
       </c>
@@ -2808,13 +2808,13 @@
       <c r="X30" s="6"/>
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
-      <c r="AA30" s="34"/>
+      <c r="AA30" s="36"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="36"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="6">
         <v>4</v>
       </c>
@@ -2829,11 +2829,11 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
-      <c r="M31" s="34"/>
-      <c r="O31" s="36" t="s">
+      <c r="M31" s="36"/>
+      <c r="O31" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="P31" s="36"/>
+      <c r="P31" s="34"/>
       <c r="Q31" s="6">
         <v>3</v>
       </c>
@@ -2850,13 +2850,13 @@
       <c r="X31" s="6"/>
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
-      <c r="AA31" s="34"/>
+      <c r="AA31" s="36"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="36"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -2871,11 +2871,11 @@
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
-      <c r="M32" s="34"/>
-      <c r="O32" s="36" t="s">
+      <c r="M32" s="36"/>
+      <c r="O32" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="P32" s="36"/>
+      <c r="P32" s="34"/>
       <c r="Q32" s="6">
         <v>1</v>
       </c>
@@ -2892,13 +2892,13 @@
       <c r="X32" s="6"/>
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
-      <c r="AA32" s="34"/>
+      <c r="AA32" s="36"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="36"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="6">
         <v>4</v>
       </c>
@@ -2917,11 +2917,11 @@
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
-      <c r="M33" s="34"/>
-      <c r="O33" s="36" t="s">
+      <c r="M33" s="36"/>
+      <c r="O33" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="P33" s="36"/>
+      <c r="P33" s="34"/>
       <c r="Q33" s="6">
         <v>4</v>
       </c>
@@ -2942,13 +2942,13 @@
       <c r="X33" s="6"/>
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
-      <c r="AA33" s="34"/>
+      <c r="AA33" s="36"/>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="36"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -2965,11 +2965,11 @@
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
-      <c r="M34" s="34"/>
-      <c r="O34" s="36" t="s">
+      <c r="M34" s="36"/>
+      <c r="O34" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="P34" s="36"/>
+      <c r="P34" s="34"/>
       <c r="Q34" s="6">
         <v>4</v>
       </c>
@@ -2986,13 +2986,13 @@
       <c r="X34" s="6"/>
       <c r="Y34" s="6"/>
       <c r="Z34" s="6"/>
-      <c r="AA34" s="34"/>
+      <c r="AA34" s="36"/>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="36"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -3003,11 +3003,11 @@
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
-      <c r="M35" s="34"/>
-      <c r="O35" s="36" t="s">
+      <c r="M35" s="36"/>
+      <c r="O35" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P35" s="36"/>
+      <c r="P35" s="34"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
       <c r="S35" s="6"/>
@@ -3018,13 +3018,13 @@
       <c r="X35" s="6"/>
       <c r="Y35" s="6"/>
       <c r="Z35" s="6"/>
-      <c r="AA35" s="34"/>
+      <c r="AA35" s="36"/>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="36"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -3035,11 +3035,11 @@
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
-      <c r="M36" s="34"/>
-      <c r="O36" s="36" t="s">
+      <c r="M36" s="36"/>
+      <c r="O36" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P36" s="36"/>
+      <c r="P36" s="34"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
@@ -3050,13 +3050,13 @@
       <c r="X36" s="6"/>
       <c r="Y36" s="6"/>
       <c r="Z36" s="6"/>
-      <c r="AA36" s="34"/>
+      <c r="AA36" s="36"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="37"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="7">
         <f t="shared" ref="C37:L37" si="12">SUM(C30:C36)</f>
         <v>12</v>
@@ -3097,11 +3097,11 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M37" s="34"/>
-      <c r="O37" s="37" t="s">
+      <c r="M37" s="36"/>
+      <c r="O37" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="P37" s="37"/>
+      <c r="P37" s="33"/>
       <c r="Q37" s="7">
         <f t="shared" ref="Q37:Z37" si="13">SUM(Q30:Q36)</f>
         <v>14</v>
@@ -3142,7 +3142,7 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AA37" s="34"/>
+      <c r="AA37" s="36"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38"/>
@@ -3201,76 +3201,76 @@
       <c r="AA39"/>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="O40" s="33" t="s">
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="O40" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
-      <c r="R40" s="33"/>
-      <c r="S40" s="33"/>
-      <c r="T40" s="33"/>
-      <c r="U40" s="33"/>
-      <c r="V40" s="33"/>
-      <c r="W40" s="33"/>
-      <c r="X40" s="33"/>
-      <c r="Y40" s="33"/>
-      <c r="Z40" s="33"/>
-      <c r="AA40" s="33"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="35"/>
+      <c r="V40" s="35"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
+      <c r="AA40" s="35"/>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33" t="s">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35"/>
       <c r="M41" s="3"/>
-      <c r="O41" s="33" t="s">
+      <c r="O41" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33" t="s">
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="R41" s="33"/>
-      <c r="S41" s="33"/>
-      <c r="T41" s="33"/>
-      <c r="U41" s="33"/>
-      <c r="V41" s="33"/>
-      <c r="W41" s="33"/>
-      <c r="X41" s="33"/>
-      <c r="Y41" s="33"/>
-      <c r="Z41" s="33"/>
+      <c r="R41" s="35"/>
+      <c r="S41" s="35"/>
+      <c r="T41" s="35"/>
+      <c r="U41" s="35"/>
+      <c r="V41" s="35"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="35"/>
+      <c r="Z41" s="35"/>
       <c r="AA41" s="3"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="2">
         <v>41</v>
       </c>
@@ -3301,9 +3301,9 @@
       <c r="L42" s="4">
         <v>50</v>
       </c>
-      <c r="M42" s="34"/>
-      <c r="O42" s="33"/>
-      <c r="P42" s="33"/>
+      <c r="M42" s="36"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
       <c r="Q42" s="2">
         <v>41</v>
       </c>
@@ -3334,13 +3334,13 @@
       <c r="Z42" s="4">
         <v>50</v>
       </c>
-      <c r="AA42" s="34"/>
+      <c r="AA42" s="36"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="36"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="6">
         <v>3</v>
       </c>
@@ -3363,11 +3363,11 @@
       </c>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
-      <c r="M43" s="34"/>
-      <c r="O43" s="36" t="s">
+      <c r="M43" s="36"/>
+      <c r="O43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="P43" s="36"/>
+      <c r="P43" s="34"/>
       <c r="Q43" s="6">
         <v>3</v>
       </c>
@@ -3388,13 +3388,13 @@
       <c r="X43" s="6"/>
       <c r="Y43" s="6"/>
       <c r="Z43" s="6"/>
-      <c r="AA43" s="34"/>
+      <c r="AA43" s="36"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="36"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6">
         <v>4</v>
       </c>
@@ -3415,11 +3415,11 @@
       </c>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
-      <c r="M44" s="34"/>
-      <c r="O44" s="36" t="s">
+      <c r="M44" s="36"/>
+      <c r="O44" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="P44" s="36"/>
+      <c r="P44" s="34"/>
       <c r="Q44" s="6">
         <v>4</v>
       </c>
@@ -3438,13 +3438,13 @@
       <c r="X44" s="6"/>
       <c r="Y44" s="6"/>
       <c r="Z44" s="6"/>
-      <c r="AA44" s="34"/>
+      <c r="AA44" s="36"/>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -3456,14 +3456,16 @@
       <c r="I45" s="6">
         <v>3</v>
       </c>
-      <c r="J45" s="6"/>
+      <c r="J45" s="6">
+        <v>4</v>
+      </c>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
-      <c r="M45" s="34"/>
-      <c r="O45" s="36" t="s">
+      <c r="M45" s="36"/>
+      <c r="O45" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="P45" s="36"/>
+      <c r="P45" s="34"/>
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
       <c r="S45" s="6"/>
@@ -3478,13 +3480,13 @@
       <c r="X45" s="6"/>
       <c r="Y45" s="6"/>
       <c r="Z45" s="6"/>
-      <c r="AA45" s="34"/>
+      <c r="AA45" s="36"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="36"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="6">
         <v>4</v>
       </c>
@@ -3501,11 +3503,11 @@
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
-      <c r="M46" s="34"/>
-      <c r="O46" s="36" t="s">
+      <c r="M46" s="36"/>
+      <c r="O46" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="P46" s="36"/>
+      <c r="P46" s="34"/>
       <c r="Q46" s="6">
         <v>4</v>
       </c>
@@ -3526,13 +3528,13 @@
       <c r="X46" s="6"/>
       <c r="Y46" s="6"/>
       <c r="Z46" s="6"/>
-      <c r="AA46" s="34"/>
+      <c r="AA46" s="36"/>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="36"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -3551,11 +3553,11 @@
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
-      <c r="M47" s="34"/>
-      <c r="O47" s="36" t="s">
+      <c r="M47" s="36"/>
+      <c r="O47" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="P47" s="36"/>
+      <c r="P47" s="34"/>
       <c r="Q47" s="6">
         <v>5</v>
       </c>
@@ -3576,13 +3578,13 @@
       <c r="X47" s="6"/>
       <c r="Y47" s="6"/>
       <c r="Z47" s="6"/>
-      <c r="AA47" s="34"/>
+      <c r="AA47" s="36"/>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="36"/>
+      <c r="B48" s="34"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -3593,11 +3595,11 @@
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
-      <c r="M48" s="34"/>
-      <c r="O48" s="36" t="s">
+      <c r="M48" s="36"/>
+      <c r="O48" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P48" s="36"/>
+      <c r="P48" s="34"/>
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
       <c r="S48" s="6"/>
@@ -3608,13 +3610,13 @@
       <c r="X48" s="6"/>
       <c r="Y48" s="6"/>
       <c r="Z48" s="6"/>
-      <c r="AA48" s="34"/>
+      <c r="AA48" s="36"/>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="36"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -3625,11 +3627,11 @@
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
-      <c r="M49" s="34"/>
-      <c r="O49" s="36" t="s">
+      <c r="M49" s="36"/>
+      <c r="O49" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="P49" s="36"/>
+      <c r="P49" s="34"/>
       <c r="Q49" s="6"/>
       <c r="R49" s="6"/>
       <c r="S49" s="6"/>
@@ -3642,13 +3644,13 @@
       <c r="X49" s="6"/>
       <c r="Y49" s="6"/>
       <c r="Z49" s="6"/>
-      <c r="AA49" s="34"/>
+      <c r="AA49" s="36"/>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="37"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="7">
         <f t="shared" ref="C50:L50" si="14">SUM(C43:C49)</f>
         <v>11</v>
@@ -3679,7 +3681,7 @@
       </c>
       <c r="J50" s="7">
         <f t="shared" si="14"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K50" s="7">
         <f t="shared" si="14"/>
@@ -3689,11 +3691,11 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M50" s="34"/>
-      <c r="O50" s="37" t="s">
+      <c r="M50" s="36"/>
+      <c r="O50" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="P50" s="37"/>
+      <c r="P50" s="33"/>
       <c r="Q50" s="7">
         <f t="shared" ref="Q50:Z50" si="15">SUM(Q43:Q49)</f>
         <v>16</v>
@@ -3734,18 +3736,81 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AA50" s="34"/>
+      <c r="AA50" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="O50:P50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="O48:P48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="O49:P49"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="O1:AA1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="O2:P3"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA3:AA11"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="O14:AA14"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="Q15:Z15"/>
+    <mergeCell ref="M16:M24"/>
+    <mergeCell ref="AA16:AA24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="O27:AA27"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="C28:L28"/>
+    <mergeCell ref="O28:P29"/>
+    <mergeCell ref="Q28:Z28"/>
+    <mergeCell ref="M29:M37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="AA29:AA37"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A40:M40"/>
     <mergeCell ref="O40:AA40"/>
     <mergeCell ref="A41:B42"/>
@@ -3762,77 +3827,14 @@
     <mergeCell ref="O45:P45"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="O46:P46"/>
-    <mergeCell ref="AA29:AA37"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="C28:L28"/>
-    <mergeCell ref="O28:P29"/>
-    <mergeCell ref="Q28:Z28"/>
-    <mergeCell ref="M29:M37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="A27:M27"/>
-    <mergeCell ref="O27:AA27"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="O14:AA14"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="Q15:Z15"/>
-    <mergeCell ref="M16:M24"/>
-    <mergeCell ref="AA16:AA24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="O1:AA1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="O2:P3"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA3:AA11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="O50:P50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="O49:P49"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -3866,183 +3868,183 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="49"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="42">
+      <c r="D3" s="52">
         <v>2</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43" t="s">
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="44" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45" t="s">
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="46" t="s">
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="47" t="s">
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
     </row>
     <row r="6" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="12" t="s">
         <v>38</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="14" t="s">
         <v>43</v>
       </c>
@@ -4092,12 +4094,12 @@
     </row>
     <row r="8" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="15"/>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
       <c r="F8" s="18">
         <v>1120</v>
       </c>
@@ -4148,12 +4150,12 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="18">
         <v>220</v>
       </c>
@@ -4186,12 +4188,12 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="18">
         <v>900</v>
       </c>
@@ -4229,46 +4231,46 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="12" t="s">
         <v>38</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="49" t="s">
+      <c r="H11" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="49"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
-      <c r="U11" s="49"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="40"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="14" t="s">
         <v>43</v>
       </c>
@@ -4318,12 +4320,12 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="25"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -4345,12 +4347,12 @@
       <c r="A14" s="15">
         <v>1</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
       <c r="F14" s="18">
         <v>20</v>
       </c>
@@ -4383,12 +4385,12 @@
       <c r="A15" s="15">
         <v>2</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
       <c r="F15" s="18">
         <v>40</v>
       </c>
@@ -4421,12 +4423,12 @@
       <c r="A16" s="15">
         <v>3</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
       <c r="F16" s="18">
         <v>40</v>
       </c>
@@ -4455,12 +4457,12 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="25"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -4482,12 +4484,12 @@
       <c r="A18" s="15">
         <v>4</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
       <c r="F18" s="18">
         <v>40</v>
       </c>
@@ -4520,12 +4522,12 @@
       <c r="A19" s="15">
         <v>5</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="18">
         <v>20</v>
       </c>
@@ -4556,12 +4558,12 @@
       <c r="A20" s="15">
         <v>6</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
       <c r="F20" s="18">
         <v>20</v>
       </c>
@@ -4590,12 +4592,12 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
@@ -4617,12 +4619,12 @@
       <c r="A22" s="15">
         <v>7</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
       <c r="F22" s="18">
         <v>21</v>
       </c>
@@ -4655,12 +4657,12 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
       <c r="F23" s="18">
         <f>(220-SUM(F14:F22))</f>
         <v>19</v>
@@ -4695,12 +4697,12 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
       <c r="F24" s="18">
         <f>SUM(F14:F23)</f>
         <v>220</v>
@@ -4734,46 +4736,46 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="12" t="s">
         <v>38</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H25" s="49" t="s">
+      <c r="H25" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="49"/>
-      <c r="R25" s="49"/>
-      <c r="S25" s="49"/>
-      <c r="T25" s="49"/>
-      <c r="U25" s="49"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="40"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="14" t="s">
         <v>43</v>
       </c>
@@ -4823,12 +4825,12 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="25"/>
       <c r="G27" s="25"/>
       <c r="H27" s="22"/>
@@ -4850,12 +4852,12 @@
       <c r="A28" s="15">
         <v>8</v>
       </c>
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="18">
         <v>55</v>
       </c>
@@ -4888,12 +4890,12 @@
       <c r="A29" s="15">
         <v>9</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="18">
         <v>60</v>
       </c>
@@ -4924,12 +4926,12 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
       <c r="H30" s="22"/>
@@ -4951,12 +4953,12 @@
       <c r="A31" s="15">
         <v>10</v>
       </c>
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
       <c r="F31" s="26">
         <v>40</v>
       </c>
@@ -4987,12 +4989,12 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
       <c r="H32" s="22"/>
@@ -5014,12 +5016,12 @@
       <c r="A33" s="15">
         <v>11</v>
       </c>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
       <c r="F33" s="26">
         <v>25</v>
       </c>
@@ -5050,12 +5052,12 @@
       <c r="A34" s="15">
         <v>12</v>
       </c>
-      <c r="B34" s="53" t="s">
+      <c r="B34" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
       <c r="F34" s="26">
         <v>25</v>
       </c>
@@ -5086,12 +5088,12 @@
       <c r="A35" s="15">
         <v>13</v>
       </c>
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="26">
         <v>20</v>
       </c>
@@ -5122,12 +5124,12 @@
       <c r="A36" s="15">
         <v>14</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
       <c r="F36" s="26">
         <v>20</v>
       </c>
@@ -5156,12 +5158,12 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="15"/>
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
       <c r="H37" s="22"/>
@@ -5183,12 +5185,12 @@
       <c r="A38" s="15">
         <v>15</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="26">
         <v>30</v>
       </c>
@@ -5219,12 +5221,12 @@
       <c r="A39" s="15">
         <v>16</v>
       </c>
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
       <c r="F39" s="26">
         <v>20</v>
       </c>
@@ -5255,12 +5257,12 @@
       <c r="A40" s="15">
         <v>17</v>
       </c>
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
       <c r="F40" s="26">
         <v>70</v>
       </c>
@@ -5293,12 +5295,12 @@
       <c r="A41" s="15">
         <v>18</v>
       </c>
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
       <c r="F41" s="26">
         <v>40</v>
       </c>
@@ -5329,12 +5331,12 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="15"/>
-      <c r="B42" s="52" t="s">
+      <c r="B42" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
       <c r="H42" s="22"/>
@@ -5356,12 +5358,12 @@
       <c r="A43" s="15">
         <v>19</v>
       </c>
-      <c r="B43" s="53" t="s">
+      <c r="B43" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
       <c r="F43" s="26">
         <v>40</v>
       </c>
@@ -5390,12 +5392,12 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="15"/>
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
       <c r="H44" s="22"/>
@@ -5417,12 +5419,12 @@
       <c r="A45" s="15">
         <v>20</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
       <c r="F45" s="26">
         <v>40</v>
       </c>
@@ -5455,12 +5457,12 @@
       <c r="A46" s="15">
         <v>21</v>
       </c>
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
       <c r="F46" s="26">
         <v>20</v>
       </c>
@@ -5491,12 +5493,12 @@
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="15"/>
-      <c r="B47" s="52" t="s">
+      <c r="B47" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
       <c r="H47" s="22"/>
@@ -5518,12 +5520,12 @@
       <c r="A48" s="15">
         <v>22</v>
       </c>
-      <c r="B48" s="53" t="s">
+      <c r="B48" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
       <c r="F48" s="26">
         <v>15</v>
       </c>
@@ -5552,12 +5554,12 @@
       <c r="A49" s="15">
         <v>23</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
       <c r="F49" s="26">
         <v>30</v>
       </c>
@@ -5588,12 +5590,12 @@
       <c r="A50" s="15">
         <v>24</v>
       </c>
-      <c r="B50" s="53" t="s">
+      <c r="B50" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
       <c r="F50" s="26">
         <v>30</v>
       </c>
@@ -5624,12 +5626,12 @@
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="15"/>
-      <c r="B51" s="52" t="s">
+      <c r="B51" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="52"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="52"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
       <c r="H51" s="22"/>
@@ -5651,12 +5653,12 @@
       <c r="A52" s="15">
         <v>25</v>
       </c>
-      <c r="B52" s="53" t="s">
+      <c r="B52" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
       <c r="F52" s="26">
         <v>20</v>
       </c>
@@ -5685,12 +5687,12 @@
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="15"/>
-      <c r="B53" s="52" t="s">
+      <c r="B53" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="52"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="22"/>
@@ -5712,12 +5714,12 @@
       <c r="A54" s="15">
         <v>26</v>
       </c>
-      <c r="B54" s="53" t="s">
+      <c r="B54" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="26">
         <v>10</v>
       </c>
@@ -5748,12 +5750,12 @@
       <c r="A55" s="15">
         <v>27</v>
       </c>
-      <c r="B55" s="53" t="s">
+      <c r="B55" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
       <c r="F55" s="26">
         <v>30</v>
       </c>
@@ -5782,12 +5784,12 @@
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
-      <c r="B56" s="52" t="s">
+      <c r="B56" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52"/>
-      <c r="E56" s="52"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="22"/>
@@ -5809,12 +5811,12 @@
       <c r="A57" s="15">
         <v>28</v>
       </c>
-      <c r="B57" s="53" t="s">
+      <c r="B57" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
       <c r="F57" s="26">
         <v>70</v>
       </c>
@@ -5845,12 +5847,12 @@
       <c r="A58" s="15">
         <v>29</v>
       </c>
-      <c r="B58" s="53" t="s">
+      <c r="B58" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="53"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
       <c r="F58" s="26">
         <v>20</v>
       </c>
@@ -5881,12 +5883,12 @@
       <c r="A59" s="15">
         <v>30</v>
       </c>
-      <c r="B59" s="53" t="s">
+      <c r="B59" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
       <c r="F59" s="26">
         <v>20</v>
       </c>
@@ -5919,12 +5921,12 @@
       <c r="A60" s="15">
         <v>33</v>
       </c>
-      <c r="B60" s="53" t="s">
+      <c r="B60" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C60" s="53"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="53"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
       <c r="F60" s="26">
         <v>20</v>
       </c>
@@ -5961,12 +5963,12 @@
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="15"/>
-      <c r="B61" s="52" t="s">
+      <c r="B61" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="52"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
       <c r="F61" s="25"/>
       <c r="G61" s="25"/>
       <c r="H61" s="22"/>
@@ -5988,12 +5990,12 @@
       <c r="A62" s="15">
         <v>32</v>
       </c>
-      <c r="B62" s="53" t="s">
+      <c r="B62" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="53"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="53"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
       <c r="F62" s="26">
         <v>35</v>
       </c>
@@ -6030,12 +6032,12 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="15"/>
-      <c r="B63" s="54" t="s">
+      <c r="B63" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="54"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
       <c r="F63" s="26">
         <f>(900-SUM(F28:F62))</f>
         <v>95</v>
@@ -6079,12 +6081,12 @@
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="15"/>
-      <c r="B64" s="53" t="s">
+      <c r="B64" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C64" s="53"/>
-      <c r="D64" s="53"/>
-      <c r="E64" s="53"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
       <c r="F64" s="26">
         <f>SUM(F28:F63)</f>
         <v>900</v>
@@ -6128,12 +6130,12 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="15"/>
-      <c r="B65" s="55" t="s">
+      <c r="B65" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="55"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
       <c r="F65" s="27">
         <f>SUM(F24,F64)</f>
         <v>1120</v>
@@ -6179,44 +6181,44 @@
       </c>
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B66" s="49"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="49" t="s">
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="I66" s="49"/>
-      <c r="J66" s="49"/>
-      <c r="K66" s="49"/>
-      <c r="L66" s="49"/>
-      <c r="M66" s="49"/>
-      <c r="N66" s="49"/>
-      <c r="O66" s="49"/>
-      <c r="P66" s="49"/>
-      <c r="Q66" s="49"/>
-      <c r="R66" s="49"/>
-      <c r="S66" s="49"/>
-      <c r="T66" s="49"/>
-      <c r="U66" s="49"/>
+      <c r="I66" s="40"/>
+      <c r="J66" s="40"/>
+      <c r="K66" s="40"/>
+      <c r="L66" s="40"/>
+      <c r="M66" s="40"/>
+      <c r="N66" s="40"/>
+      <c r="O66" s="40"/>
+      <c r="P66" s="40"/>
+      <c r="Q66" s="40"/>
+      <c r="R66" s="40"/>
+      <c r="S66" s="40"/>
+      <c r="T66" s="40"/>
+      <c r="U66" s="40"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B67" s="56" t="s">
+      <c r="B67" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="56"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="41"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="15">
         <v>40</v>
       </c>
@@ -6262,14 +6264,14 @@
       <c r="A68" s="15">
         <v>1</v>
       </c>
-      <c r="B68" s="57" t="s">
+      <c r="B68" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="57"/>
-      <c r="D68" s="57"/>
-      <c r="E68" s="57"/>
-      <c r="F68" s="57"/>
-      <c r="G68" s="57"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
       <c r="H68" s="28"/>
       <c r="I68" s="28"/>
       <c r="J68" s="28"/>
@@ -6291,14 +6293,14 @@
       <c r="A69" s="15">
         <v>2</v>
       </c>
-      <c r="B69" s="57" t="s">
+      <c r="B69" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="C69" s="57"/>
-      <c r="D69" s="57"/>
-      <c r="E69" s="57"/>
-      <c r="F69" s="57"/>
-      <c r="G69" s="57"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
       <c r="H69" s="28"/>
       <c r="I69" s="28"/>
       <c r="J69" s="28"/>
@@ -6320,14 +6322,14 @@
       <c r="A70" s="15">
         <v>3</v>
       </c>
-      <c r="B70" s="57" t="s">
+      <c r="B70" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="C70" s="57"/>
-      <c r="D70" s="57"/>
-      <c r="E70" s="57"/>
-      <c r="F70" s="57"/>
-      <c r="G70" s="57"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="38"/>
       <c r="H70" s="28"/>
       <c r="I70" s="28"/>
       <c r="J70" s="28"/>
@@ -6349,14 +6351,14 @@
       <c r="A71" s="15">
         <v>4</v>
       </c>
-      <c r="B71" s="57" t="s">
+      <c r="B71" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="C71" s="57"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="57"/>
-      <c r="F71" s="57"/>
-      <c r="G71" s="57"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
       <c r="H71" s="28"/>
       <c r="I71" s="28"/>
       <c r="J71" s="28"/>
@@ -6378,14 +6380,14 @@
       <c r="A72" s="15">
         <v>5</v>
       </c>
-      <c r="B72" s="57" t="s">
+      <c r="B72" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="C72" s="57"/>
-      <c r="D72" s="57"/>
-      <c r="E72" s="57"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="57"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="38"/>
       <c r="H72" s="28"/>
       <c r="I72" s="28"/>
       <c r="J72" s="28"/>
@@ -6407,14 +6409,14 @@
       <c r="A73" s="15">
         <v>6</v>
       </c>
-      <c r="B73" s="57" t="s">
+      <c r="B73" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="57"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="57"/>
-      <c r="F73" s="57"/>
-      <c r="G73" s="57"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
       <c r="H73" s="28"/>
       <c r="I73" s="28"/>
       <c r="J73" s="28"/>
@@ -6436,14 +6438,14 @@
       <c r="A74" s="15">
         <v>7</v>
       </c>
-      <c r="B74" s="57" t="s">
+      <c r="B74" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="C74" s="57"/>
-      <c r="D74" s="57"/>
-      <c r="E74" s="57"/>
-      <c r="F74" s="57"/>
-      <c r="G74" s="57"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="38"/>
       <c r="H74" s="28"/>
       <c r="I74" s="28"/>
       <c r="J74" s="28"/>
@@ -6465,14 +6467,14 @@
       <c r="A75" s="15">
         <v>8</v>
       </c>
-      <c r="B75" s="57" t="s">
+      <c r="B75" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="C75" s="57"/>
-      <c r="D75" s="57"/>
-      <c r="E75" s="57"/>
-      <c r="F75" s="57"/>
-      <c r="G75" s="57"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
       <c r="H75" s="28"/>
       <c r="I75" s="28"/>
       <c r="J75" s="28"/>
@@ -6494,14 +6496,14 @@
       <c r="A76" s="15">
         <v>9</v>
       </c>
-      <c r="B76" s="57" t="s">
+      <c r="B76" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="C76" s="57"/>
-      <c r="D76" s="57"/>
-      <c r="E76" s="57"/>
-      <c r="F76" s="57"/>
-      <c r="G76" s="57"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="38"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="38"/>
       <c r="H76" s="28"/>
       <c r="I76" s="28"/>
       <c r="J76" s="28"/>
@@ -6523,14 +6525,14 @@
       <c r="A77" s="15">
         <v>10</v>
       </c>
-      <c r="B77" s="57" t="s">
+      <c r="B77" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="C77" s="57"/>
-      <c r="D77" s="57"/>
-      <c r="E77" s="57"/>
-      <c r="F77" s="57"/>
-      <c r="G77" s="57"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
       <c r="H77" s="28"/>
       <c r="I77" s="28"/>
       <c r="J77" s="28"/>
@@ -6552,14 +6554,14 @@
       <c r="A78" s="15">
         <v>11</v>
       </c>
-      <c r="B78" s="57" t="s">
+      <c r="B78" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="C78" s="57"/>
-      <c r="D78" s="57"/>
-      <c r="E78" s="57"/>
-      <c r="F78" s="57"/>
-      <c r="G78" s="57"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38"/>
       <c r="H78" s="28"/>
       <c r="I78" s="28"/>
       <c r="J78" s="28"/>
@@ -6581,14 +6583,14 @@
       <c r="A79" s="15">
         <v>12</v>
       </c>
-      <c r="B79" s="57" t="s">
+      <c r="B79" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="C79" s="57"/>
-      <c r="D79" s="57"/>
-      <c r="E79" s="57"/>
-      <c r="F79" s="57"/>
-      <c r="G79" s="57"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="38"/>
       <c r="H79" s="28"/>
       <c r="I79" s="28"/>
       <c r="J79" s="28"/>
@@ -6607,48 +6609,48 @@
       <c r="U79" s="16"/>
     </row>
     <row r="80" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="49" t="s">
+      <c r="A80" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="B80" s="49"/>
-      <c r="C80" s="49"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="49"/>
-      <c r="F80" s="49" t="s">
+      <c r="B80" s="40"/>
+      <c r="C80" s="40"/>
+      <c r="D80" s="40"/>
+      <c r="E80" s="40"/>
+      <c r="F80" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G80" s="49" t="s">
+      <c r="G80" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="H80" s="49" t="s">
+      <c r="H80" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="I80" s="49"/>
-      <c r="J80" s="49"/>
-      <c r="K80" s="49"/>
-      <c r="L80" s="49"/>
-      <c r="M80" s="49"/>
-      <c r="N80" s="49"/>
-      <c r="O80" s="49"/>
-      <c r="P80" s="49"/>
-      <c r="Q80" s="49"/>
-      <c r="R80" s="49"/>
-      <c r="S80" s="49"/>
-      <c r="T80" s="49"/>
-      <c r="U80" s="49"/>
+      <c r="I80" s="40"/>
+      <c r="J80" s="40"/>
+      <c r="K80" s="40"/>
+      <c r="L80" s="40"/>
+      <c r="M80" s="40"/>
+      <c r="N80" s="40"/>
+      <c r="O80" s="40"/>
+      <c r="P80" s="40"/>
+      <c r="Q80" s="40"/>
+      <c r="R80" s="40"/>
+      <c r="S80" s="40"/>
+      <c r="T80" s="40"/>
+      <c r="U80" s="40"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B81" s="56" t="s">
+      <c r="B81" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C81" s="56"/>
-      <c r="D81" s="56"/>
-      <c r="E81" s="56"/>
-      <c r="F81" s="56"/>
-      <c r="G81" s="56"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="41"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="41"/>
       <c r="H81" s="30">
         <v>40</v>
       </c>
@@ -6694,14 +6696,14 @@
       <c r="A82" s="15">
         <v>0</v>
       </c>
-      <c r="B82" s="57" t="s">
+      <c r="B82" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="C82" s="57"/>
-      <c r="D82" s="57"/>
-      <c r="E82" s="57"/>
-      <c r="F82" s="57"/>
-      <c r="G82" s="57"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="38"/>
       <c r="H82" s="28"/>
       <c r="I82" s="28"/>
       <c r="J82" s="28"/>
@@ -6721,14 +6723,14 @@
       <c r="A83" s="15">
         <v>1</v>
       </c>
-      <c r="B83" s="57" t="s">
+      <c r="B83" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="C83" s="57"/>
-      <c r="D83" s="57"/>
-      <c r="E83" s="57"/>
-      <c r="F83" s="57"/>
-      <c r="G83" s="57"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="38"/>
+      <c r="G83" s="38"/>
       <c r="H83" s="28"/>
       <c r="I83" s="28"/>
       <c r="J83" s="28"/>
@@ -6748,14 +6750,14 @@
       <c r="A84" s="15">
         <v>2</v>
       </c>
-      <c r="B84" s="57" t="s">
+      <c r="B84" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C84" s="57"/>
-      <c r="D84" s="57"/>
-      <c r="E84" s="57"/>
-      <c r="F84" s="57"/>
-      <c r="G84" s="57"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="38"/>
       <c r="H84" s="28"/>
       <c r="I84" s="28" t="s">
         <v>124</v>
@@ -6777,14 +6779,14 @@
       <c r="A85" s="15">
         <v>3</v>
       </c>
-      <c r="B85" s="57" t="s">
+      <c r="B85" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C85" s="57"/>
-      <c r="D85" s="57"/>
-      <c r="E85" s="57"/>
-      <c r="F85" s="57"/>
-      <c r="G85" s="57"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="38"/>
       <c r="H85" s="28"/>
       <c r="I85" s="28"/>
       <c r="J85" s="28"/>
@@ -6806,14 +6808,14 @@
       <c r="A86" s="15">
         <v>4</v>
       </c>
-      <c r="B86" s="58" t="s">
+      <c r="B86" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="C86" s="58"/>
-      <c r="D86" s="58"/>
-      <c r="E86" s="58"/>
-      <c r="F86" s="58"/>
-      <c r="G86" s="58"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="39"/>
       <c r="H86" s="28"/>
       <c r="I86" s="28"/>
       <c r="J86" s="28"/>
@@ -6833,14 +6835,14 @@
       <c r="A87" s="15">
         <v>5</v>
       </c>
-      <c r="B87" s="57" t="s">
+      <c r="B87" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C87" s="57"/>
-      <c r="D87" s="57"/>
-      <c r="E87" s="57"/>
-      <c r="F87" s="57"/>
-      <c r="G87" s="57"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="38"/>
       <c r="H87" s="28"/>
       <c r="I87" s="28"/>
       <c r="J87" s="28"/>
@@ -6862,14 +6864,14 @@
       <c r="A88" s="15">
         <v>6</v>
       </c>
-      <c r="B88" s="57" t="s">
+      <c r="B88" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C88" s="57"/>
-      <c r="D88" s="57"/>
-      <c r="E88" s="57"/>
-      <c r="F88" s="57"/>
-      <c r="G88" s="57"/>
+      <c r="C88" s="38"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="38"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="38"/>
       <c r="H88" s="28"/>
       <c r="I88" s="28"/>
       <c r="J88" s="28"/>
@@ -6889,6 +6891,93 @@
     </row>
   </sheetData>
   <mergeCells count="101">
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:U2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="G4:O4"/>
+    <mergeCell ref="P4:U5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:O5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="H6:U6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="H11:U11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="H25:U25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="H80:U80"/>
+    <mergeCell ref="B81:G81"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="H66:U66"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="B73:G73"/>
     <mergeCell ref="B82:G82"/>
     <mergeCell ref="B83:G83"/>
     <mergeCell ref="B84:G84"/>
@@ -6903,93 +6992,6 @@
     <mergeCell ref="B78:G78"/>
     <mergeCell ref="B79:G79"/>
     <mergeCell ref="A80:G80"/>
-    <mergeCell ref="H80:U80"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="H66:U66"/>
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="H25:U25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="H6:U6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="H11:U11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:U2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:O3"/>
-    <mergeCell ref="P3:U3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="G4:O4"/>
-    <mergeCell ref="P4:U5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:O5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
lägga till dennis tid
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,452 +5,457 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsrapport" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tidsplan" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="145">
   <si>
-    <t>HELA GRUPPEN – TID</t>
-  </si>
-  <si>
-    <t>DENNIS DERECICHEI</t>
-  </si>
-  <si>
-    <t>NAMN</t>
-  </si>
-  <si>
-    <t>VECKONUMMER (NÄR)</t>
-  </si>
-  <si>
-    <t>Summa</t>
-  </si>
-  <si>
-    <t>timmar</t>
-  </si>
-  <si>
-    <t>Jakob Arvidsson</t>
-  </si>
-  <si>
-    <t>Måndag</t>
-  </si>
-  <si>
-    <t>Juan Basaez</t>
-  </si>
-  <si>
-    <t>Tisdag</t>
-  </si>
-  <si>
-    <t>Johan Can</t>
-  </si>
-  <si>
-    <t>Onsdag</t>
-  </si>
-  <si>
-    <t>Dennis Derecichei</t>
-  </si>
-  <si>
-    <t>Torsdag</t>
-  </si>
-  <si>
-    <t>Emir Hadzisalihovic</t>
-  </si>
-  <si>
-    <t>Fredag</t>
-  </si>
-  <si>
-    <t>Yousef Hashem</t>
-  </si>
-  <si>
-    <t>Lördag</t>
-  </si>
-  <si>
-    <t>Noah Hellman</t>
-  </si>
-  <si>
-    <t>Söndag</t>
-  </si>
-  <si>
-    <t>Summa timmar</t>
-  </si>
-  <si>
-    <t>JAKOB ARVIDSSON</t>
-  </si>
-  <si>
-    <t>EMIR HADZISALIHOVIC</t>
-  </si>
-  <si>
-    <t>JUAN BASAEZ</t>
-  </si>
-  <si>
-    <t>YOUSEF HASHEM</t>
-  </si>
-  <si>
-    <t>JOHAN CAN</t>
-  </si>
-  <si>
-    <t>NOAH HELLMAN</t>
-  </si>
-  <si>
-    <t>Godkännande av</t>
-  </si>
-  <si>
-    <t>Projekt:</t>
-  </si>
-  <si>
-    <t>Projektgrupp:</t>
-  </si>
-  <si>
-    <t>Datum: 2018-11-06</t>
-  </si>
-  <si>
-    <t>Granskad:</t>
-  </si>
-  <si>
-    <t>Beställare: Mattias Krysander</t>
-  </si>
-  <si>
-    <t>Version: 1.2</t>
-  </si>
-  <si>
-    <t>YH, JA</t>
-  </si>
-  <si>
-    <t>Kurs: TSEA29</t>
-  </si>
-  <si>
-    <t>Utfärdare: Jakob Arvidsson</t>
-  </si>
-  <si>
-    <t>OLIKA FASER</t>
-  </si>
-  <si>
-    <t>TID</t>
-  </si>
-  <si>
-    <t>VEM</t>
-  </si>
-  <si>
-    <t>TIDPLAN (när), veckonummer</t>
-  </si>
-  <si>
-    <t>Nr</t>
-  </si>
-  <si>
-    <t>Beskrivning</t>
-  </si>
-  <si>
-    <t>Timmar</t>
-  </si>
-  <si>
-    <t>Initialer</t>
-  </si>
-  <si>
-    <t>Totalt</t>
-  </si>
-  <si>
-    <t>Alla</t>
-  </si>
-  <si>
-    <t>Designfas (v40 – v45)</t>
-  </si>
-  <si>
-    <t>Utförandefas (v46 – v50)</t>
-  </si>
-  <si>
-    <t>DESIGNFAS</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Systemdesign</t>
-  </si>
-  <si>
-    <t>Hårdvarudesign</t>
-  </si>
-  <si>
-    <t>Mjukvarudesign</t>
-  </si>
-  <si>
-    <t>Dokument</t>
-  </si>
-  <si>
-    <t>Rapporter</t>
-  </si>
-  <si>
-    <t>Rita blockdiagram</t>
-  </si>
-  <si>
-    <t>Rita kretsscheman</t>
-  </si>
-  <si>
-    <t>JB, EH</t>
-  </si>
-  <si>
-    <t>Övrigt</t>
-  </si>
-  <si>
-    <t>Möten</t>
-  </si>
-  <si>
-    <t>Buffer</t>
-  </si>
-  <si>
-    <t>UTFÖRANDEFAS</t>
-  </si>
-  <si>
-    <t>Allmänt</t>
-  </si>
-  <si>
-    <t>Koppla och installera</t>
-  </si>
-  <si>
-    <t>DD, EH, Alla</t>
-  </si>
-  <si>
-    <t>Implementera mjukvarubaser</t>
-  </si>
-  <si>
-    <t>NH, EH, DD, JC</t>
-  </si>
-  <si>
-    <t>Kommunikationsmodul</t>
-  </si>
-  <si>
-    <t>Mjukvara för kommunikationsmodul</t>
-  </si>
-  <si>
-    <t>NH, JC</t>
-  </si>
-  <si>
-    <t>Bildbearbetning</t>
-  </si>
-  <si>
-    <t>Upptäcka kanter I bilder</t>
-  </si>
-  <si>
-    <t>Upptäcka linjer</t>
-  </si>
-  <si>
-    <t>NH, DD</t>
-  </si>
-  <si>
-    <t>Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
-  </si>
-  <si>
-    <t>JC, DD, JB</t>
-  </si>
-  <si>
-    <t>Avgör felvärde, beräkna det från 2D kartan</t>
-  </si>
-  <si>
-    <t>NH, JB</t>
-  </si>
-  <si>
-    <t>Autonom körning</t>
-  </si>
-  <si>
-    <t>Position i karta</t>
-  </si>
-  <si>
-    <t>JB, JC, DD</t>
-  </si>
-  <si>
-    <t>Hitta kortaste säkra väg</t>
-  </si>
-  <si>
-    <t>EH</t>
-  </si>
-  <si>
-    <t>Reglera styrning utefter felvärde och följ vägfiler</t>
-  </si>
-  <si>
-    <t>JA,YH</t>
-  </si>
-  <si>
-    <t>Navigera till bestämd stopplinje/parkeringsficka</t>
-  </si>
-  <si>
-    <t>NH, JA</t>
-  </si>
-  <si>
-    <t>Styrmodul</t>
-  </si>
-  <si>
-    <t>Driva bilen</t>
-  </si>
-  <si>
-    <t>Sensormodul</t>
-  </si>
-  <si>
-    <t>Bearbeta sensorvärden</t>
-  </si>
-  <si>
-    <t>EH, JB</t>
-  </si>
-  <si>
-    <t>Skicka ut värden till andra moduler</t>
-  </si>
-  <si>
-    <t>Användargränssnitt</t>
-  </si>
-  <si>
-    <t>Kör och styr taxin från gränssnittet</t>
-  </si>
-  <si>
-    <t>JC,YH</t>
-  </si>
-  <si>
-    <t>Inmatning till gränssnitt</t>
-  </si>
-  <si>
-    <t>JC, EH, JB</t>
-  </si>
-  <si>
-    <t>Visa info på gränssnitt</t>
-  </si>
-  <si>
-    <t>JC, DD</t>
-  </si>
-  <si>
-    <t>Anslutningar</t>
-  </si>
-  <si>
-    <t>Kommunikation via trådlös länk</t>
-  </si>
-  <si>
-    <t>DD,YH</t>
-  </si>
-  <si>
-    <t>Testning</t>
-  </si>
-  <si>
-    <t>Integrationstester</t>
-  </si>
-  <si>
-    <t>Helsystemtestning</t>
-  </si>
-  <si>
-    <t>YH, JC</t>
-  </si>
-  <si>
-    <t>Teknisk dokumentation</t>
-  </si>
-  <si>
-    <t>EH, DD, JB, JA</t>
-  </si>
-  <si>
-    <t>Efterstudie och presentation</t>
-  </si>
-  <si>
-    <t>JA, JC, DD</t>
-  </si>
-  <si>
-    <t>Användarmanual</t>
-  </si>
-  <si>
-    <t>EH, NH, JB, YH</t>
-  </si>
-  <si>
-    <t>Tids- och statusrapporter</t>
-  </si>
-  <si>
-    <t>Summa antal timmar:</t>
-  </si>
-  <si>
-    <t>MILSTOLPAR</t>
-  </si>
-  <si>
-    <t>DEADLINE (när), veckodag &amp; vecka</t>
-  </si>
-  <si>
-    <t>Milstolpe</t>
-  </si>
-  <si>
-    <t>Utvecklingsmiljöer för mikrokontroller och processorer</t>
-  </si>
-  <si>
-    <t>ONS</t>
-  </si>
-  <si>
-    <t>Designspecifikationen är färdigställd</t>
-  </si>
-  <si>
-    <t>TIS</t>
-  </si>
-  <si>
-    <t>Elektroniska komponenter är kopplade</t>
-  </si>
-  <si>
-    <t>MÅN</t>
-  </si>
-  <si>
-    <t>Seriell kommunikation sker mellan moduler</t>
-  </si>
-  <si>
-    <t>Mätvärden visas på användargränssnittet och reglerparametrar kan skickas till taxin under körning</t>
-  </si>
-  <si>
-    <t>Taxin kan fjärrstyras</t>
-  </si>
-  <si>
-    <t>Kameran tar bilder och dessa behandlas</t>
-  </si>
-  <si>
-    <t>TOR</t>
-  </si>
-  <si>
-    <t>Mata in karta och tolka den</t>
-  </si>
-  <si>
-    <t>Taxin håller sig inom vägen</t>
-  </si>
-  <si>
-    <t>Taxin kan navigera kartan på ett säkert sätt</t>
-  </si>
-  <si>
-    <t>FRE</t>
-  </si>
-  <si>
-    <t>Taxin kan parkera i parkeringsfickor</t>
-  </si>
-  <si>
-    <t>Taxin utför sitt uppdrag 3 av 4 gånger</t>
-  </si>
-  <si>
-    <t>BESLUTSPUNKTER</t>
-  </si>
-  <si>
-    <t>DEADLINE (när), datum</t>
-  </si>
-  <si>
-    <t>Godkännande av projektdirektiv, start av förstudier</t>
-  </si>
-  <si>
-    <t>Godkännande av kravspecifikation, start av förberedelsefasen</t>
-  </si>
-  <si>
-    <t>Godkännande av projektplanering, start av utförandefasen</t>
-  </si>
-  <si>
-    <t>Godkännande av designspecifikation, fortsättning av utförandefasen</t>
-  </si>
-  <si>
-    <t>Används ej</t>
-  </si>
-  <si>
-    <t>Godkännande av produktens funktionalitet, leverans</t>
-  </si>
-  <si>
-    <t>Godkännande av leverans, upplösning av projektgrupp</t>
+    <t xml:space="preserve">HELA GRUPPEN – TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DENNIS DERECICHEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAMN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VECKONUMMER (NÄR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakob Arvidsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Måndag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan Basaez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tisdag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johan Can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onsdag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dennis Derecichei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torsdag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emir Hadzisalihovic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fredag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yousef Hashem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lördag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noah Hellman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Söndag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summa timmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JAKOB ARVIDSSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMIR HADZISALIHOVIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUAN BASAEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOUSEF HASHEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHAN CAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOAH HELLMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projekt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projektgrupp:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum: 2018-11-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granskad:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beställare: Mattias Krysander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YH, JA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurs: TSEA29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utfärdare: Jakob Arvidsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLIKA FASER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIDPLAN (när), veckonummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beskrivning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designfas (v40 – v45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utförandefas (v46 – v50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESIGNFAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systemdesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hårdvarudesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mjukvarudesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dokument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rita blockdiagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rita kretsscheman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JB, EH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Övrigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Möten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTFÖRANDEFAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allmänt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koppla och installera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD, EH, Alla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementera mjukvarubaser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH, EH, DD, JC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommunikationsmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mjukvara för kommunikationsmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH, JC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bildbearbetning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upptäcka kanter I bilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upptäcka linjer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH, DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC, DD, JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avgör felvärde, beräkna det från 2D kartan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH, JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autonom körning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position i karta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JB, JC, DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hitta kortaste säkra väg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reglera styrning utefter felvärde och följ vägfiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA,YH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigera till bestämd stopplinje/parkeringsficka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH, JA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Styrmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driva bilen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensormodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bearbeta sensorvärden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH, JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skicka ut värden till andra moduler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Användargränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kör och styr taxin från gränssnittet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC,YH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inmatning till gränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC, EH, JB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visa info på gränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JC, DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anslutningar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommunikation via trådlös länk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD,YH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrationstester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helsystemtestning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YH, JC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teknisk dokumentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH, DD, JB, JA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efterstudie och presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JA, JC, DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Användarmanual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH, NH, JB, YH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tids- och statusrapporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summa antal timmar:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILSTOLPAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE (när), veckodag &amp; vecka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milstolpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utvecklingsmiljöer för mikrokontroller och processorer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designspecifikationen är färdigställd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elektroniska komponenter är kopplade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MÅN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seriell kommunikation sker mellan moduler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mätvärden visas på användargränssnittet och reglerparametrar kan skickas till taxin under körning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin kan fjärrstyras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kameran tar bilder och dessa behandlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mata in karta och tolka den</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin håller sig inom vägen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin kan navigera kartan på ett säkert sätt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin kan parkera i parkeringsfickor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxin utför sitt uppdrag 3 av 4 gånger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BESLUTSPUNKTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE (när), datum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av projektdirektiv, start av förstudier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av kravspecifikation, start av förberedelsefasen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av projektplanering, start av utförandefasen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av designspecifikation, fortsättning av utförandefasen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Används ej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av produktens funktionalitet, leverans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Godkännande av leverans, upplösning av projektgrupp</t>
   </si>
 </sst>
 </file>
@@ -458,7 +463,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -930,12 +935,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1007,24 +1012,24 @@
   </sheetPr>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J37" activeCellId="0" sqref="J37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X5" activeCellId="0" sqref="X5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="3" style="1" width="5.01020408163265"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.86734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="8.86224489795918"/>
-    <col collapsed="false" hidden="false" max="26" min="17" style="1" width="5.85714285714286"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="1" width="9"/>
-    <col collapsed="false" hidden="false" max="40" min="31" style="1" width="13.1377551020408"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="6.01020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="42" style="1" width="11.4183673469388"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="1" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="17" style="1" width="5.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="7.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="31" style="1" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="42" style="1" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1242,9 @@
       <c r="W4" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="X4" s="8"/>
+      <c r="X4" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="6"/>
@@ -1308,7 +1315,9 @@
       <c r="W5" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="X5" s="8"/>
+      <c r="X5" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="6"/>
@@ -1377,7 +1386,9 @@
       <c r="W6" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="X6" s="8"/>
+      <c r="X6" s="8" t="n">
+        <v>5</v>
+      </c>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="6"/>
@@ -1417,7 +1428,7 @@
       </c>
       <c r="J7" s="8" t="n">
         <f aca="false">SUM(X4:X10)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K7" s="8" t="n">
         <f aca="false">SUM(Y4:Y10)</f>
@@ -1429,7 +1440,7 @@
       </c>
       <c r="M7" s="9" t="n">
         <f aca="false">SUM(C7:L7)</f>
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>13</v>
@@ -1450,7 +1461,9 @@
       <c r="W7" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="X7" s="8"/>
+      <c r="X7" s="8" t="n">
+        <v>3</v>
+      </c>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="6"/>
@@ -1525,7 +1538,9 @@
       <c r="W8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="X8" s="8"/>
+      <c r="X8" s="8" t="n">
+        <v>6</v>
+      </c>
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="6"/>
@@ -1695,7 +1710,7 @@
       </c>
       <c r="J11" s="9" t="n">
         <f aca="false">SUM(J4:J10)</f>
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="K11" s="9" t="n">
         <f aca="false">SUM(K4:K10)</f>
@@ -1707,7 +1722,7 @@
       </c>
       <c r="M11" s="9" t="n">
         <f aca="false">SUM(C11:L11)</f>
-        <v>731</v>
+        <v>755</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>20</v>
@@ -1743,7 +1758,7 @@
       </c>
       <c r="X11" s="9" t="n">
         <f aca="false">SUM(X4:X10)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Y11" s="9" t="n">
         <f aca="false">SUM(Y4:Y10)</f>
@@ -3649,7 +3664,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3664,22 +3679,22 @@
   </sheetPr>
   <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.14285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.86734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="8" style="0" width="5.42857142857143"/>
-    <col collapsed="false" hidden="false" max="1014" min="22" style="0" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="11.4183673469388"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="8" style="0" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="22" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6810,10 +6825,10 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
timeplan for this week
</commit_message>
<xml_diff>
--- a/doc/tidsrapport/tidsrapport.xlsx
+++ b/doc/tidsrapport/tidsrapport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tidsrapport" sheetId="1" state="visible" r:id="rId2"/>
@@ -938,12 +938,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1015,15 +1015,15 @@
   </sheetPr>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y9" activeCellId="0" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="1" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="17" style="1" width="5.86"/>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="K4" s="8" t="n">
         <f aca="false">SUM(K17:K23)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L4" s="8" t="n">
         <f aca="false">SUM(L17:L23)</f>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="M4" s="9" t="n">
         <f aca="false">SUM(C4:L4)</f>
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>7</v>
@@ -1248,7 +1248,9 @@
       <c r="X4" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="Y4" s="8"/>
+      <c r="Y4" s="8" t="n">
+        <v>2</v>
+      </c>
       <c r="Z4" s="8"/>
       <c r="AA4" s="6"/>
     </row>
@@ -1321,7 +1323,9 @@
       <c r="X5" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="Y5" s="8"/>
+      <c r="Y5" s="8" t="n">
+        <v>3</v>
+      </c>
       <c r="Z5" s="8"/>
       <c r="AA5" s="6"/>
     </row>
@@ -1392,7 +1396,9 @@
       <c r="X6" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="Y6" s="8"/>
+      <c r="Y6" s="8" t="n">
+        <v>3</v>
+      </c>
       <c r="Z6" s="8"/>
       <c r="AA6" s="6"/>
     </row>
@@ -1435,7 +1441,7 @@
       </c>
       <c r="K7" s="8" t="n">
         <f aca="false">SUM(Y4:Y10)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L7" s="8" t="n">
         <f aca="false">SUM(Z4:Z10)</f>
@@ -1443,7 +1449,7 @@
       </c>
       <c r="M7" s="9" t="n">
         <f aca="false">SUM(C7:L7)</f>
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>13</v>
@@ -1467,7 +1473,9 @@
       <c r="X7" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="Y7" s="8"/>
+      <c r="Y7" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="Z7" s="8"/>
       <c r="AA7" s="6"/>
     </row>
@@ -1544,7 +1552,9 @@
       <c r="X8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="Y8" s="8"/>
+      <c r="Y8" s="8" t="n">
+        <v>8</v>
+      </c>
       <c r="Z8" s="8"/>
       <c r="AA8" s="6"/>
     </row>
@@ -1717,7 +1727,7 @@
       </c>
       <c r="K11" s="9" t="n">
         <f aca="false">SUM(K4:K10)</f>
-        <v>154</v>
+        <v>194</v>
       </c>
       <c r="L11" s="9" t="n">
         <f aca="false">SUM(L4:L10)</f>
@@ -1725,7 +1735,7 @@
       </c>
       <c r="M11" s="9" t="n">
         <f aca="false">SUM(C11:L11)</f>
-        <v>940</v>
+        <v>980</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>20</v>
@@ -1765,7 +1775,7 @@
       </c>
       <c r="Y11" s="9" t="n">
         <f aca="false">SUM(Y4:Y10)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z11" s="9" t="n">
         <f aca="false">SUM(Z4:Z10)</f>
@@ -1932,7 +1942,9 @@
       <c r="J17" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="K17" s="8"/>
+      <c r="K17" s="8" t="n">
+        <v>2</v>
+      </c>
       <c r="L17" s="8"/>
       <c r="M17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -1986,7 +1998,9 @@
       <c r="J18" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="K18" s="8"/>
+      <c r="K18" s="8" t="n">
+        <v>3</v>
+      </c>
       <c r="L18" s="8"/>
       <c r="M18" s="6"/>
       <c r="O18" s="10" t="s">
@@ -2034,7 +2048,9 @@
       <c r="J19" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="K19" s="8"/>
+      <c r="K19" s="8" t="n">
+        <v>3</v>
+      </c>
       <c r="L19" s="8"/>
       <c r="M19" s="6"/>
       <c r="O19" s="10" t="s">
@@ -2084,7 +2100,9 @@
       <c r="J20" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="K20" s="8"/>
+      <c r="K20" s="8" t="n">
+        <v>4</v>
+      </c>
       <c r="L20" s="8"/>
       <c r="M20" s="6"/>
       <c r="O20" s="10" t="s">
@@ -2138,7 +2156,9 @@
       <c r="J21" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="K21" s="8"/>
+      <c r="K21" s="8" t="n">
+        <v>8</v>
+      </c>
       <c r="L21" s="8"/>
       <c r="M21" s="6"/>
       <c r="O21" s="10" t="s">
@@ -2272,7 +2292,7 @@
       </c>
       <c r="K24" s="9" t="n">
         <f aca="false">SUM(K17:K23)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L24" s="9" t="n">
         <f aca="false">SUM(L17:L23)</f>
@@ -3572,17 +3592,17 @@
   </sheetPr>
   <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W19" activeCellId="0" sqref="W19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R58" activeCellId="0" sqref="R58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="8" style="0" width="5.43"/>
@@ -3853,12 +3873,11 @@
         <v>171</v>
       </c>
       <c r="Q8" s="34" t="n">
-        <f aca="false">SUM(Q13:Q23,Q27:Q63)</f>
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="R8" s="34" t="n">
         <f aca="false">SUM(R13:R23,R27:R63)</f>
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="S8" s="34" t="n">
         <f aca="false">SUM(S13:S23,S27:S63)</f>
@@ -3941,7 +3960,7 @@
         <v>164</v>
       </c>
       <c r="R10" s="34" t="n">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="S10" s="34" t="n">
         <v>22</v>
@@ -3949,7 +3968,7 @@
       <c r="T10" s="38"/>
       <c r="U10" s="32" t="n">
         <f aca="false">SUM(H10:S10)</f>
-        <v>838</v>
+        <v>808</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5042,13 +5061,13 @@
         <v>35</v>
       </c>
       <c r="R41" s="43" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="S41" s="36"/>
       <c r="T41" s="38"/>
       <c r="U41" s="32" t="n">
         <f aca="false">SUM(H41:S41)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5556,13 +5575,13 @@
       <c r="P57" s="43"/>
       <c r="Q57" s="43"/>
       <c r="R57" s="43" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="S57" s="36"/>
       <c r="T57" s="38"/>
       <c r="U57" s="32" t="n">
         <f aca="false">SUM(H57:S57)</f>
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5838,7 +5857,7 @@
       </c>
       <c r="R64" s="43" t="n">
         <f aca="false">SUM(R28:R63)</f>
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="S64" s="43" t="n">
         <f aca="false">SUM(S28:S63)</f>
@@ -5847,7 +5866,7 @@
       <c r="T64" s="38"/>
       <c r="U64" s="32" t="n">
         <f aca="false">SUM(H64:S64)</f>
-        <v>838</v>
+        <v>808</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5890,7 +5909,7 @@
       </c>
       <c r="R65" s="46" t="n">
         <f aca="false">SUM(R13:R23,R27:R63)</f>
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="S65" s="46" t="n">
         <f aca="false">SUM(S13:S23,S27:S63)</f>
@@ -5899,7 +5918,7 @@
       <c r="T65" s="38"/>
       <c r="U65" s="32" t="n">
         <f aca="false">SUM(H65:S65)</f>
-        <v>872</v>
+        <v>842</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>